<commit_message>
continuacao do commit anterior
</commit_message>
<xml_diff>
--- a/#Excel/Analises.xlsx
+++ b/#Excel/Analises.xlsx
@@ -26,7 +26,7 @@
     <pivotCache cacheId="17" r:id="rId9"/>
     <pivotCache cacheId="20" r:id="rId10"/>
     <pivotCache cacheId="23" r:id="rId11"/>
-    <pivotCache cacheId="26" r:id="rId12"/>
+    <pivotCache cacheId="41" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2498,7 +2498,7 @@
                   <c:v>31588</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>9570.9500000000007</c:v>
+                  <c:v>10207.549999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2514,11 +2514,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="115021664"/>
-        <c:axId val="115021104"/>
+        <c:axId val="199034496"/>
+        <c:axId val="199035056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115021664"/>
+        <c:axId val="199034496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2561,7 +2561,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115021104"/>
+        <c:crossAx val="199035056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2569,7 +2569,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115021104"/>
+        <c:axId val="199035056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2620,7 +2620,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115021664"/>
+        <c:crossAx val="199034496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3290,1405 +3290,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Rui Miranda" refreshedDate="41444.125931249997" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
-  <cacheSource type="external" connectionId="2"/>
-  <cacheFields count="9">
-    <cacheField name="[Measures].[Valor]" caption="Valor" numFmtId="0" hierarchy="10" level="32767"/>
-    <cacheField name="[Meses].[Ano - Mês Número].[Ano]" caption="Ano" numFmtId="0" level="1">
-      <sharedItems count="4">
-        <s v="[Meses].[Ano - Mês Número].[Ano].&amp;[2010]" c="2010"/>
-        <s v="[Meses].[Ano - Mês Número].[Ano].&amp;[2011]" c="2011"/>
-        <s v="[Meses].[Ano - Mês Número].[Ano].&amp;[2012]" c="2012"/>
-        <s v="[Meses].[Ano - Mês Número].[Ano].&amp;[2013]" c="2013"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Meses].[Ano - Mês Número].[Trimestre]" caption="Trimestre" numFmtId="0" level="2" mappingCount="1">
-      <sharedItems count="16">
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2010]&amp;[1]" c="1" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2010]&amp;[2]" c="2" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2010]&amp;[3]" c="3" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2010]&amp;[4]" c="4" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2011]&amp;[1]" c="1" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2011]&amp;[2]" c="2" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2011]&amp;[3]" c="3" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2011]&amp;[4]" c="4" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2012]&amp;[1]" c="1" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2012]&amp;[2]" c="2" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2012]&amp;[3]" c="3" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2012]&amp;[4]" c="4" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2013]&amp;[1]" c="1" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2013]&amp;[2]" c="2" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2013]&amp;[3]" c="3" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2013]&amp;[4]" c="4" cp="1">
-          <x v="3"/>
-        </s>
-      </sharedItems>
-      <mpMap v="4"/>
-    </cacheField>
-    <cacheField name="[Meses].[Ano - Mês Número].[Mês Número]" caption="Mês Número" numFmtId="0" level="3" mappingCount="1">
-      <sharedItems count="48">
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[1]&amp;[1]" c="1" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[1]&amp;[2]" c="2" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[1]&amp;[3]" c="3" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[2]&amp;[4]" c="4" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[2]&amp;[5]" c="5" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[2]&amp;[6]" c="6" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[3]&amp;[7]" c="7" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[3]&amp;[8]" c="8" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[3]&amp;[9]" c="9" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[4]&amp;[10]" c="10" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[4]&amp;[11]" c="11" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[4]&amp;[12]" c="12" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[1]&amp;[1]" c="1" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[1]&amp;[2]" c="2" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[1]&amp;[3]" c="3" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[2]&amp;[4]" c="4" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[2]&amp;[5]" c="5" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[2]&amp;[6]" c="6" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[3]&amp;[7]" c="7" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[3]&amp;[8]" c="8" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[3]&amp;[9]" c="9" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[4]&amp;[10]" c="10" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[4]&amp;[11]" c="11" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[4]&amp;[12]" c="12" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[1]&amp;[1]" c="1" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[1]&amp;[2]" c="2" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[1]&amp;[3]" c="3" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[2]&amp;[4]" c="4" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[2]&amp;[5]" c="5" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[2]&amp;[6]" c="6" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[3]&amp;[7]" c="7" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[3]&amp;[8]" c="8" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[3]&amp;[9]" c="9" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[4]&amp;[10]" c="10" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[4]&amp;[11]" c="11" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[4]&amp;[12]" c="12" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[1]&amp;[1]" c="1" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[1]&amp;[2]" c="2" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[1]&amp;[3]" c="3" cp="1">
-          <x/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[2]&amp;[4]" c="4" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[2]&amp;[5]" c="5" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[2]&amp;[6]" c="6" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[3]&amp;[7]" c="7" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[3]&amp;[8]" c="8" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[3]&amp;[9]" c="9" cp="1">
-          <x v="2"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[4]&amp;[10]" c="10" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[4]&amp;[11]" c="11" cp="1">
-          <x v="3"/>
-        </s>
-        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[4]&amp;[12]" c="12" cp="1">
-          <x v="3"/>
-        </s>
-      </sharedItems>
-      <mpMap v="5"/>
-    </cacheField>
-    <cacheField name="[Meses].[Ano - Mês Número].[Trimestre].[Ano]" caption="Ano" propertyName="Ano" numFmtId="0" level="2" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2010" maxValue="2013" count="4">
-        <n v="2010"/>
-        <n v="2011"/>
-        <n v="2012"/>
-        <n v="2013"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Meses].[Ano - Mês Número].[Mês Número].[Trimestre]" caption="Trimestre" propertyName="Trimestre" numFmtId="0" level="3" memberPropertyField="1">
-      <sharedItems count="4">
-        <s v="1"/>
-        <s v="2"/>
-        <s v="3"/>
-        <s v="4"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Rubrica].[Classe - Nome].[Classe]" caption="Classe" numFmtId="0" hierarchy="3" level="1">
-      <sharedItems count="2">
-        <s v="[Rubrica].[Classe - Nome].[Classe].&amp;[Custo]" c="Custo"/>
-        <s v="[Rubrica].[Classe - Nome].[Classe].&amp;[Proveito]" c="Proveito"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Rubrica].[Classe - Nome].[Nome]" caption="Nome" numFmtId="0" hierarchy="3" level="2" mappingCount="1">
-      <sharedItems count="4">
-        <s v="[Rubrica].[Classe - Nome].[Nome].&amp;[Custo]&amp;[Financeiro]" c="Financeiro" cp="1">
-          <x/>
-        </s>
-        <s v="[Rubrica].[Classe - Nome].[Nome].&amp;[Custo]&amp;[Material]" c="Material" cp="1">
-          <x/>
-        </s>
-        <s v="[Rubrica].[Classe - Nome].[Nome].&amp;[Custo]&amp;[Outros]" c="Outros" cp="1">
-          <x/>
-        </s>
-        <s v="[Rubrica].[Classe - Nome].[Nome].&amp;[Custo]&amp;[Salarios]" c="Salarios" cp="1">
-          <x/>
-        </s>
-      </sharedItems>
-      <mpMap v="8"/>
-    </cacheField>
-    <cacheField name="[Rubrica].[Classe - Nome].[Nome].[Classe]" caption="Classe" propertyName="Classe" numFmtId="0" hierarchy="3" level="2" memberPropertyField="1">
-      <sharedItems count="1">
-        <s v="Custo"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <cacheHierarchies count="12">
-    <cacheHierarchy uniqueName="[Meses].[Ano - Mês Número]" caption="Ano - Mês Número" time="1" defaultMemberUniqueName="[Meses].[Ano - Mês Número].[All]" allUniqueName="[Meses].[Ano - Mês Número].[All]" dimensionUniqueName="[Meses]" displayFolder="" count="4" unbalanced="0">
-      <fieldsUsage count="4">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-        <fieldUsage x="2"/>
-        <fieldUsage x="3"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Meses].[Mês Nome]" caption="Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Meses].[Mês Nome].[All]" allUniqueName="[Meses].[Mês Nome].[All]" dimensionUniqueName="[Meses]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Rubrica].[Classe]" caption="Classe" attribute="1" defaultMemberUniqueName="[Rubrica].[Classe].[All]" allUniqueName="[Rubrica].[Classe].[All]" dimensionUniqueName="[Rubrica]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Rubrica].[Classe - Nome]" caption="Classe - Nome" defaultMemberUniqueName="[Rubrica].[Classe - Nome].[All]" allUniqueName="[Rubrica].[Classe - Nome].[All]" dimensionUniqueName="[Rubrica]" displayFolder="" count="3" unbalanced="0">
-      <fieldsUsage count="3">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="6"/>
-        <fieldUsage x="7"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Rubrica].[Nome]" caption="Nome" attribute="1" defaultMemberUniqueName="[Rubrica].[Nome].[All]" allUniqueName="[Rubrica].[Nome].[All]" dimensionUniqueName="[Rubrica]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Meses].[Ano]" caption="Ano" attribute="1" time="1" defaultMemberUniqueName="[Meses].[Ano].[All]" allUniqueName="[Meses].[Ano].[All]" dimensionUniqueName="[Meses]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Meses].[Keycol]" caption="Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Meses].[Keycol].[All]" allUniqueName="[Meses].[Keycol].[All]" dimensionUniqueName="[Meses]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Meses].[Mês Número]" caption="Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Meses].[Mês Número].[All]" allUniqueName="[Meses].[Mês Número].[All]" dimensionUniqueName="[Meses]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Meses].[Trimestre]" caption="Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Meses].[Trimestre].[All]" allUniqueName="[Meses].[Trimestre].[All]" dimensionUniqueName="[Meses]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Rubrica].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Rubrica].[Keycol].[All]" allUniqueName="[Rubrica].[Keycol].[All]" dimensionUniqueName="[Rubrica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Valor]" caption="Valor" measure="1" displayFolder="" measureGroup="Resultados" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Contagem de Resultados]" caption="Contagem de Resultados" measure="1" displayFolder="" measureGroup="Resultados" count="0"/>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <dimensions count="3">
-    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
-    <dimension name="Meses" uniqueName="[Meses]" caption="Meses"/>
-    <dimension name="Rubrica" uniqueName="[Rubrica]" caption="Rubrica"/>
-  </dimensions>
-  <measureGroups count="1">
-    <measureGroup name="Resultados" caption="Resultados"/>
-  </measureGroups>
-  <maps count="2">
-    <map measureGroup="0" dimension="1"/>
-    <map measureGroup="0" dimension="2"/>
-  </maps>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Rui Miranda" refreshedDate="41444.125963425926" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
-  <cacheSource type="external" connectionId="3"/>
-  <cacheFields count="16">
-    <cacheField name="[Measures].[Contagem de Entregas]" caption="Contagem de Entregas" numFmtId="0" hierarchy="129" level="32767"/>
-    <cacheField name="[Funcionário].[Localização - Loja].[Localização]" caption="Localização" numFmtId="0" hierarchy="35" level="1">
-      <sharedItems count="2">
-        <s v="[Funcionário].[Localização - Loja].[Localização].&amp;[Lisboa]" c="Lisboa"/>
-        <s v="[Funcionário].[Localização - Loja].[Localização].&amp;[Porto]" c="Porto"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Funcionário].[Localização - Loja].[Loja]" caption="Loja" numFmtId="0" hierarchy="35" level="2" mappingCount="1">
-      <sharedItems count="2">
-        <s v="[Funcionário].[Localização - Loja].[Loja].&amp;[Lisboa]&amp;[Sede]" c="Sede" cp="1">
-          <x/>
-        </s>
-        <s v="[Funcionário].[Localização - Loja].[Loja].&amp;[Porto]&amp;[Filial1]" c="Filial1" cp="1">
-          <x v="1"/>
-        </s>
-      </sharedItems>
-      <mpMap v="4"/>
-    </cacheField>
-    <cacheField name="[Funcionário].[Localização - Loja].[Nome Completo]" caption="Nome Completo" numFmtId="0" hierarchy="35" level="3" mappingCount="3">
-      <sharedItems count="3">
-        <s v="[Funcionário].[Localização - Loja].[Nome Completo].&amp;[Luciano Salgado]&amp;[Alarico Medina]" c="Alarico Medina" cp="3">
-          <x/>
-          <x/>
-          <x/>
-        </s>
-        <s v="[Funcionário].[Localização - Loja].[Nome Completo].&amp;[Sabrina Prada]&amp;[Vasco Moita]" c="Vasco Moita" cp="3">
-          <x/>
-          <x v="1"/>
-          <x v="1"/>
-        </s>
-        <s v="[Funcionário].[Localização - Loja].[Nome Completo].&amp;[Luciano Salgado]&amp;[Vanda Seabra]" u="1" c="Vanda Seabra"/>
-      </sharedItems>
-      <mpMap v="5"/>
-      <mpMap v="6"/>
-      <mpMap v="7"/>
-    </cacheField>
-    <cacheField name="[Funcionário].[Localização - Loja].[Loja].[Localização]" caption="Localização" propertyName="Localização" numFmtId="0" hierarchy="35" level="2" memberPropertyField="1">
-      <sharedItems count="2">
-        <s v="Lisboa"/>
-        <s v="Porto"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Funcionário].[Localização - Loja].[Nome Completo].[Função]" caption="Função" propertyName="Função" numFmtId="0" hierarchy="35" level="3" memberPropertyField="1">
-      <sharedItems count="1">
-        <s v="Paquete"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Funcionário].[Localização - Loja].[Nome Completo].[Loja]" caption="Loja" propertyName="Loja" numFmtId="0" hierarchy="35" level="3" memberPropertyField="1">
-      <sharedItems count="2">
-        <s v="Sede"/>
-        <s v="Filial1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Funcionário].[Localização - Loja].[Nome Completo].[Nome Completo Do Chefe]" caption="Nome Completo Do Chefe" propertyName="Nome Completo Do Chefe" numFmtId="0" hierarchy="35" level="3" memberPropertyField="1">
-      <sharedItems count="2">
-        <s v="Luciano Salgado"/>
-        <s v="Sabrina Prada"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Ano]" caption="Ano" numFmtId="0" hierarchy="29" level="1">
-      <sharedItems count="4">
-        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2010]" c="2010"/>
-        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2011]" c="2011"/>
-        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2012]" c="2012"/>
-        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2013]" c="2013"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Trimestre]" caption="Trimestre" numFmtId="0" hierarchy="29" level="2" mappingCount="1">
-      <sharedItems count="2">
-        <s v="[Data Tentativa].[Ano - Dia].[Trimestre].&amp;[2013]&amp;[1]" c="1" cp="1">
-          <x/>
-        </s>
-        <s v="[Data Tentativa].[Ano - Dia].[Trimestre].&amp;[2013]&amp;[2]" c="2" cp="1">
-          <x/>
-        </s>
-      </sharedItems>
-      <mpMap v="12"/>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Mês Número]" caption="Mês Número" numFmtId="0" hierarchy="29" level="3" mappingCount="1">
-      <sharedItems count="3">
-        <s v="[Data Tentativa].[Ano - Dia].[Mês Número].&amp;[2013]&amp;[2]&amp;[4]" c="4" cp="1">
-          <x/>
-        </s>
-        <s v="[Data Tentativa].[Ano - Dia].[Mês Número].&amp;[2013]&amp;[2]&amp;[5]" c="5" cp="1">
-          <x/>
-        </s>
-        <s v="[Data Tentativa].[Ano - Dia].[Mês Número].&amp;[2013]&amp;[2]&amp;[6]" c="6" cp="1">
-          <x/>
-        </s>
-      </sharedItems>
-      <mpMap v="13"/>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Dia]" caption="Dia" numFmtId="0" hierarchy="29" level="4">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Trimestre].[Ano]" caption="Ano" propertyName="Ano" numFmtId="0" hierarchy="29" level="2" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2013" maxValue="2013" count="1">
-        <n v="2013"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Mês Número].[Trimestre]" caption="Trimestre" propertyName="Trimestre" numFmtId="0" hierarchy="29" level="3" memberPropertyField="1">
-      <sharedItems count="1">
-        <s v="2"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Dia].[Mês Número]" caption="Mês Número" propertyName="Mês Número" numFmtId="0" hierarchy="29" level="4" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Tipo Servico].[Tipo].[Tipo]" caption="Tipo" numFmtId="0" hierarchy="72" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-  </cacheFields>
-  <cacheHierarchies count="130">
-    <cacheHierarchy uniqueName="[Cliente].[Activo]" caption="Activo" attribute="1" defaultMemberUniqueName="[Cliente].[Activo].[All]" allUniqueName="[Cliente].[Activo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Codigo Postal]" caption="Codigo Postal" attribute="1" defaultMemberUniqueName="[Cliente].[Codigo Postal].[All]" allUniqueName="[Cliente].[Codigo Postal].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Educação]" caption="Educação" attribute="1" defaultMemberUniqueName="[Cliente].[Educação].[All]" allUniqueName="[Cliente].[Educação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Estado Civil]" caption="Estado Civil" attribute="1" defaultMemberUniqueName="[Cliente].[Estado Civil].[All]" allUniqueName="[Cliente].[Estado Civil].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Género]" caption="Género" attribute="1" defaultMemberUniqueName="[Cliente].[Género].[All]" allUniqueName="[Cliente].[Género].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Idade]" caption="Intervalo Idade" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Idade].[All]" allUniqueName="[Cliente].[Intervalo Idade].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Idade Nome]" caption="Intervalo Idade Nome" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Idade Nome].[All]" allUniqueName="[Cliente].[Intervalo Idade Nome].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento]" caption="Intervalo Rendimento" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento].[All]" allUniqueName="[Cliente].[Intervalo Rendimento].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento Classe]" caption="Intervalo Rendimento Classe" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento Classe].[All]" allUniqueName="[Cliente].[Intervalo Rendimento Classe].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento Codigo]" caption="Intervalo Rendimento Codigo" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento Codigo].[All]" allUniqueName="[Cliente].[Intervalo Rendimento Codigo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Nome De Contacto]" caption="Nome De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Nome De Contacto].[All]" allUniqueName="[Cliente].[Nome De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Número De Carros Possuidos]" caption="Número De Carros Possuidos" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Carros Possuidos].[All]" allUniqueName="[Cliente].[Número De Carros Possuidos].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Número De Filhos]" caption="Número De Filhos" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Filhos].[All]" allUniqueName="[Cliente].[Número De Filhos].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Número De Filhos Em Casa]" caption="Número De Filhos Em Casa" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Filhos Em Casa].[All]" allUniqueName="[Cliente].[Número De Filhos Em Casa].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Ocupação]" caption="Ocupação" attribute="1" defaultMemberUniqueName="[Cliente].[Ocupação].[All]" allUniqueName="[Cliente].[Ocupação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Por Designação]" caption="Por Designação" defaultMemberUniqueName="[Cliente].[Por Designação].[All]" allUniqueName="[Cliente].[Por Designação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Possui Casa]" caption="Possui Casa" attribute="1" defaultMemberUniqueName="[Cliente].[Possui Casa].[All]" allUniqueName="[Cliente].[Possui Casa].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Singular]" caption="Singular" attribute="1" defaultMemberUniqueName="[Cliente].[Singular].[All]" allUniqueName="[Cliente].[Singular].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Sobrenome De Contacto]" caption="Sobrenome De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Sobrenome De Contacto].[All]" allUniqueName="[Cliente].[Sobrenome De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Ano - Dia]" caption="Data Conclusao.Ano - Dia" time="1" defaultMemberUniqueName="[Data Conclusao].[Ano - Dia].[All]" allUniqueName="[Data Conclusao].[Ano - Dia].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Data]" caption="Data Conclusao.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Data].[All]" allUniqueName="[Data Conclusao].[Data].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Dia Da Semana Nome]" caption="Data Conclusao.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia Da Semana Nome].[All]" allUniqueName="[Data Conclusao].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Dia Da Semana Número]" caption="Data Conclusao.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia Da Semana Número].[All]" allUniqueName="[Data Conclusao].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Mês Nome]" caption="Data Conclusao.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Mês Nome].[All]" allUniqueName="[Data Conclusao].[Mês Nome].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Ano - Dia]" caption="Data Requisicao.Ano - Dia" time="1" defaultMemberUniqueName="[Data Requisicao].[Ano - Dia].[All]" allUniqueName="[Data Requisicao].[Ano - Dia].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Data]" caption="Data Requisicao.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Data].[All]" allUniqueName="[Data Requisicao].[Data].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Dia Da Semana Nome]" caption="Data Requisicao.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia Da Semana Nome].[All]" allUniqueName="[Data Requisicao].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Dia Da Semana Número]" caption="Data Requisicao.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia Da Semana Número].[All]" allUniqueName="[Data Requisicao].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Mês Nome]" caption="Data Requisicao.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Mês Nome].[All]" allUniqueName="[Data Requisicao].[Mês Nome].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Ano - Dia]" caption="Data Tentativa.Ano - Dia" time="1" defaultMemberUniqueName="[Data Tentativa].[Ano - Dia].[All]" allUniqueName="[Data Tentativa].[Ano - Dia].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="5" unbalanced="0">
-      <fieldsUsage count="5">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="8"/>
-        <fieldUsage x="9"/>
-        <fieldUsage x="10"/>
-        <fieldUsage x="11"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Data]" caption="Data Tentativa.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Data].[All]" allUniqueName="[Data Tentativa].[Data].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Dia Da Semana Nome]" caption="Data Tentativa.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia Da Semana Nome].[All]" allUniqueName="[Data Tentativa].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Dia Da Semana Número]" caption="Data Tentativa.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia Da Semana Número].[All]" allUniqueName="[Data Tentativa].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Mês Nome]" caption="Data Tentativa.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Mês Nome].[All]" allUniqueName="[Data Tentativa].[Mês Nome].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Activo]" caption="Activo" attribute="1" defaultMemberUniqueName="[Funcionário].[Activo].[All]" allUniqueName="[Funcionário].[Activo].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Localização - Loja]" caption="Localização - Loja" defaultMemberUniqueName="[Funcionário].[Localização - Loja].[All]" allUniqueName="[Funcionário].[Localização - Loja].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="4" unbalanced="0">
-      <fieldsUsage count="4">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-        <fieldUsage x="2"/>
-        <fieldUsage x="3"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Funcionário].[Nome]" caption="Nome" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome].[All]" allUniqueName="[Funcionário].[Nome].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Nome Do Chefe]" caption="Nome Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Do Chefe].[All]" allUniqueName="[Funcionário].[Nome Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Por Função Do Chefe]" caption="Por Função Do Chefe" defaultMemberUniqueName="[Funcionário].[Por Função Do Chefe].[All]" allUniqueName="[Funcionário].[Por Função Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Por Nome Completo Do Chefe]" caption="Por Nome Completo Do Chefe" defaultMemberUniqueName="[Funcionário].[Por Nome Completo Do Chefe].[All]" allUniqueName="[Funcionário].[Por Nome Completo Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Sobrenome]" caption="Sobrenome" attribute="1" defaultMemberUniqueName="[Funcionário].[Sobrenome].[All]" allUniqueName="[Funcionário].[Sobrenome].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Sobrenome Do Chefe]" caption="Sobrenome Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Sobrenome Do Chefe].[All]" allUniqueName="[Funcionário].[Sobrenome Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Conclusao].[Hora 12h]" caption="Hora Conclusao.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Conclusao].[Hora 12h].[All]" allUniqueName="[Hora Conclusao].[Hora 12h].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Conclusao].[Hora 24h]" caption="Hora Conclusao.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Conclusao].[Hora 24h].[All]" allUniqueName="[Hora Conclusao].[Hora 24h].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Entrega].[Hora 12h]" caption="Hora Entrega.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Entrega].[Hora 12h].[All]" allUniqueName="[Hora Entrega].[Hora 12h].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Entrega].[Hora 24h]" caption="Hora Entrega.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Entrega].[Hora 24h].[All]" allUniqueName="[Hora Entrega].[Hora 24h].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Requisicao].[Hora 12h]" caption="Hora Requisicao.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Requisicao].[Hora 12h].[All]" allUniqueName="[Hora Requisicao].[Hora 12h].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Requisicao].[Hora 24h]" caption="Hora Requisicao.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Requisicao].[Hora 24h].[All]" allUniqueName="[Hora Requisicao].[Hora 24h].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Tentativa].[Hora 12h]" caption="Hora Tentativa.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Tentativa].[Hora 12h].[All]" allUniqueName="[Hora Tentativa].[Hora 12h].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Tentativa].[Hora 24h]" caption="Hora Tentativa.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Tentativa].[Hora 24h].[All]" allUniqueName="[Hora Tentativa].[Hora 24h].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Intervalo]" caption="Intervalo Idade Cliente.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Intervalo].[All]" allUniqueName="[Intervalo Idade Cliente].[Intervalo].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Nome]" caption="Intervalo Idade Cliente.Nome" attribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Nome].[All]" allUniqueName="[Intervalo Idade Cliente].[Nome].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Intervalo]" caption="Intervalo Idade Na Requisição.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Intervalo].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Intervalo].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Nome]" caption="Intervalo Idade Na Requisição.Nome" attribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Nome].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Nome].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Classe]" caption="Intervalo Rendimento Cliente.Classe" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Classe].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Classe].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Codigo]" caption="Intervalo Rendimento Cliente.Codigo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Codigo].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Codigo].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Intervalo]" caption="Intervalo Rendimento Cliente.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Intervalo].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Intervalo].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Classe]" caption="Intervalo Rendimento Na Requisição.Classe" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Classe].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Classe].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Codigo]" caption="Intervalo Rendimento Na Requisição.Codigo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Codigo].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Codigo].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Intervalo]" caption="Intervalo Rendimento Na Requisição.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Intervalo].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Intervalo].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Código Postal]" caption="Morada Entrega.Código Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Código Postal].[All]" allUniqueName="[Morada Entrega].[Código Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Código Postal Completo]" caption="Morada Entrega.Código Postal Completo" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Código Postal Completo].[All]" allUniqueName="[Morada Entrega].[Código Postal Completo].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Designação Postal]" caption="Morada Entrega.Designação Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Designação Postal].[All]" allUniqueName="[Morada Entrega].[Designação Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Distrito - Número Da Porta]" caption="Morada Entrega.Distrito - Número Da Porta" defaultMemberUniqueName="[Morada Entrega].[Distrito - Número Da Porta].[All]" allUniqueName="[Morada Entrega].[Distrito - Número Da Porta].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Extensão Código Postal]" caption="Morada Entrega.Extensão Código Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Extensão Código Postal].[All]" allUniqueName="[Morada Entrega].[Extensão Código Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Localidade]" caption="Morada Entrega.Localidade" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Localidade].[All]" allUniqueName="[Morada Entrega].[Localidade].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Código Postal]" caption="Morada Facturacao.Código Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Código Postal].[All]" allUniqueName="[Morada Facturacao].[Código Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Código Postal Completo]" caption="Morada Facturacao.Código Postal Completo" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Código Postal Completo].[All]" allUniqueName="[Morada Facturacao].[Código Postal Completo].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Designação Postal]" caption="Morada Facturacao.Designação Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Designação Postal].[All]" allUniqueName="[Morada Facturacao].[Designação Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Distrito - Número Da Porta]" caption="Morada Facturacao.Distrito - Número Da Porta" defaultMemberUniqueName="[Morada Facturacao].[Distrito - Número Da Porta].[All]" allUniqueName="[Morada Facturacao].[Distrito - Número Da Porta].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Extensão Código Postal]" caption="Morada Facturacao.Extensão Código Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Extensão Código Postal].[All]" allUniqueName="[Morada Facturacao].[Extensão Código Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Localidade]" caption="Morada Facturacao.Localidade" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Localidade].[All]" allUniqueName="[Morada Facturacao].[Localidade].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Tipo Servico].[Tipo]" caption="Tipo" attribute="1" defaultMemberUniqueName="[Tipo Servico].[Tipo].[All]" allUniqueName="[Tipo Servico].[Tipo].[All]" dimensionUniqueName="[Tipo Servico]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="15"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Cliente].[Designação]" caption="Designação" attribute="1" defaultMemberUniqueName="[Cliente].[Designação].[All]" allUniqueName="[Cliente].[Designação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente].[Keycol].[All]" allUniqueName="[Cliente].[Keycol].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Nome Completo De Contacto]" caption="Nome Completo De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Nome Completo De Contacto].[All]" allUniqueName="[Cliente].[Nome Completo De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Ano]" caption="Data Conclusao.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Ano].[All]" allUniqueName="[Data Conclusao].[Ano].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Dia]" caption="Data Conclusao.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia].[All]" allUniqueName="[Data Conclusao].[Dia].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Keycol]" caption="Data Conclusao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Conclusao].[Keycol].[All]" allUniqueName="[Data Conclusao].[Keycol].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Mês Número]" caption="Data Conclusao.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Mês Número].[All]" allUniqueName="[Data Conclusao].[Mês Número].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Trimestre]" caption="Data Conclusao.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Trimestre].[All]" allUniqueName="[Data Conclusao].[Trimestre].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Ano]" caption="Data Requisicao.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Ano].[All]" allUniqueName="[Data Requisicao].[Ano].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Dia]" caption="Data Requisicao.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia].[All]" allUniqueName="[Data Requisicao].[Dia].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Keycol]" caption="Data Requisicao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Requisicao].[Keycol].[All]" allUniqueName="[Data Requisicao].[Keycol].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Mês Número]" caption="Data Requisicao.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Mês Número].[All]" allUniqueName="[Data Requisicao].[Mês Número].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Trimestre]" caption="Data Requisicao.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Trimestre].[All]" allUniqueName="[Data Requisicao].[Trimestre].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Ano]" caption="Data Tentativa.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Ano].[All]" allUniqueName="[Data Tentativa].[Ano].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Dia]" caption="Data Tentativa.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia].[All]" allUniqueName="[Data Tentativa].[Dia].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Keycol]" caption="Data Tentativa.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Tentativa].[Keycol].[All]" allUniqueName="[Data Tentativa].[Keycol].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Mês Número]" caption="Data Tentativa.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Mês Número].[All]" allUniqueName="[Data Tentativa].[Mês Número].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Trimestre]" caption="Data Tentativa.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Trimestre].[All]" allUniqueName="[Data Tentativa].[Trimestre].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Função]" caption="Função" attribute="1" defaultMemberUniqueName="[Funcionário].[Função].[All]" allUniqueName="[Funcionário].[Função].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Função Do Chefe]" caption="Função Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Função Do Chefe].[All]" allUniqueName="[Funcionário].[Função Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Funcionário].[Keycol].[All]" allUniqueName="[Funcionário].[Keycol].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Localização]" caption="Localização" attribute="1" defaultMemberUniqueName="[Funcionário].[Localização].[All]" allUniqueName="[Funcionário].[Localização].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Loja]" caption="Loja" attribute="1" defaultMemberUniqueName="[Funcionário].[Loja].[All]" allUniqueName="[Funcionário].[Loja].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Nome Completo]" caption="Nome Completo" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Completo].[All]" allUniqueName="[Funcionário].[Nome Completo].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Nome Completo Do Chefe]" caption="Nome Completo Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Completo Do Chefe].[All]" allUniqueName="[Funcionário].[Nome Completo Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Hora Conclusao].[Keycol]" caption="Hora Conclusao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Conclusao].[Keycol].[All]" allUniqueName="[Hora Conclusao].[Keycol].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Hora Entrega].[Keycol]" caption="Hora Entrega.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Entrega].[Keycol].[All]" allUniqueName="[Hora Entrega].[Keycol].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Hora Requisicao].[Keycol]" caption="Hora Requisicao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Requisicao].[Keycol].[All]" allUniqueName="[Hora Requisicao].[Keycol].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Hora Tentativa].[Keycol]" caption="Hora Tentativa.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Tentativa].[Keycol].[All]" allUniqueName="[Hora Tentativa].[Keycol].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Keycol]" caption="Intervalo Idade Cliente.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Keycol].[All]" allUniqueName="[Intervalo Idade Cliente].[Keycol].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Keycol]" caption="Intervalo Idade Na Requisição.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Keycol].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Keycol].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Keycol]" caption="Intervalo Rendimento Cliente.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Keycol].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Keycol].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Keycol]" caption="Intervalo Rendimento Na Requisição.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Keycol].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Keycol].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Concelho]" caption="Morada Entrega.Concelho" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Concelho].[All]" allUniqueName="[Morada Entrega].[Concelho].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Distrito]" caption="Morada Entrega.Distrito" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Distrito].[All]" allUniqueName="[Morada Entrega].[Distrito].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Freguesia]" caption="Morada Entrega.Freguesia" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Freguesia].[All]" allUniqueName="[Morada Entrega].[Freguesia].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Keycol]" caption="Morada Entrega.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Morada Entrega].[Keycol].[All]" allUniqueName="[Morada Entrega].[Keycol].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Número Da Porta]" caption="Morada Entrega.Número Da Porta" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Número Da Porta].[All]" allUniqueName="[Morada Entrega].[Número Da Porta].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Rua]" caption="Morada Entrega.Rua" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Rua].[All]" allUniqueName="[Morada Entrega].[Rua].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Concelho]" caption="Morada Facturacao.Concelho" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Concelho].[All]" allUniqueName="[Morada Facturacao].[Concelho].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Distrito]" caption="Morada Facturacao.Distrito" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Distrito].[All]" allUniqueName="[Morada Facturacao].[Distrito].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Freguesia]" caption="Morada Facturacao.Freguesia" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Freguesia].[All]" allUniqueName="[Morada Facturacao].[Freguesia].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Keycol]" caption="Morada Facturacao.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Morada Facturacao].[Keycol].[All]" allUniqueName="[Morada Facturacao].[Keycol].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Número Da Porta]" caption="Morada Facturacao.Número Da Porta" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Número Da Porta].[All]" allUniqueName="[Morada Facturacao].[Número Da Porta].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Rua]" caption="Morada Facturacao.Rua" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Rua].[All]" allUniqueName="[Morada Facturacao].[Rua].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Tipo Servico].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Tipo Servico].[Keycol].[All]" allUniqueName="[Tipo Servico].[Keycol].[All]" dimensionUniqueName="[Tipo Servico]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Número De Entregas]" caption="Número De Entregas" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Valor]" caption="Valor" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Dentro Do SLA]" caption="Dentro Do SLA" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Concluido]" caption="Concluido" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Contagem de Servicos]" caption="Contagem de Servicos" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Número Entregas por Serviço]" caption="Número Entregas por Serviço" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Valor do Serviço]" caption="Valor do Serviço" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Serviço Dentro Do SLA]" caption="Serviço Dentro Do SLA" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Serviço Concluido]" caption="Serviço Concluido" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Sucesso]" caption="Sucesso" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Contagem de Entregas]" caption="Contagem de Entregas" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <dimensions count="17">
-    <dimension name="Cliente" uniqueName="[Cliente]" caption="Cliente"/>
-    <dimension name="Data Conclusao" uniqueName="[Data Conclusao]" caption="Data Conclusao"/>
-    <dimension name="Data Requisicao" uniqueName="[Data Requisicao]" caption="Data Requisicao"/>
-    <dimension name="Data Tentativa" uniqueName="[Data Tentativa]" caption="Data Tentativa"/>
-    <dimension name="Funcionário" uniqueName="[Funcionário]" caption="Funcionário"/>
-    <dimension name="Hora Conclusao" uniqueName="[Hora Conclusao]" caption="Hora Conclusao"/>
-    <dimension name="Hora Entrega" uniqueName="[Hora Entrega]" caption="Hora Entrega"/>
-    <dimension name="Hora Requisicao" uniqueName="[Hora Requisicao]" caption="Hora Requisicao"/>
-    <dimension name="Hora Tentativa" uniqueName="[Hora Tentativa]" caption="Hora Tentativa"/>
-    <dimension name="Intervalo Idade Cliente" uniqueName="[Intervalo Idade Cliente]" caption="Intervalo Idade Cliente"/>
-    <dimension name="Intervalo Idade Na Requisição" uniqueName="[Intervalo Idade Na Requisição]" caption="Intervalo Idade Na Requisição"/>
-    <dimension name="Intervalo Rendimento Cliente" uniqueName="[Intervalo Rendimento Cliente]" caption="Intervalo Rendimento Cliente"/>
-    <dimension name="Intervalo Rendimento Na Requisição" uniqueName="[Intervalo Rendimento Na Requisição]" caption="Intervalo Rendimento Na Requisição"/>
-    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
-    <dimension name="Morada Entrega" uniqueName="[Morada Entrega]" caption="Morada Entrega"/>
-    <dimension name="Morada Facturacao" uniqueName="[Morada Facturacao]" caption="Morada Facturacao"/>
-    <dimension name="Tipo Servico" uniqueName="[Tipo Servico]" caption="Tipo Servico"/>
-  </dimensions>
-  <measureGroups count="2">
-    <measureGroup name="Entregas Dos Servicos" caption="Entregas Dos Servicos"/>
-    <measureGroup name="Servicos" caption="Servicos"/>
-  </measureGroups>
-  <maps count="25">
-    <map measureGroup="0" dimension="0"/>
-    <map measureGroup="0" dimension="1"/>
-    <map measureGroup="0" dimension="2"/>
-    <map measureGroup="0" dimension="3"/>
-    <map measureGroup="0" dimension="4"/>
-    <map measureGroup="0" dimension="5"/>
-    <map measureGroup="0" dimension="6"/>
-    <map measureGroup="0" dimension="7"/>
-    <map measureGroup="0" dimension="8"/>
-    <map measureGroup="0" dimension="9"/>
-    <map measureGroup="0" dimension="11"/>
-    <map measureGroup="0" dimension="14"/>
-    <map measureGroup="0" dimension="15"/>
-    <map measureGroup="0" dimension="16"/>
-    <map measureGroup="1" dimension="0"/>
-    <map measureGroup="1" dimension="1"/>
-    <map measureGroup="1" dimension="2"/>
-    <map measureGroup="1" dimension="5"/>
-    <map measureGroup="1" dimension="6"/>
-    <map measureGroup="1" dimension="7"/>
-    <map measureGroup="1" dimension="10"/>
-    <map measureGroup="1" dimension="12"/>
-    <map measureGroup="1" dimension="14"/>
-    <map measureGroup="1" dimension="15"/>
-    <map measureGroup="1" dimension="16"/>
-  </maps>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Rui Miranda" refreshedDate="41444.125984722225" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
-  <cacheSource type="external" connectionId="5"/>
-  <cacheFields count="19">
-    <cacheField name="[Measures].[Contagem de Entregas]" caption="Contagem de Entregas" numFmtId="0" hierarchy="129" level="32767"/>
-    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Distrito]" caption="Distrito" numFmtId="0" hierarchy="69" level="1">
-      <sharedItems count="2">
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Distrito].&amp;[Lisboa]" c="Lisboa"/>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Distrito].&amp;[Porto]" c="Porto"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Concelho]" caption="Concelho" numFmtId="0" hierarchy="69" level="2" mappingCount="1">
-      <sharedItems count="2">
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Concelho].&amp;[Lisboa]&amp;[Lisboa]" c="Lisboa" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Concelho].&amp;[Porto]&amp;[Porto]" c="Porto" cp="1">
-          <x v="1"/>
-        </s>
-      </sharedItems>
-      <mpMap v="6"/>
-    </cacheField>
-    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia]" caption="Freguesia" numFmtId="0" hierarchy="69" level="3" mappingCount="1">
-      <sharedItems count="50">
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Ajuda]" c="Ajuda" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Alcântara]" c="Alcântara" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Alvalade]" c="Alvalade" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Anjos]" c="Anjos" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Beato]" c="Beato" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Benfica]" c="Benfica" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Campo Grande]" c="Campo Grande" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Campolide]" c="Campolide" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Carnide]" c="Carnide" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Coração de Jesus]" c="Coração de Jesus" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Encarnação]" c="Encarnação" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Lapa]" c="Lapa" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Lumiar]" c="Lumiar" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Madalena]" c="Madalena" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Mártires]" c="Mártires" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Marvila]" c="Marvila" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Nossa Senhora de Fátima]" c="Nossa Senhora de Fátima" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Pena]" c="Pena" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Penha de França]" c="Penha de França" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Prazeres]" c="Prazeres" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Sacramento]" c="Sacramento" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santa Catarina]" c="Santa Catarina" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santa Engrácia]" c="Santa Engrácia" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santa Isabel]" c="Santa Isabel" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santa Maria de Belém]" c="Santa Maria de Belém" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santa Maria dos Olivais]" c="Santa Maria dos Olivais" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santo Condestável]" c="Santo Condestável" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santos-o-Velho]" c="Santos-o-Velho" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Cristóvão]" c="São Cristóvão" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Domingos de Benfica]" c="São Domingos de Benfica" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São João de Brito]" c="São João de Brito" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São João de Deus]" c="São João de Deus" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Jorge de Arroios]" c="São Jorge de Arroios" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São José]" c="São José" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Mamede]" c="São Mamede" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Nicolau]" c="São Nicolau" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Paulo]" c="São Paulo" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Sebastião da Pedreira]" c="São Sebastião da Pedreira" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Vicente de Fora]" c="São Vicente de Fora" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Sé]" c="Sé" cp="1">
-          <x/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Aldoar]" c="Aldoar" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Bonfim]" c="Bonfim" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Campanhã]" c="Campanhã" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Cedofeita]" c="Cedofeita" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Lordelo do Ouro]" c="Lordelo do Ouro" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Massarelos]" c="Massarelos" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Paranhos]" c="Paranhos" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Ramalde]" c="Ramalde" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Santo Ildefonso]" c="Santo Ildefonso" cp="1">
-          <x v="1"/>
-        </s>
-        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Vitória]" c="Vitória" cp="1">
-          <x v="1"/>
-        </s>
-      </sharedItems>
-      <mpMap v="7"/>
-    </cacheField>
-    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Rua]" caption="Rua" numFmtId="0" hierarchy="69" level="4">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Número Da Porta]" caption="Número Da Porta" numFmtId="0" hierarchy="69" level="5">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Concelho].[Distrito]" caption="Distrito" propertyName="Distrito" numFmtId="0" hierarchy="69" level="2" memberPropertyField="1">
-      <sharedItems count="2">
-        <s v="Lisboa"/>
-        <s v="Porto"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].[Concelho]" caption="Concelho" propertyName="Concelho" numFmtId="0" hierarchy="69" level="3" memberPropertyField="1">
-      <sharedItems count="2">
-        <s v="Lisboa"/>
-        <s v="Porto"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Rua].[Freguesia]" caption="Freguesia" propertyName="Freguesia" numFmtId="0" hierarchy="69" level="4" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Número Da Porta].[Rua]" caption="Rua" propertyName="Rua" numFmtId="0" hierarchy="69" level="5" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Tipo Servico].[Tipo].[Tipo]" caption="Tipo" numFmtId="0" hierarchy="72" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Ano]" caption="Ano" numFmtId="0" hierarchy="29" level="1">
-      <sharedItems count="4">
-        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2010]" c="2010"/>
-        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2011]" c="2011"/>
-        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2012]" c="2012"/>
-        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2013]" c="2013"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Trimestre]" caption="Trimestre" numFmtId="0" hierarchy="29" level="2" mappingCount="1">
-      <sharedItems count="2">
-        <s v="[Data Tentativa].[Ano - Dia].[Trimestre].&amp;[2013]&amp;[1]" c="1" cp="1">
-          <x/>
-        </s>
-        <s v="[Data Tentativa].[Ano - Dia].[Trimestre].&amp;[2013]&amp;[2]" c="2" cp="1">
-          <x/>
-        </s>
-      </sharedItems>
-      <mpMap v="15"/>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Mês Número]" caption="Mês Número" numFmtId="0" hierarchy="29" level="3">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Dia]" caption="Dia" numFmtId="0" hierarchy="29" level="4">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Trimestre].[Ano]" caption="Ano" propertyName="Ano" numFmtId="0" hierarchy="29" level="2" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2013" maxValue="2013" count="1">
-        <n v="2013"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Mês Número].[Trimestre]" caption="Trimestre" propertyName="Trimestre" numFmtId="0" hierarchy="29" level="3" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Dia].[Mês Número]" caption="Mês Número" propertyName="Mês Número" numFmtId="0" hierarchy="29" level="4" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="Dummy0" numFmtId="0" hierarchy="130" level="32767">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{63CAB8AC-B538-458d-9737-405883B0398D}">
-          <x14:cacheField ignore="1"/>
-        </ext>
-      </extLst>
-    </cacheField>
-  </cacheFields>
-  <cacheHierarchies count="131">
-    <cacheHierarchy uniqueName="[Cliente].[Activo]" caption="Activo" attribute="1" defaultMemberUniqueName="[Cliente].[Activo].[All]" allUniqueName="[Cliente].[Activo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Codigo Postal]" caption="Codigo Postal" attribute="1" defaultMemberUniqueName="[Cliente].[Codigo Postal].[All]" allUniqueName="[Cliente].[Codigo Postal].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Educação]" caption="Educação" attribute="1" defaultMemberUniqueName="[Cliente].[Educação].[All]" allUniqueName="[Cliente].[Educação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Estado Civil]" caption="Estado Civil" attribute="1" defaultMemberUniqueName="[Cliente].[Estado Civil].[All]" allUniqueName="[Cliente].[Estado Civil].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Género]" caption="Género" attribute="1" defaultMemberUniqueName="[Cliente].[Género].[All]" allUniqueName="[Cliente].[Género].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Idade]" caption="Intervalo Idade" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Idade].[All]" allUniqueName="[Cliente].[Intervalo Idade].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Idade Nome]" caption="Intervalo Idade Nome" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Idade Nome].[All]" allUniqueName="[Cliente].[Intervalo Idade Nome].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento]" caption="Intervalo Rendimento" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento].[All]" allUniqueName="[Cliente].[Intervalo Rendimento].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento Classe]" caption="Intervalo Rendimento Classe" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento Classe].[All]" allUniqueName="[Cliente].[Intervalo Rendimento Classe].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento Codigo]" caption="Intervalo Rendimento Codigo" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento Codigo].[All]" allUniqueName="[Cliente].[Intervalo Rendimento Codigo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Nome De Contacto]" caption="Nome De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Nome De Contacto].[All]" allUniqueName="[Cliente].[Nome De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Número De Carros Possuidos]" caption="Número De Carros Possuidos" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Carros Possuidos].[All]" allUniqueName="[Cliente].[Número De Carros Possuidos].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Número De Filhos]" caption="Número De Filhos" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Filhos].[All]" allUniqueName="[Cliente].[Número De Filhos].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Número De Filhos Em Casa]" caption="Número De Filhos Em Casa" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Filhos Em Casa].[All]" allUniqueName="[Cliente].[Número De Filhos Em Casa].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Ocupação]" caption="Ocupação" attribute="1" defaultMemberUniqueName="[Cliente].[Ocupação].[All]" allUniqueName="[Cliente].[Ocupação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Por Designação]" caption="Por Designação" defaultMemberUniqueName="[Cliente].[Por Designação].[All]" allUniqueName="[Cliente].[Por Designação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Possui Casa]" caption="Possui Casa" attribute="1" defaultMemberUniqueName="[Cliente].[Possui Casa].[All]" allUniqueName="[Cliente].[Possui Casa].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Singular]" caption="Singular" attribute="1" defaultMemberUniqueName="[Cliente].[Singular].[All]" allUniqueName="[Cliente].[Singular].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Sobrenome De Contacto]" caption="Sobrenome De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Sobrenome De Contacto].[All]" allUniqueName="[Cliente].[Sobrenome De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Ano - Dia]" caption="Data Conclusao.Ano - Dia" time="1" defaultMemberUniqueName="[Data Conclusao].[Ano - Dia].[All]" allUniqueName="[Data Conclusao].[Ano - Dia].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Data]" caption="Data Conclusao.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Data].[All]" allUniqueName="[Data Conclusao].[Data].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Dia Da Semana Nome]" caption="Data Conclusao.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia Da Semana Nome].[All]" allUniqueName="[Data Conclusao].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Dia Da Semana Número]" caption="Data Conclusao.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia Da Semana Número].[All]" allUniqueName="[Data Conclusao].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Mês Nome]" caption="Data Conclusao.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Mês Nome].[All]" allUniqueName="[Data Conclusao].[Mês Nome].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Ano - Dia]" caption="Data Requisicao.Ano - Dia" time="1" defaultMemberUniqueName="[Data Requisicao].[Ano - Dia].[All]" allUniqueName="[Data Requisicao].[Ano - Dia].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Data]" caption="Data Requisicao.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Data].[All]" allUniqueName="[Data Requisicao].[Data].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Dia Da Semana Nome]" caption="Data Requisicao.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia Da Semana Nome].[All]" allUniqueName="[Data Requisicao].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Dia Da Semana Número]" caption="Data Requisicao.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia Da Semana Número].[All]" allUniqueName="[Data Requisicao].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Mês Nome]" caption="Data Requisicao.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Mês Nome].[All]" allUniqueName="[Data Requisicao].[Mês Nome].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Ano - Dia]" caption="Data Tentativa.Ano - Dia" time="1" defaultMemberUniqueName="[Data Tentativa].[Ano - Dia].[All]" allUniqueName="[Data Tentativa].[Ano - Dia].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="5" unbalanced="0">
-      <fieldsUsage count="5">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="11"/>
-        <fieldUsage x="12"/>
-        <fieldUsage x="13"/>
-        <fieldUsage x="14"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Data]" caption="Data Tentativa.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Data].[All]" allUniqueName="[Data Tentativa].[Data].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Dia Da Semana Nome]" caption="Data Tentativa.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia Da Semana Nome].[All]" allUniqueName="[Data Tentativa].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Dia Da Semana Número]" caption="Data Tentativa.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia Da Semana Número].[All]" allUniqueName="[Data Tentativa].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Mês Nome]" caption="Data Tentativa.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Mês Nome].[All]" allUniqueName="[Data Tentativa].[Mês Nome].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Activo]" caption="Activo" attribute="1" defaultMemberUniqueName="[Funcionário].[Activo].[All]" allUniqueName="[Funcionário].[Activo].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Localização - Loja]" caption="Localização - Loja" defaultMemberUniqueName="[Funcionário].[Localização - Loja].[All]" allUniqueName="[Funcionário].[Localização - Loja].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Nome]" caption="Nome" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome].[All]" allUniqueName="[Funcionário].[Nome].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Nome Do Chefe]" caption="Nome Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Do Chefe].[All]" allUniqueName="[Funcionário].[Nome Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Por Função Do Chefe]" caption="Por Função Do Chefe" defaultMemberUniqueName="[Funcionário].[Por Função Do Chefe].[All]" allUniqueName="[Funcionário].[Por Função Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Por Nome Completo Do Chefe]" caption="Por Nome Completo Do Chefe" defaultMemberUniqueName="[Funcionário].[Por Nome Completo Do Chefe].[All]" allUniqueName="[Funcionário].[Por Nome Completo Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Sobrenome]" caption="Sobrenome" attribute="1" defaultMemberUniqueName="[Funcionário].[Sobrenome].[All]" allUniqueName="[Funcionário].[Sobrenome].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Sobrenome Do Chefe]" caption="Sobrenome Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Sobrenome Do Chefe].[All]" allUniqueName="[Funcionário].[Sobrenome Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Conclusao].[Hora 12h]" caption="Hora Conclusao.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Conclusao].[Hora 12h].[All]" allUniqueName="[Hora Conclusao].[Hora 12h].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Conclusao].[Hora 24h]" caption="Hora Conclusao.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Conclusao].[Hora 24h].[All]" allUniqueName="[Hora Conclusao].[Hora 24h].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Entrega].[Hora 12h]" caption="Hora Entrega.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Entrega].[Hora 12h].[All]" allUniqueName="[Hora Entrega].[Hora 12h].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Entrega].[Hora 24h]" caption="Hora Entrega.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Entrega].[Hora 24h].[All]" allUniqueName="[Hora Entrega].[Hora 24h].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Requisicao].[Hora 12h]" caption="Hora Requisicao.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Requisicao].[Hora 12h].[All]" allUniqueName="[Hora Requisicao].[Hora 12h].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Requisicao].[Hora 24h]" caption="Hora Requisicao.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Requisicao].[Hora 24h].[All]" allUniqueName="[Hora Requisicao].[Hora 24h].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Tentativa].[Hora 12h]" caption="Hora Tentativa.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Tentativa].[Hora 12h].[All]" allUniqueName="[Hora Tentativa].[Hora 12h].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Tentativa].[Hora 24h]" caption="Hora Tentativa.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Tentativa].[Hora 24h].[All]" allUniqueName="[Hora Tentativa].[Hora 24h].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Intervalo]" caption="Intervalo Idade Cliente.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Intervalo].[All]" allUniqueName="[Intervalo Idade Cliente].[Intervalo].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Nome]" caption="Intervalo Idade Cliente.Nome" attribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Nome].[All]" allUniqueName="[Intervalo Idade Cliente].[Nome].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Intervalo]" caption="Intervalo Idade Na Requisição.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Intervalo].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Intervalo].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Nome]" caption="Intervalo Idade Na Requisição.Nome" attribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Nome].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Nome].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Classe]" caption="Intervalo Rendimento Cliente.Classe" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Classe].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Classe].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Codigo]" caption="Intervalo Rendimento Cliente.Codigo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Codigo].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Codigo].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Intervalo]" caption="Intervalo Rendimento Cliente.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Intervalo].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Intervalo].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Classe]" caption="Intervalo Rendimento Na Requisição.Classe" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Classe].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Classe].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Codigo]" caption="Intervalo Rendimento Na Requisição.Codigo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Codigo].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Codigo].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Intervalo]" caption="Intervalo Rendimento Na Requisição.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Intervalo].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Intervalo].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Código Postal]" caption="Morada Entrega.Código Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Código Postal].[All]" allUniqueName="[Morada Entrega].[Código Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Código Postal Completo]" caption="Morada Entrega.Código Postal Completo" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Código Postal Completo].[All]" allUniqueName="[Morada Entrega].[Código Postal Completo].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Designação Postal]" caption="Morada Entrega.Designação Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Designação Postal].[All]" allUniqueName="[Morada Entrega].[Designação Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Distrito - Número Da Porta]" caption="Morada Entrega.Distrito - Número Da Porta" defaultMemberUniqueName="[Morada Entrega].[Distrito - Número Da Porta].[All]" allUniqueName="[Morada Entrega].[Distrito - Número Da Porta].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Extensão Código Postal]" caption="Morada Entrega.Extensão Código Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Extensão Código Postal].[All]" allUniqueName="[Morada Entrega].[Extensão Código Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Localidade]" caption="Morada Entrega.Localidade" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Localidade].[All]" allUniqueName="[Morada Entrega].[Localidade].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Código Postal]" caption="Morada Facturacao.Código Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Código Postal].[All]" allUniqueName="[Morada Facturacao].[Código Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Código Postal Completo]" caption="Morada Facturacao.Código Postal Completo" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Código Postal Completo].[All]" allUniqueName="[Morada Facturacao].[Código Postal Completo].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Designação Postal]" caption="Morada Facturacao.Designação Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Designação Postal].[All]" allUniqueName="[Morada Facturacao].[Designação Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Distrito - Número Da Porta]" caption="Morada Facturacao.Distrito - Número Da Porta" defaultMemberUniqueName="[Morada Facturacao].[Distrito - Número Da Porta].[All]" allUniqueName="[Morada Facturacao].[Distrito - Número Da Porta].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="6" unbalanced="0">
-      <fieldsUsage count="6">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-        <fieldUsage x="2"/>
-        <fieldUsage x="3"/>
-        <fieldUsage x="4"/>
-        <fieldUsage x="5"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Extensão Código Postal]" caption="Morada Facturacao.Extensão Código Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Extensão Código Postal].[All]" allUniqueName="[Morada Facturacao].[Extensão Código Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Localidade]" caption="Morada Facturacao.Localidade" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Localidade].[All]" allUniqueName="[Morada Facturacao].[Localidade].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Tipo Servico].[Tipo]" caption="Tipo" attribute="1" defaultMemberUniqueName="[Tipo Servico].[Tipo].[All]" allUniqueName="[Tipo Servico].[Tipo].[All]" dimensionUniqueName="[Tipo Servico]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="10"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Cliente].[Designação]" caption="Designação" attribute="1" defaultMemberUniqueName="[Cliente].[Designação].[All]" allUniqueName="[Cliente].[Designação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente].[Keycol].[All]" allUniqueName="[Cliente].[Keycol].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Nome Completo De Contacto]" caption="Nome Completo De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Nome Completo De Contacto].[All]" allUniqueName="[Cliente].[Nome Completo De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Ano]" caption="Data Conclusao.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Ano].[All]" allUniqueName="[Data Conclusao].[Ano].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Dia]" caption="Data Conclusao.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia].[All]" allUniqueName="[Data Conclusao].[Dia].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Keycol]" caption="Data Conclusao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Conclusao].[Keycol].[All]" allUniqueName="[Data Conclusao].[Keycol].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Mês Número]" caption="Data Conclusao.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Mês Número].[All]" allUniqueName="[Data Conclusao].[Mês Número].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Trimestre]" caption="Data Conclusao.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Trimestre].[All]" allUniqueName="[Data Conclusao].[Trimestre].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Ano]" caption="Data Requisicao.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Ano].[All]" allUniqueName="[Data Requisicao].[Ano].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Dia]" caption="Data Requisicao.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia].[All]" allUniqueName="[Data Requisicao].[Dia].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Keycol]" caption="Data Requisicao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Requisicao].[Keycol].[All]" allUniqueName="[Data Requisicao].[Keycol].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Mês Número]" caption="Data Requisicao.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Mês Número].[All]" allUniqueName="[Data Requisicao].[Mês Número].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Trimestre]" caption="Data Requisicao.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Trimestre].[All]" allUniqueName="[Data Requisicao].[Trimestre].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Ano]" caption="Data Tentativa.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Ano].[All]" allUniqueName="[Data Tentativa].[Ano].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Dia]" caption="Data Tentativa.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia].[All]" allUniqueName="[Data Tentativa].[Dia].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Keycol]" caption="Data Tentativa.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Tentativa].[Keycol].[All]" allUniqueName="[Data Tentativa].[Keycol].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Mês Número]" caption="Data Tentativa.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Mês Número].[All]" allUniqueName="[Data Tentativa].[Mês Número].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Trimestre]" caption="Data Tentativa.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Trimestre].[All]" allUniqueName="[Data Tentativa].[Trimestre].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Função]" caption="Função" attribute="1" defaultMemberUniqueName="[Funcionário].[Função].[All]" allUniqueName="[Funcionário].[Função].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Função Do Chefe]" caption="Função Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Função Do Chefe].[All]" allUniqueName="[Funcionário].[Função Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Funcionário].[Keycol].[All]" allUniqueName="[Funcionário].[Keycol].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Localização]" caption="Localização" attribute="1" defaultMemberUniqueName="[Funcionário].[Localização].[All]" allUniqueName="[Funcionário].[Localização].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Loja]" caption="Loja" attribute="1" defaultMemberUniqueName="[Funcionário].[Loja].[All]" allUniqueName="[Funcionário].[Loja].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Nome Completo]" caption="Nome Completo" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Completo].[All]" allUniqueName="[Funcionário].[Nome Completo].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Nome Completo Do Chefe]" caption="Nome Completo Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Completo Do Chefe].[All]" allUniqueName="[Funcionário].[Nome Completo Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Hora Conclusao].[Keycol]" caption="Hora Conclusao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Conclusao].[Keycol].[All]" allUniqueName="[Hora Conclusao].[Keycol].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Hora Entrega].[Keycol]" caption="Hora Entrega.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Entrega].[Keycol].[All]" allUniqueName="[Hora Entrega].[Keycol].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Hora Requisicao].[Keycol]" caption="Hora Requisicao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Requisicao].[Keycol].[All]" allUniqueName="[Hora Requisicao].[Keycol].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Hora Tentativa].[Keycol]" caption="Hora Tentativa.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Tentativa].[Keycol].[All]" allUniqueName="[Hora Tentativa].[Keycol].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Keycol]" caption="Intervalo Idade Cliente.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Keycol].[All]" allUniqueName="[Intervalo Idade Cliente].[Keycol].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Keycol]" caption="Intervalo Idade Na Requisição.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Keycol].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Keycol].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Keycol]" caption="Intervalo Rendimento Cliente.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Keycol].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Keycol].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Keycol]" caption="Intervalo Rendimento Na Requisição.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Keycol].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Keycol].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Concelho]" caption="Morada Entrega.Concelho" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Concelho].[All]" allUniqueName="[Morada Entrega].[Concelho].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Distrito]" caption="Morada Entrega.Distrito" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Distrito].[All]" allUniqueName="[Morada Entrega].[Distrito].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Freguesia]" caption="Morada Entrega.Freguesia" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Freguesia].[All]" allUniqueName="[Morada Entrega].[Freguesia].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Keycol]" caption="Morada Entrega.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Morada Entrega].[Keycol].[All]" allUniqueName="[Morada Entrega].[Keycol].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Número Da Porta]" caption="Morada Entrega.Número Da Porta" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Número Da Porta].[All]" allUniqueName="[Morada Entrega].[Número Da Porta].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Rua]" caption="Morada Entrega.Rua" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Rua].[All]" allUniqueName="[Morada Entrega].[Rua].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Concelho]" caption="Morada Facturacao.Concelho" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Concelho].[All]" allUniqueName="[Morada Facturacao].[Concelho].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Distrito]" caption="Morada Facturacao.Distrito" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Distrito].[All]" allUniqueName="[Morada Facturacao].[Distrito].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Freguesia]" caption="Morada Facturacao.Freguesia" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Freguesia].[All]" allUniqueName="[Morada Facturacao].[Freguesia].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Keycol]" caption="Morada Facturacao.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Morada Facturacao].[Keycol].[All]" allUniqueName="[Morada Facturacao].[Keycol].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Número Da Porta]" caption="Morada Facturacao.Número Da Porta" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Número Da Porta].[All]" allUniqueName="[Morada Facturacao].[Número Da Porta].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Rua]" caption="Morada Facturacao.Rua" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Rua].[All]" allUniqueName="[Morada Facturacao].[Rua].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Tipo Servico].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Tipo Servico].[Keycol].[All]" allUniqueName="[Tipo Servico].[Keycol].[All]" dimensionUniqueName="[Tipo Servico]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Número De Entregas]" caption="Número De Entregas" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Valor]" caption="Valor" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Dentro Do SLA]" caption="Dentro Do SLA" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Concluido]" caption="Concluido" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Contagem de Servicos]" caption="Contagem de Servicos" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Número Entregas por Serviço]" caption="Número Entregas por Serviço" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Valor do Serviço]" caption="Valor do Serviço" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Serviço Dentro Do SLA]" caption="Serviço Dentro Do SLA" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Serviço Concluido]" caption="Serviço Concluido" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Sucesso]" caption="Sucesso" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Contagem de Entregas]" caption="Contagem de Entregas" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="Dummy0" caption="Activo" measure="1" count="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{8CF416AD-EC4C-4aba-99F5-12A058AE0983}">
-          <x14:cacheHierarchy ignore="1"/>
-        </ext>
-      </extLst>
-    </cacheHierarchy>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <dimensions count="17">
-    <dimension name="Cliente" uniqueName="[Cliente]" caption="Cliente"/>
-    <dimension name="Data Conclusao" uniqueName="[Data Conclusao]" caption="Data Conclusao"/>
-    <dimension name="Data Requisicao" uniqueName="[Data Requisicao]" caption="Data Requisicao"/>
-    <dimension name="Data Tentativa" uniqueName="[Data Tentativa]" caption="Data Tentativa"/>
-    <dimension name="Funcionário" uniqueName="[Funcionário]" caption="Funcionário"/>
-    <dimension name="Hora Conclusao" uniqueName="[Hora Conclusao]" caption="Hora Conclusao"/>
-    <dimension name="Hora Entrega" uniqueName="[Hora Entrega]" caption="Hora Entrega"/>
-    <dimension name="Hora Requisicao" uniqueName="[Hora Requisicao]" caption="Hora Requisicao"/>
-    <dimension name="Hora Tentativa" uniqueName="[Hora Tentativa]" caption="Hora Tentativa"/>
-    <dimension name="Intervalo Idade Cliente" uniqueName="[Intervalo Idade Cliente]" caption="Intervalo Idade Cliente"/>
-    <dimension name="Intervalo Idade Na Requisição" uniqueName="[Intervalo Idade Na Requisição]" caption="Intervalo Idade Na Requisição"/>
-    <dimension name="Intervalo Rendimento Cliente" uniqueName="[Intervalo Rendimento Cliente]" caption="Intervalo Rendimento Cliente"/>
-    <dimension name="Intervalo Rendimento Na Requisição" uniqueName="[Intervalo Rendimento Na Requisição]" caption="Intervalo Rendimento Na Requisição"/>
-    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
-    <dimension name="Morada Entrega" uniqueName="[Morada Entrega]" caption="Morada Entrega"/>
-    <dimension name="Morada Facturacao" uniqueName="[Morada Facturacao]" caption="Morada Facturacao"/>
-    <dimension name="Tipo Servico" uniqueName="[Tipo Servico]" caption="Tipo Servico"/>
-  </dimensions>
-  <measureGroups count="2">
-    <measureGroup name="Entregas Dos Servicos" caption="Entregas Dos Servicos"/>
-    <measureGroup name="Servicos" caption="Servicos"/>
-  </measureGroups>
-  <maps count="25">
-    <map measureGroup="0" dimension="0"/>
-    <map measureGroup="0" dimension="1"/>
-    <map measureGroup="0" dimension="2"/>
-    <map measureGroup="0" dimension="3"/>
-    <map measureGroup="0" dimension="4"/>
-    <map measureGroup="0" dimension="5"/>
-    <map measureGroup="0" dimension="6"/>
-    <map measureGroup="0" dimension="7"/>
-    <map measureGroup="0" dimension="8"/>
-    <map measureGroup="0" dimension="9"/>
-    <map measureGroup="0" dimension="11"/>
-    <map measureGroup="0" dimension="14"/>
-    <map measureGroup="0" dimension="15"/>
-    <map measureGroup="0" dimension="16"/>
-    <map measureGroup="1" dimension="0"/>
-    <map measureGroup="1" dimension="1"/>
-    <map measureGroup="1" dimension="2"/>
-    <map measureGroup="1" dimension="5"/>
-    <map measureGroup="1" dimension="6"/>
-    <map measureGroup="1" dimension="7"/>
-    <map measureGroup="1" dimension="10"/>
-    <map measureGroup="1" dimension="12"/>
-    <map measureGroup="1" dimension="14"/>
-    <map measureGroup="1" dimension="15"/>
-    <map measureGroup="1" dimension="16"/>
-  </maps>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Rui Miranda" refreshedDate="41444.126004166668" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
-  <cacheSource type="external" connectionId="4"/>
-  <cacheFields count="9">
-    <cacheField name="[Measures].[Contagem de Entregas]" caption="Contagem de Entregas" numFmtId="0" hierarchy="129" level="32767"/>
-    <cacheField name="[Hora Tentativa].[Hora 24h].[Hora 24h]" caption="Hora 24h" numFmtId="0" hierarchy="49" level="1">
-      <sharedItems count="16">
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[00:00]" c="00:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[09:00]" c="09:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[10:00]" c="10:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[11:00]" c="11:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[12:00]" c="12:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[13:00]" c="13:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[14:00]" c="14:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[15:00]" c="15:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[16:00]" c="16:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[17:00]" c="17:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[18:00]" c="18:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[19:00]" c="19:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[20:00]" c="20:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[21:00]" c="21:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[22:00]" c="22:00"/>
-        <s v="[Hora Tentativa].[Hora 24h].&amp;[23:00]" c="23:00"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Ano]" caption="Ano" numFmtId="0" hierarchy="29" level="1">
-      <sharedItems count="4">
-        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2010]" c="2010"/>
-        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2011]" c="2011"/>
-        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2012]" c="2012"/>
-        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2013]" c="2013"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Trimestre]" caption="Trimestre" numFmtId="0" hierarchy="29" level="2" mappingCount="1">
-      <sharedItems count="2">
-        <s v="[Data Tentativa].[Ano - Dia].[Trimestre].&amp;[2013]&amp;[1]" c="1" cp="1">
-          <x/>
-        </s>
-        <s v="[Data Tentativa].[Ano - Dia].[Trimestre].&amp;[2013]&amp;[2]" c="2" cp="1">
-          <x/>
-        </s>
-      </sharedItems>
-      <mpMap v="6"/>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Mês Número]" caption="Mês Número" numFmtId="0" hierarchy="29" level="3" mappingCount="1">
-      <sharedItems count="3">
-        <s v="[Data Tentativa].[Ano - Dia].[Mês Número].&amp;[2013]&amp;[2]&amp;[4]" c="4" cp="1">
-          <x/>
-        </s>
-        <s v="[Data Tentativa].[Ano - Dia].[Mês Número].&amp;[2013]&amp;[2]&amp;[5]" c="5" cp="1">
-          <x/>
-        </s>
-        <s v="[Data Tentativa].[Ano - Dia].[Mês Número].&amp;[2013]&amp;[2]&amp;[6]" c="6" cp="1">
-          <x/>
-        </s>
-      </sharedItems>
-      <mpMap v="7"/>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Dia]" caption="Dia" numFmtId="0" hierarchy="29" level="4">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Trimestre].[Ano]" caption="Ano" propertyName="Ano" numFmtId="0" hierarchy="29" level="2" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2013" maxValue="2013" count="1">
-        <n v="2013"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Mês Número].[Trimestre]" caption="Trimestre" propertyName="Trimestre" numFmtId="0" hierarchy="29" level="3" memberPropertyField="1">
-      <sharedItems count="1">
-        <s v="2"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Data Tentativa].[Ano - Dia].[Dia].[Mês Número]" caption="Mês Número" propertyName="Mês Número" numFmtId="0" hierarchy="29" level="4" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-  </cacheFields>
-  <cacheHierarchies count="130">
-    <cacheHierarchy uniqueName="[Cliente].[Activo]" caption="Activo" attribute="1" defaultMemberUniqueName="[Cliente].[Activo].[All]" allUniqueName="[Cliente].[Activo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Codigo Postal]" caption="Codigo Postal" attribute="1" defaultMemberUniqueName="[Cliente].[Codigo Postal].[All]" allUniqueName="[Cliente].[Codigo Postal].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Educação]" caption="Educação" attribute="1" defaultMemberUniqueName="[Cliente].[Educação].[All]" allUniqueName="[Cliente].[Educação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Estado Civil]" caption="Estado Civil" attribute="1" defaultMemberUniqueName="[Cliente].[Estado Civil].[All]" allUniqueName="[Cliente].[Estado Civil].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Género]" caption="Género" attribute="1" defaultMemberUniqueName="[Cliente].[Género].[All]" allUniqueName="[Cliente].[Género].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Idade]" caption="Intervalo Idade" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Idade].[All]" allUniqueName="[Cliente].[Intervalo Idade].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Idade Nome]" caption="Intervalo Idade Nome" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Idade Nome].[All]" allUniqueName="[Cliente].[Intervalo Idade Nome].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento]" caption="Intervalo Rendimento" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento].[All]" allUniqueName="[Cliente].[Intervalo Rendimento].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento Classe]" caption="Intervalo Rendimento Classe" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento Classe].[All]" allUniqueName="[Cliente].[Intervalo Rendimento Classe].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento Codigo]" caption="Intervalo Rendimento Codigo" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento Codigo].[All]" allUniqueName="[Cliente].[Intervalo Rendimento Codigo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Nome De Contacto]" caption="Nome De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Nome De Contacto].[All]" allUniqueName="[Cliente].[Nome De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Número De Carros Possuidos]" caption="Número De Carros Possuidos" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Carros Possuidos].[All]" allUniqueName="[Cliente].[Número De Carros Possuidos].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Número De Filhos]" caption="Número De Filhos" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Filhos].[All]" allUniqueName="[Cliente].[Número De Filhos].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Número De Filhos Em Casa]" caption="Número De Filhos Em Casa" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Filhos Em Casa].[All]" allUniqueName="[Cliente].[Número De Filhos Em Casa].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Ocupação]" caption="Ocupação" attribute="1" defaultMemberUniqueName="[Cliente].[Ocupação].[All]" allUniqueName="[Cliente].[Ocupação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Por Designação]" caption="Por Designação" defaultMemberUniqueName="[Cliente].[Por Designação].[All]" allUniqueName="[Cliente].[Por Designação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Possui Casa]" caption="Possui Casa" attribute="1" defaultMemberUniqueName="[Cliente].[Possui Casa].[All]" allUniqueName="[Cliente].[Possui Casa].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Singular]" caption="Singular" attribute="1" defaultMemberUniqueName="[Cliente].[Singular].[All]" allUniqueName="[Cliente].[Singular].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Sobrenome De Contacto]" caption="Sobrenome De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Sobrenome De Contacto].[All]" allUniqueName="[Cliente].[Sobrenome De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Ano - Dia]" caption="Data Conclusao.Ano - Dia" time="1" defaultMemberUniqueName="[Data Conclusao].[Ano - Dia].[All]" allUniqueName="[Data Conclusao].[Ano - Dia].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Data]" caption="Data Conclusao.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Data].[All]" allUniqueName="[Data Conclusao].[Data].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Dia Da Semana Nome]" caption="Data Conclusao.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia Da Semana Nome].[All]" allUniqueName="[Data Conclusao].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Dia Da Semana Número]" caption="Data Conclusao.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia Da Semana Número].[All]" allUniqueName="[Data Conclusao].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Mês Nome]" caption="Data Conclusao.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Mês Nome].[All]" allUniqueName="[Data Conclusao].[Mês Nome].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Ano - Dia]" caption="Data Requisicao.Ano - Dia" time="1" defaultMemberUniqueName="[Data Requisicao].[Ano - Dia].[All]" allUniqueName="[Data Requisicao].[Ano - Dia].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Data]" caption="Data Requisicao.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Data].[All]" allUniqueName="[Data Requisicao].[Data].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Dia Da Semana Nome]" caption="Data Requisicao.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia Da Semana Nome].[All]" allUniqueName="[Data Requisicao].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Dia Da Semana Número]" caption="Data Requisicao.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia Da Semana Número].[All]" allUniqueName="[Data Requisicao].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Mês Nome]" caption="Data Requisicao.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Mês Nome].[All]" allUniqueName="[Data Requisicao].[Mês Nome].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Ano - Dia]" caption="Data Tentativa.Ano - Dia" time="1" defaultMemberUniqueName="[Data Tentativa].[Ano - Dia].[All]" allUniqueName="[Data Tentativa].[Ano - Dia].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="5" unbalanced="0">
-      <fieldsUsage count="5">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="2"/>
-        <fieldUsage x="3"/>
-        <fieldUsage x="4"/>
-        <fieldUsage x="5"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Data]" caption="Data Tentativa.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Data].[All]" allUniqueName="[Data Tentativa].[Data].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Dia Da Semana Nome]" caption="Data Tentativa.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia Da Semana Nome].[All]" allUniqueName="[Data Tentativa].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Dia Da Semana Número]" caption="Data Tentativa.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia Da Semana Número].[All]" allUniqueName="[Data Tentativa].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Mês Nome]" caption="Data Tentativa.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Mês Nome].[All]" allUniqueName="[Data Tentativa].[Mês Nome].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Activo]" caption="Activo" attribute="1" defaultMemberUniqueName="[Funcionário].[Activo].[All]" allUniqueName="[Funcionário].[Activo].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Localização - Loja]" caption="Localização - Loja" defaultMemberUniqueName="[Funcionário].[Localização - Loja].[All]" allUniqueName="[Funcionário].[Localização - Loja].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Nome]" caption="Nome" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome].[All]" allUniqueName="[Funcionário].[Nome].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Nome Do Chefe]" caption="Nome Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Do Chefe].[All]" allUniqueName="[Funcionário].[Nome Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Por Função Do Chefe]" caption="Por Função Do Chefe" defaultMemberUniqueName="[Funcionário].[Por Função Do Chefe].[All]" allUniqueName="[Funcionário].[Por Função Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Por Nome Completo Do Chefe]" caption="Por Nome Completo Do Chefe" defaultMemberUniqueName="[Funcionário].[Por Nome Completo Do Chefe].[All]" allUniqueName="[Funcionário].[Por Nome Completo Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Sobrenome]" caption="Sobrenome" attribute="1" defaultMemberUniqueName="[Funcionário].[Sobrenome].[All]" allUniqueName="[Funcionário].[Sobrenome].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Sobrenome Do Chefe]" caption="Sobrenome Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Sobrenome Do Chefe].[All]" allUniqueName="[Funcionário].[Sobrenome Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Conclusao].[Hora 12h]" caption="Hora Conclusao.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Conclusao].[Hora 12h].[All]" allUniqueName="[Hora Conclusao].[Hora 12h].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Conclusao].[Hora 24h]" caption="Hora Conclusao.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Conclusao].[Hora 24h].[All]" allUniqueName="[Hora Conclusao].[Hora 24h].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Entrega].[Hora 12h]" caption="Hora Entrega.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Entrega].[Hora 12h].[All]" allUniqueName="[Hora Entrega].[Hora 12h].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Entrega].[Hora 24h]" caption="Hora Entrega.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Entrega].[Hora 24h].[All]" allUniqueName="[Hora Entrega].[Hora 24h].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Requisicao].[Hora 12h]" caption="Hora Requisicao.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Requisicao].[Hora 12h].[All]" allUniqueName="[Hora Requisicao].[Hora 12h].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Requisicao].[Hora 24h]" caption="Hora Requisicao.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Requisicao].[Hora 24h].[All]" allUniqueName="[Hora Requisicao].[Hora 24h].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Tentativa].[Hora 12h]" caption="Hora Tentativa.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Tentativa].[Hora 12h].[All]" allUniqueName="[Hora Tentativa].[Hora 12h].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Hora Tentativa].[Hora 24h]" caption="Hora Tentativa.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Tentativa].[Hora 24h].[All]" allUniqueName="[Hora Tentativa].[Hora 24h].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Intervalo]" caption="Intervalo Idade Cliente.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Intervalo].[All]" allUniqueName="[Intervalo Idade Cliente].[Intervalo].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Nome]" caption="Intervalo Idade Cliente.Nome" attribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Nome].[All]" allUniqueName="[Intervalo Idade Cliente].[Nome].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Intervalo]" caption="Intervalo Idade Na Requisição.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Intervalo].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Intervalo].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Nome]" caption="Intervalo Idade Na Requisição.Nome" attribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Nome].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Nome].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Classe]" caption="Intervalo Rendimento Cliente.Classe" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Classe].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Classe].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Codigo]" caption="Intervalo Rendimento Cliente.Codigo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Codigo].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Codigo].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Intervalo]" caption="Intervalo Rendimento Cliente.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Intervalo].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Intervalo].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Classe]" caption="Intervalo Rendimento Na Requisição.Classe" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Classe].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Classe].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Codigo]" caption="Intervalo Rendimento Na Requisição.Codigo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Codigo].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Codigo].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Intervalo]" caption="Intervalo Rendimento Na Requisição.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Intervalo].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Intervalo].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Código Postal]" caption="Morada Entrega.Código Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Código Postal].[All]" allUniqueName="[Morada Entrega].[Código Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Código Postal Completo]" caption="Morada Entrega.Código Postal Completo" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Código Postal Completo].[All]" allUniqueName="[Morada Entrega].[Código Postal Completo].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Designação Postal]" caption="Morada Entrega.Designação Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Designação Postal].[All]" allUniqueName="[Morada Entrega].[Designação Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Distrito - Número Da Porta]" caption="Morada Entrega.Distrito - Número Da Porta" defaultMemberUniqueName="[Morada Entrega].[Distrito - Número Da Porta].[All]" allUniqueName="[Morada Entrega].[Distrito - Número Da Porta].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Extensão Código Postal]" caption="Morada Entrega.Extensão Código Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Extensão Código Postal].[All]" allUniqueName="[Morada Entrega].[Extensão Código Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Localidade]" caption="Morada Entrega.Localidade" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Localidade].[All]" allUniqueName="[Morada Entrega].[Localidade].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Código Postal]" caption="Morada Facturacao.Código Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Código Postal].[All]" allUniqueName="[Morada Facturacao].[Código Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Código Postal Completo]" caption="Morada Facturacao.Código Postal Completo" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Código Postal Completo].[All]" allUniqueName="[Morada Facturacao].[Código Postal Completo].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Designação Postal]" caption="Morada Facturacao.Designação Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Designação Postal].[All]" allUniqueName="[Morada Facturacao].[Designação Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Distrito - Número Da Porta]" caption="Morada Facturacao.Distrito - Número Da Porta" defaultMemberUniqueName="[Morada Facturacao].[Distrito - Número Da Porta].[All]" allUniqueName="[Morada Facturacao].[Distrito - Número Da Porta].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Extensão Código Postal]" caption="Morada Facturacao.Extensão Código Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Extensão Código Postal].[All]" allUniqueName="[Morada Facturacao].[Extensão Código Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Localidade]" caption="Morada Facturacao.Localidade" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Localidade].[All]" allUniqueName="[Morada Facturacao].[Localidade].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Tipo Servico].[Tipo]" caption="Tipo" attribute="1" defaultMemberUniqueName="[Tipo Servico].[Tipo].[All]" allUniqueName="[Tipo Servico].[Tipo].[All]" dimensionUniqueName="[Tipo Servico]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente].[Designação]" caption="Designação" attribute="1" defaultMemberUniqueName="[Cliente].[Designação].[All]" allUniqueName="[Cliente].[Designação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente].[Keycol].[All]" allUniqueName="[Cliente].[Keycol].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Nome Completo De Contacto]" caption="Nome Completo De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Nome Completo De Contacto].[All]" allUniqueName="[Cliente].[Nome Completo De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Ano]" caption="Data Conclusao.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Ano].[All]" allUniqueName="[Data Conclusao].[Ano].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Dia]" caption="Data Conclusao.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia].[All]" allUniqueName="[Data Conclusao].[Dia].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Keycol]" caption="Data Conclusao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Conclusao].[Keycol].[All]" allUniqueName="[Data Conclusao].[Keycol].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Mês Número]" caption="Data Conclusao.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Mês Número].[All]" allUniqueName="[Data Conclusao].[Mês Número].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Conclusao].[Trimestre]" caption="Data Conclusao.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Trimestre].[All]" allUniqueName="[Data Conclusao].[Trimestre].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Ano]" caption="Data Requisicao.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Ano].[All]" allUniqueName="[Data Requisicao].[Ano].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Dia]" caption="Data Requisicao.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia].[All]" allUniqueName="[Data Requisicao].[Dia].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Keycol]" caption="Data Requisicao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Requisicao].[Keycol].[All]" allUniqueName="[Data Requisicao].[Keycol].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Mês Número]" caption="Data Requisicao.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Mês Número].[All]" allUniqueName="[Data Requisicao].[Mês Número].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Requisicao].[Trimestre]" caption="Data Requisicao.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Trimestre].[All]" allUniqueName="[Data Requisicao].[Trimestre].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Ano]" caption="Data Tentativa.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Ano].[All]" allUniqueName="[Data Tentativa].[Ano].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Dia]" caption="Data Tentativa.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia].[All]" allUniqueName="[Data Tentativa].[Dia].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Keycol]" caption="Data Tentativa.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Tentativa].[Keycol].[All]" allUniqueName="[Data Tentativa].[Keycol].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Mês Número]" caption="Data Tentativa.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Mês Número].[All]" allUniqueName="[Data Tentativa].[Mês Número].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Data Tentativa].[Trimestre]" caption="Data Tentativa.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Trimestre].[All]" allUniqueName="[Data Tentativa].[Trimestre].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Função]" caption="Função" attribute="1" defaultMemberUniqueName="[Funcionário].[Função].[All]" allUniqueName="[Funcionário].[Função].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Função Do Chefe]" caption="Função Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Função Do Chefe].[All]" allUniqueName="[Funcionário].[Função Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Funcionário].[Keycol].[All]" allUniqueName="[Funcionário].[Keycol].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Localização]" caption="Localização" attribute="1" defaultMemberUniqueName="[Funcionário].[Localização].[All]" allUniqueName="[Funcionário].[Localização].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Loja]" caption="Loja" attribute="1" defaultMemberUniqueName="[Funcionário].[Loja].[All]" allUniqueName="[Funcionário].[Loja].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Nome Completo]" caption="Nome Completo" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Completo].[All]" allUniqueName="[Funcionário].[Nome Completo].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Funcionário].[Nome Completo Do Chefe]" caption="Nome Completo Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Completo Do Chefe].[All]" allUniqueName="[Funcionário].[Nome Completo Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Hora Conclusao].[Keycol]" caption="Hora Conclusao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Conclusao].[Keycol].[All]" allUniqueName="[Hora Conclusao].[Keycol].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Hora Entrega].[Keycol]" caption="Hora Entrega.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Entrega].[Keycol].[All]" allUniqueName="[Hora Entrega].[Keycol].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Hora Requisicao].[Keycol]" caption="Hora Requisicao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Requisicao].[Keycol].[All]" allUniqueName="[Hora Requisicao].[Keycol].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Hora Tentativa].[Keycol]" caption="Hora Tentativa.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Tentativa].[Keycol].[All]" allUniqueName="[Hora Tentativa].[Keycol].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Keycol]" caption="Intervalo Idade Cliente.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Keycol].[All]" allUniqueName="[Intervalo Idade Cliente].[Keycol].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Keycol]" caption="Intervalo Idade Na Requisição.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Keycol].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Keycol].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Keycol]" caption="Intervalo Rendimento Cliente.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Keycol].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Keycol].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Keycol]" caption="Intervalo Rendimento Na Requisição.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Keycol].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Keycol].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Concelho]" caption="Morada Entrega.Concelho" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Concelho].[All]" allUniqueName="[Morada Entrega].[Concelho].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Distrito]" caption="Morada Entrega.Distrito" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Distrito].[All]" allUniqueName="[Morada Entrega].[Distrito].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Freguesia]" caption="Morada Entrega.Freguesia" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Freguesia].[All]" allUniqueName="[Morada Entrega].[Freguesia].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Keycol]" caption="Morada Entrega.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Morada Entrega].[Keycol].[All]" allUniqueName="[Morada Entrega].[Keycol].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Número Da Porta]" caption="Morada Entrega.Número Da Porta" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Número Da Porta].[All]" allUniqueName="[Morada Entrega].[Número Da Porta].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Entrega].[Rua]" caption="Morada Entrega.Rua" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Rua].[All]" allUniqueName="[Morada Entrega].[Rua].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Concelho]" caption="Morada Facturacao.Concelho" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Concelho].[All]" allUniqueName="[Morada Facturacao].[Concelho].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Distrito]" caption="Morada Facturacao.Distrito" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Distrito].[All]" allUniqueName="[Morada Facturacao].[Distrito].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Freguesia]" caption="Morada Facturacao.Freguesia" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Freguesia].[All]" allUniqueName="[Morada Facturacao].[Freguesia].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Keycol]" caption="Morada Facturacao.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Morada Facturacao].[Keycol].[All]" allUniqueName="[Morada Facturacao].[Keycol].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Número Da Porta]" caption="Morada Facturacao.Número Da Porta" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Número Da Porta].[All]" allUniqueName="[Morada Facturacao].[Número Da Porta].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Morada Facturacao].[Rua]" caption="Morada Facturacao.Rua" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Rua].[All]" allUniqueName="[Morada Facturacao].[Rua].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Tipo Servico].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Tipo Servico].[Keycol].[All]" allUniqueName="[Tipo Servico].[Keycol].[All]" dimensionUniqueName="[Tipo Servico]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Número De Entregas]" caption="Número De Entregas" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Valor]" caption="Valor" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Dentro Do SLA]" caption="Dentro Do SLA" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Concluido]" caption="Concluido" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Contagem de Servicos]" caption="Contagem de Servicos" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Número Entregas por Serviço]" caption="Número Entregas por Serviço" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Valor do Serviço]" caption="Valor do Serviço" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Serviço Dentro Do SLA]" caption="Serviço Dentro Do SLA" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Serviço Concluido]" caption="Serviço Concluido" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Sucesso]" caption="Sucesso" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Contagem de Entregas]" caption="Contagem de Entregas" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <dimensions count="17">
-    <dimension name="Cliente" uniqueName="[Cliente]" caption="Cliente"/>
-    <dimension name="Data Conclusao" uniqueName="[Data Conclusao]" caption="Data Conclusao"/>
-    <dimension name="Data Requisicao" uniqueName="[Data Requisicao]" caption="Data Requisicao"/>
-    <dimension name="Data Tentativa" uniqueName="[Data Tentativa]" caption="Data Tentativa"/>
-    <dimension name="Funcionário" uniqueName="[Funcionário]" caption="Funcionário"/>
-    <dimension name="Hora Conclusao" uniqueName="[Hora Conclusao]" caption="Hora Conclusao"/>
-    <dimension name="Hora Entrega" uniqueName="[Hora Entrega]" caption="Hora Entrega"/>
-    <dimension name="Hora Requisicao" uniqueName="[Hora Requisicao]" caption="Hora Requisicao"/>
-    <dimension name="Hora Tentativa" uniqueName="[Hora Tentativa]" caption="Hora Tentativa"/>
-    <dimension name="Intervalo Idade Cliente" uniqueName="[Intervalo Idade Cliente]" caption="Intervalo Idade Cliente"/>
-    <dimension name="Intervalo Idade Na Requisição" uniqueName="[Intervalo Idade Na Requisição]" caption="Intervalo Idade Na Requisição"/>
-    <dimension name="Intervalo Rendimento Cliente" uniqueName="[Intervalo Rendimento Cliente]" caption="Intervalo Rendimento Cliente"/>
-    <dimension name="Intervalo Rendimento Na Requisição" uniqueName="[Intervalo Rendimento Na Requisição]" caption="Intervalo Rendimento Na Requisição"/>
-    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
-    <dimension name="Morada Entrega" uniqueName="[Morada Entrega]" caption="Morada Entrega"/>
-    <dimension name="Morada Facturacao" uniqueName="[Morada Facturacao]" caption="Morada Facturacao"/>
-    <dimension name="Tipo Servico" uniqueName="[Tipo Servico]" caption="Tipo Servico"/>
-  </dimensions>
-  <measureGroups count="2">
-    <measureGroup name="Entregas Dos Servicos" caption="Entregas Dos Servicos"/>
-    <measureGroup name="Servicos" caption="Servicos"/>
-  </measureGroups>
-  <maps count="25">
-    <map measureGroup="0" dimension="0"/>
-    <map measureGroup="0" dimension="1"/>
-    <map measureGroup="0" dimension="2"/>
-    <map measureGroup="0" dimension="3"/>
-    <map measureGroup="0" dimension="4"/>
-    <map measureGroup="0" dimension="5"/>
-    <map measureGroup="0" dimension="6"/>
-    <map measureGroup="0" dimension="7"/>
-    <map measureGroup="0" dimension="8"/>
-    <map measureGroup="0" dimension="9"/>
-    <map measureGroup="0" dimension="11"/>
-    <map measureGroup="0" dimension="14"/>
-    <map measureGroup="0" dimension="15"/>
-    <map measureGroup="0" dimension="16"/>
-    <map measureGroup="1" dimension="0"/>
-    <map measureGroup="1" dimension="1"/>
-    <map measureGroup="1" dimension="2"/>
-    <map measureGroup="1" dimension="5"/>
-    <map measureGroup="1" dimension="6"/>
-    <map measureGroup="1" dimension="7"/>
-    <map measureGroup="1" dimension="10"/>
-    <map measureGroup="1" dimension="12"/>
-    <map measureGroup="1" dimension="14"/>
-    <map measureGroup="1" dimension="15"/>
-    <map measureGroup="1" dimension="16"/>
-  </maps>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Rui Miranda" refreshedDate="41444.12602476852" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Rui Miranda" refreshedDate="41444.925375810184" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="7"/>
   <cacheFields count="19">
     <cacheField name="[Measures].[Valor]" caption="Valor" numFmtId="0" hierarchy="120" level="32767"/>
@@ -4966,8 +3568,1406 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Rui Miranda" refreshedDate="41444.925394791666" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+  <cacheSource type="external" connectionId="4"/>
+  <cacheFields count="9">
+    <cacheField name="[Measures].[Contagem de Entregas]" caption="Contagem de Entregas" numFmtId="0" hierarchy="129" level="32767"/>
+    <cacheField name="[Hora Tentativa].[Hora 24h].[Hora 24h]" caption="Hora 24h" numFmtId="0" hierarchy="49" level="1">
+      <sharedItems count="16">
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[00:00]" c="00:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[09:00]" c="09:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[10:00]" c="10:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[11:00]" c="11:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[12:00]" c="12:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[13:00]" c="13:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[14:00]" c="14:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[15:00]" c="15:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[16:00]" c="16:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[17:00]" c="17:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[18:00]" c="18:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[19:00]" c="19:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[20:00]" c="20:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[21:00]" c="21:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[22:00]" c="22:00"/>
+        <s v="[Hora Tentativa].[Hora 24h].&amp;[23:00]" c="23:00"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Ano]" caption="Ano" numFmtId="0" hierarchy="29" level="1">
+      <sharedItems count="4">
+        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2010]" c="2010"/>
+        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2011]" c="2011"/>
+        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2012]" c="2012"/>
+        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2013]" c="2013"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Trimestre]" caption="Trimestre" numFmtId="0" hierarchy="29" level="2" mappingCount="1">
+      <sharedItems count="2">
+        <s v="[Data Tentativa].[Ano - Dia].[Trimestre].&amp;[2013]&amp;[1]" c="1" cp="1">
+          <x/>
+        </s>
+        <s v="[Data Tentativa].[Ano - Dia].[Trimestre].&amp;[2013]&amp;[2]" c="2" cp="1">
+          <x/>
+        </s>
+      </sharedItems>
+      <mpMap v="6"/>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Mês Número]" caption="Mês Número" numFmtId="0" hierarchy="29" level="3" mappingCount="1">
+      <sharedItems count="3">
+        <s v="[Data Tentativa].[Ano - Dia].[Mês Número].&amp;[2013]&amp;[2]&amp;[4]" c="4" cp="1">
+          <x/>
+        </s>
+        <s v="[Data Tentativa].[Ano - Dia].[Mês Número].&amp;[2013]&amp;[2]&amp;[5]" c="5" cp="1">
+          <x/>
+        </s>
+        <s v="[Data Tentativa].[Ano - Dia].[Mês Número].&amp;[2013]&amp;[2]&amp;[6]" c="6" cp="1">
+          <x/>
+        </s>
+      </sharedItems>
+      <mpMap v="7"/>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Dia]" caption="Dia" numFmtId="0" hierarchy="29" level="4">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Trimestre].[Ano]" caption="Ano" propertyName="Ano" numFmtId="0" hierarchy="29" level="2" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2013" maxValue="2013" count="1">
+        <n v="2013"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Mês Número].[Trimestre]" caption="Trimestre" propertyName="Trimestre" numFmtId="0" hierarchy="29" level="3" memberPropertyField="1">
+      <sharedItems count="1">
+        <s v="2"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Dia].[Mês Número]" caption="Mês Número" propertyName="Mês Número" numFmtId="0" hierarchy="29" level="4" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="130">
+    <cacheHierarchy uniqueName="[Cliente].[Activo]" caption="Activo" attribute="1" defaultMemberUniqueName="[Cliente].[Activo].[All]" allUniqueName="[Cliente].[Activo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Codigo Postal]" caption="Codigo Postal" attribute="1" defaultMemberUniqueName="[Cliente].[Codigo Postal].[All]" allUniqueName="[Cliente].[Codigo Postal].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Educação]" caption="Educação" attribute="1" defaultMemberUniqueName="[Cliente].[Educação].[All]" allUniqueName="[Cliente].[Educação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Estado Civil]" caption="Estado Civil" attribute="1" defaultMemberUniqueName="[Cliente].[Estado Civil].[All]" allUniqueName="[Cliente].[Estado Civil].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Género]" caption="Género" attribute="1" defaultMemberUniqueName="[Cliente].[Género].[All]" allUniqueName="[Cliente].[Género].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Idade]" caption="Intervalo Idade" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Idade].[All]" allUniqueName="[Cliente].[Intervalo Idade].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Idade Nome]" caption="Intervalo Idade Nome" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Idade Nome].[All]" allUniqueName="[Cliente].[Intervalo Idade Nome].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento]" caption="Intervalo Rendimento" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento].[All]" allUniqueName="[Cliente].[Intervalo Rendimento].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento Classe]" caption="Intervalo Rendimento Classe" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento Classe].[All]" allUniqueName="[Cliente].[Intervalo Rendimento Classe].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento Codigo]" caption="Intervalo Rendimento Codigo" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento Codigo].[All]" allUniqueName="[Cliente].[Intervalo Rendimento Codigo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Nome De Contacto]" caption="Nome De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Nome De Contacto].[All]" allUniqueName="[Cliente].[Nome De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Número De Carros Possuidos]" caption="Número De Carros Possuidos" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Carros Possuidos].[All]" allUniqueName="[Cliente].[Número De Carros Possuidos].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Número De Filhos]" caption="Número De Filhos" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Filhos].[All]" allUniqueName="[Cliente].[Número De Filhos].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Número De Filhos Em Casa]" caption="Número De Filhos Em Casa" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Filhos Em Casa].[All]" allUniqueName="[Cliente].[Número De Filhos Em Casa].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Ocupação]" caption="Ocupação" attribute="1" defaultMemberUniqueName="[Cliente].[Ocupação].[All]" allUniqueName="[Cliente].[Ocupação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Por Designação]" caption="Por Designação" defaultMemberUniqueName="[Cliente].[Por Designação].[All]" allUniqueName="[Cliente].[Por Designação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Possui Casa]" caption="Possui Casa" attribute="1" defaultMemberUniqueName="[Cliente].[Possui Casa].[All]" allUniqueName="[Cliente].[Possui Casa].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Singular]" caption="Singular" attribute="1" defaultMemberUniqueName="[Cliente].[Singular].[All]" allUniqueName="[Cliente].[Singular].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Sobrenome De Contacto]" caption="Sobrenome De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Sobrenome De Contacto].[All]" allUniqueName="[Cliente].[Sobrenome De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Ano - Dia]" caption="Data Conclusao.Ano - Dia" time="1" defaultMemberUniqueName="[Data Conclusao].[Ano - Dia].[All]" allUniqueName="[Data Conclusao].[Ano - Dia].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Data]" caption="Data Conclusao.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Data].[All]" allUniqueName="[Data Conclusao].[Data].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Dia Da Semana Nome]" caption="Data Conclusao.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia Da Semana Nome].[All]" allUniqueName="[Data Conclusao].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Dia Da Semana Número]" caption="Data Conclusao.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia Da Semana Número].[All]" allUniqueName="[Data Conclusao].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Mês Nome]" caption="Data Conclusao.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Mês Nome].[All]" allUniqueName="[Data Conclusao].[Mês Nome].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Ano - Dia]" caption="Data Requisicao.Ano - Dia" time="1" defaultMemberUniqueName="[Data Requisicao].[Ano - Dia].[All]" allUniqueName="[Data Requisicao].[Ano - Dia].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Data]" caption="Data Requisicao.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Data].[All]" allUniqueName="[Data Requisicao].[Data].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Dia Da Semana Nome]" caption="Data Requisicao.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia Da Semana Nome].[All]" allUniqueName="[Data Requisicao].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Dia Da Semana Número]" caption="Data Requisicao.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia Da Semana Número].[All]" allUniqueName="[Data Requisicao].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Mês Nome]" caption="Data Requisicao.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Mês Nome].[All]" allUniqueName="[Data Requisicao].[Mês Nome].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Ano - Dia]" caption="Data Tentativa.Ano - Dia" time="1" defaultMemberUniqueName="[Data Tentativa].[Ano - Dia].[All]" allUniqueName="[Data Tentativa].[Ano - Dia].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="5" unbalanced="0">
+      <fieldsUsage count="5">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+        <fieldUsage x="3"/>
+        <fieldUsage x="4"/>
+        <fieldUsage x="5"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Data]" caption="Data Tentativa.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Data].[All]" allUniqueName="[Data Tentativa].[Data].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Dia Da Semana Nome]" caption="Data Tentativa.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia Da Semana Nome].[All]" allUniqueName="[Data Tentativa].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Dia Da Semana Número]" caption="Data Tentativa.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia Da Semana Número].[All]" allUniqueName="[Data Tentativa].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Mês Nome]" caption="Data Tentativa.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Mês Nome].[All]" allUniqueName="[Data Tentativa].[Mês Nome].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Activo]" caption="Activo" attribute="1" defaultMemberUniqueName="[Funcionário].[Activo].[All]" allUniqueName="[Funcionário].[Activo].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Localização - Loja]" caption="Localização - Loja" defaultMemberUniqueName="[Funcionário].[Localização - Loja].[All]" allUniqueName="[Funcionário].[Localização - Loja].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Nome]" caption="Nome" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome].[All]" allUniqueName="[Funcionário].[Nome].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Nome Do Chefe]" caption="Nome Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Do Chefe].[All]" allUniqueName="[Funcionário].[Nome Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Por Função Do Chefe]" caption="Por Função Do Chefe" defaultMemberUniqueName="[Funcionário].[Por Função Do Chefe].[All]" allUniqueName="[Funcionário].[Por Função Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Por Nome Completo Do Chefe]" caption="Por Nome Completo Do Chefe" defaultMemberUniqueName="[Funcionário].[Por Nome Completo Do Chefe].[All]" allUniqueName="[Funcionário].[Por Nome Completo Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Sobrenome]" caption="Sobrenome" attribute="1" defaultMemberUniqueName="[Funcionário].[Sobrenome].[All]" allUniqueName="[Funcionário].[Sobrenome].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Sobrenome Do Chefe]" caption="Sobrenome Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Sobrenome Do Chefe].[All]" allUniqueName="[Funcionário].[Sobrenome Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Conclusao].[Hora 12h]" caption="Hora Conclusao.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Conclusao].[Hora 12h].[All]" allUniqueName="[Hora Conclusao].[Hora 12h].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Conclusao].[Hora 24h]" caption="Hora Conclusao.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Conclusao].[Hora 24h].[All]" allUniqueName="[Hora Conclusao].[Hora 24h].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Entrega].[Hora 12h]" caption="Hora Entrega.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Entrega].[Hora 12h].[All]" allUniqueName="[Hora Entrega].[Hora 12h].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Entrega].[Hora 24h]" caption="Hora Entrega.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Entrega].[Hora 24h].[All]" allUniqueName="[Hora Entrega].[Hora 24h].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Requisicao].[Hora 12h]" caption="Hora Requisicao.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Requisicao].[Hora 12h].[All]" allUniqueName="[Hora Requisicao].[Hora 12h].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Requisicao].[Hora 24h]" caption="Hora Requisicao.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Requisicao].[Hora 24h].[All]" allUniqueName="[Hora Requisicao].[Hora 24h].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Tentativa].[Hora 12h]" caption="Hora Tentativa.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Tentativa].[Hora 12h].[All]" allUniqueName="[Hora Tentativa].[Hora 12h].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Tentativa].[Hora 24h]" caption="Hora Tentativa.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Tentativa].[Hora 24h].[All]" allUniqueName="[Hora Tentativa].[Hora 24h].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Intervalo]" caption="Intervalo Idade Cliente.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Intervalo].[All]" allUniqueName="[Intervalo Idade Cliente].[Intervalo].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Nome]" caption="Intervalo Idade Cliente.Nome" attribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Nome].[All]" allUniqueName="[Intervalo Idade Cliente].[Nome].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Intervalo]" caption="Intervalo Idade Na Requisição.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Intervalo].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Intervalo].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Nome]" caption="Intervalo Idade Na Requisição.Nome" attribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Nome].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Nome].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Classe]" caption="Intervalo Rendimento Cliente.Classe" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Classe].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Classe].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Codigo]" caption="Intervalo Rendimento Cliente.Codigo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Codigo].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Codigo].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Intervalo]" caption="Intervalo Rendimento Cliente.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Intervalo].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Intervalo].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Classe]" caption="Intervalo Rendimento Na Requisição.Classe" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Classe].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Classe].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Codigo]" caption="Intervalo Rendimento Na Requisição.Codigo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Codigo].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Codigo].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Intervalo]" caption="Intervalo Rendimento Na Requisição.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Intervalo].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Intervalo].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Código Postal]" caption="Morada Entrega.Código Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Código Postal].[All]" allUniqueName="[Morada Entrega].[Código Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Código Postal Completo]" caption="Morada Entrega.Código Postal Completo" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Código Postal Completo].[All]" allUniqueName="[Morada Entrega].[Código Postal Completo].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Designação Postal]" caption="Morada Entrega.Designação Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Designação Postal].[All]" allUniqueName="[Morada Entrega].[Designação Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Distrito - Número Da Porta]" caption="Morada Entrega.Distrito - Número Da Porta" defaultMemberUniqueName="[Morada Entrega].[Distrito - Número Da Porta].[All]" allUniqueName="[Morada Entrega].[Distrito - Número Da Porta].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Extensão Código Postal]" caption="Morada Entrega.Extensão Código Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Extensão Código Postal].[All]" allUniqueName="[Morada Entrega].[Extensão Código Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Localidade]" caption="Morada Entrega.Localidade" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Localidade].[All]" allUniqueName="[Morada Entrega].[Localidade].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Código Postal]" caption="Morada Facturacao.Código Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Código Postal].[All]" allUniqueName="[Morada Facturacao].[Código Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Código Postal Completo]" caption="Morada Facturacao.Código Postal Completo" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Código Postal Completo].[All]" allUniqueName="[Morada Facturacao].[Código Postal Completo].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Designação Postal]" caption="Morada Facturacao.Designação Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Designação Postal].[All]" allUniqueName="[Morada Facturacao].[Designação Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Distrito - Número Da Porta]" caption="Morada Facturacao.Distrito - Número Da Porta" defaultMemberUniqueName="[Morada Facturacao].[Distrito - Número Da Porta].[All]" allUniqueName="[Morada Facturacao].[Distrito - Número Da Porta].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Extensão Código Postal]" caption="Morada Facturacao.Extensão Código Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Extensão Código Postal].[All]" allUniqueName="[Morada Facturacao].[Extensão Código Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Localidade]" caption="Morada Facturacao.Localidade" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Localidade].[All]" allUniqueName="[Morada Facturacao].[Localidade].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Tipo Servico].[Tipo]" caption="Tipo" attribute="1" defaultMemberUniqueName="[Tipo Servico].[Tipo].[All]" allUniqueName="[Tipo Servico].[Tipo].[All]" dimensionUniqueName="[Tipo Servico]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Designação]" caption="Designação" attribute="1" defaultMemberUniqueName="[Cliente].[Designação].[All]" allUniqueName="[Cliente].[Designação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente].[Keycol].[All]" allUniqueName="[Cliente].[Keycol].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Nome Completo De Contacto]" caption="Nome Completo De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Nome Completo De Contacto].[All]" allUniqueName="[Cliente].[Nome Completo De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Ano]" caption="Data Conclusao.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Ano].[All]" allUniqueName="[Data Conclusao].[Ano].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Dia]" caption="Data Conclusao.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia].[All]" allUniqueName="[Data Conclusao].[Dia].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Keycol]" caption="Data Conclusao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Conclusao].[Keycol].[All]" allUniqueName="[Data Conclusao].[Keycol].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Mês Número]" caption="Data Conclusao.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Mês Número].[All]" allUniqueName="[Data Conclusao].[Mês Número].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Trimestre]" caption="Data Conclusao.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Trimestre].[All]" allUniqueName="[Data Conclusao].[Trimestre].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Ano]" caption="Data Requisicao.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Ano].[All]" allUniqueName="[Data Requisicao].[Ano].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Dia]" caption="Data Requisicao.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia].[All]" allUniqueName="[Data Requisicao].[Dia].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Keycol]" caption="Data Requisicao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Requisicao].[Keycol].[All]" allUniqueName="[Data Requisicao].[Keycol].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Mês Número]" caption="Data Requisicao.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Mês Número].[All]" allUniqueName="[Data Requisicao].[Mês Número].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Trimestre]" caption="Data Requisicao.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Trimestre].[All]" allUniqueName="[Data Requisicao].[Trimestre].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Ano]" caption="Data Tentativa.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Ano].[All]" allUniqueName="[Data Tentativa].[Ano].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Dia]" caption="Data Tentativa.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia].[All]" allUniqueName="[Data Tentativa].[Dia].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Keycol]" caption="Data Tentativa.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Tentativa].[Keycol].[All]" allUniqueName="[Data Tentativa].[Keycol].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Mês Número]" caption="Data Tentativa.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Mês Número].[All]" allUniqueName="[Data Tentativa].[Mês Número].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Trimestre]" caption="Data Tentativa.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Trimestre].[All]" allUniqueName="[Data Tentativa].[Trimestre].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Função]" caption="Função" attribute="1" defaultMemberUniqueName="[Funcionário].[Função].[All]" allUniqueName="[Funcionário].[Função].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Função Do Chefe]" caption="Função Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Função Do Chefe].[All]" allUniqueName="[Funcionário].[Função Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Funcionário].[Keycol].[All]" allUniqueName="[Funcionário].[Keycol].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Localização]" caption="Localização" attribute="1" defaultMemberUniqueName="[Funcionário].[Localização].[All]" allUniqueName="[Funcionário].[Localização].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Loja]" caption="Loja" attribute="1" defaultMemberUniqueName="[Funcionário].[Loja].[All]" allUniqueName="[Funcionário].[Loja].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Nome Completo]" caption="Nome Completo" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Completo].[All]" allUniqueName="[Funcionário].[Nome Completo].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Nome Completo Do Chefe]" caption="Nome Completo Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Completo Do Chefe].[All]" allUniqueName="[Funcionário].[Nome Completo Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Hora Conclusao].[Keycol]" caption="Hora Conclusao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Conclusao].[Keycol].[All]" allUniqueName="[Hora Conclusao].[Keycol].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Hora Entrega].[Keycol]" caption="Hora Entrega.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Entrega].[Keycol].[All]" allUniqueName="[Hora Entrega].[Keycol].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Hora Requisicao].[Keycol]" caption="Hora Requisicao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Requisicao].[Keycol].[All]" allUniqueName="[Hora Requisicao].[Keycol].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Hora Tentativa].[Keycol]" caption="Hora Tentativa.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Tentativa].[Keycol].[All]" allUniqueName="[Hora Tentativa].[Keycol].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Keycol]" caption="Intervalo Idade Cliente.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Keycol].[All]" allUniqueName="[Intervalo Idade Cliente].[Keycol].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Keycol]" caption="Intervalo Idade Na Requisição.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Keycol].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Keycol].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Keycol]" caption="Intervalo Rendimento Cliente.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Keycol].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Keycol].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Keycol]" caption="Intervalo Rendimento Na Requisição.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Keycol].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Keycol].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Concelho]" caption="Morada Entrega.Concelho" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Concelho].[All]" allUniqueName="[Morada Entrega].[Concelho].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Distrito]" caption="Morada Entrega.Distrito" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Distrito].[All]" allUniqueName="[Morada Entrega].[Distrito].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Freguesia]" caption="Morada Entrega.Freguesia" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Freguesia].[All]" allUniqueName="[Morada Entrega].[Freguesia].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Keycol]" caption="Morada Entrega.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Morada Entrega].[Keycol].[All]" allUniqueName="[Morada Entrega].[Keycol].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Número Da Porta]" caption="Morada Entrega.Número Da Porta" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Número Da Porta].[All]" allUniqueName="[Morada Entrega].[Número Da Porta].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Rua]" caption="Morada Entrega.Rua" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Rua].[All]" allUniqueName="[Morada Entrega].[Rua].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Concelho]" caption="Morada Facturacao.Concelho" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Concelho].[All]" allUniqueName="[Morada Facturacao].[Concelho].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Distrito]" caption="Morada Facturacao.Distrito" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Distrito].[All]" allUniqueName="[Morada Facturacao].[Distrito].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Freguesia]" caption="Morada Facturacao.Freguesia" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Freguesia].[All]" allUniqueName="[Morada Facturacao].[Freguesia].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Keycol]" caption="Morada Facturacao.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Morada Facturacao].[Keycol].[All]" allUniqueName="[Morada Facturacao].[Keycol].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Número Da Porta]" caption="Morada Facturacao.Número Da Porta" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Número Da Porta].[All]" allUniqueName="[Morada Facturacao].[Número Da Porta].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Rua]" caption="Morada Facturacao.Rua" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Rua].[All]" allUniqueName="[Morada Facturacao].[Rua].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Tipo Servico].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Tipo Servico].[Keycol].[All]" allUniqueName="[Tipo Servico].[Keycol].[All]" dimensionUniqueName="[Tipo Servico]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Número De Entregas]" caption="Número De Entregas" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Valor]" caption="Valor" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Dentro Do SLA]" caption="Dentro Do SLA" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Concluido]" caption="Concluido" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Contagem de Servicos]" caption="Contagem de Servicos" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Número Entregas por Serviço]" caption="Número Entregas por Serviço" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Valor do Serviço]" caption="Valor do Serviço" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Serviço Dentro Do SLA]" caption="Serviço Dentro Do SLA" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Serviço Concluido]" caption="Serviço Concluido" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Sucesso]" caption="Sucesso" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Contagem de Entregas]" caption="Contagem de Entregas" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="17">
+    <dimension name="Cliente" uniqueName="[Cliente]" caption="Cliente"/>
+    <dimension name="Data Conclusao" uniqueName="[Data Conclusao]" caption="Data Conclusao"/>
+    <dimension name="Data Requisicao" uniqueName="[Data Requisicao]" caption="Data Requisicao"/>
+    <dimension name="Data Tentativa" uniqueName="[Data Tentativa]" caption="Data Tentativa"/>
+    <dimension name="Funcionário" uniqueName="[Funcionário]" caption="Funcionário"/>
+    <dimension name="Hora Conclusao" uniqueName="[Hora Conclusao]" caption="Hora Conclusao"/>
+    <dimension name="Hora Entrega" uniqueName="[Hora Entrega]" caption="Hora Entrega"/>
+    <dimension name="Hora Requisicao" uniqueName="[Hora Requisicao]" caption="Hora Requisicao"/>
+    <dimension name="Hora Tentativa" uniqueName="[Hora Tentativa]" caption="Hora Tentativa"/>
+    <dimension name="Intervalo Idade Cliente" uniqueName="[Intervalo Idade Cliente]" caption="Intervalo Idade Cliente"/>
+    <dimension name="Intervalo Idade Na Requisição" uniqueName="[Intervalo Idade Na Requisição]" caption="Intervalo Idade Na Requisição"/>
+    <dimension name="Intervalo Rendimento Cliente" uniqueName="[Intervalo Rendimento Cliente]" caption="Intervalo Rendimento Cliente"/>
+    <dimension name="Intervalo Rendimento Na Requisição" uniqueName="[Intervalo Rendimento Na Requisição]" caption="Intervalo Rendimento Na Requisição"/>
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Morada Entrega" uniqueName="[Morada Entrega]" caption="Morada Entrega"/>
+    <dimension name="Morada Facturacao" uniqueName="[Morada Facturacao]" caption="Morada Facturacao"/>
+    <dimension name="Tipo Servico" uniqueName="[Tipo Servico]" caption="Tipo Servico"/>
+  </dimensions>
+  <measureGroups count="2">
+    <measureGroup name="Entregas Dos Servicos" caption="Entregas Dos Servicos"/>
+    <measureGroup name="Servicos" caption="Servicos"/>
+  </measureGroups>
+  <maps count="25">
+    <map measureGroup="0" dimension="0"/>
+    <map measureGroup="0" dimension="1"/>
+    <map measureGroup="0" dimension="2"/>
+    <map measureGroup="0" dimension="3"/>
+    <map measureGroup="0" dimension="4"/>
+    <map measureGroup="0" dimension="5"/>
+    <map measureGroup="0" dimension="6"/>
+    <map measureGroup="0" dimension="7"/>
+    <map measureGroup="0" dimension="8"/>
+    <map measureGroup="0" dimension="9"/>
+    <map measureGroup="0" dimension="11"/>
+    <map measureGroup="0" dimension="14"/>
+    <map measureGroup="0" dimension="15"/>
+    <map measureGroup="0" dimension="16"/>
+    <map measureGroup="1" dimension="0"/>
+    <map measureGroup="1" dimension="1"/>
+    <map measureGroup="1" dimension="2"/>
+    <map measureGroup="1" dimension="5"/>
+    <map measureGroup="1" dimension="6"/>
+    <map measureGroup="1" dimension="7"/>
+    <map measureGroup="1" dimension="10"/>
+    <map measureGroup="1" dimension="12"/>
+    <map measureGroup="1" dimension="14"/>
+    <map measureGroup="1" dimension="15"/>
+    <map measureGroup="1" dimension="16"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Rui Miranda" refreshedDate="41444.925415509257" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+  <cacheSource type="external" connectionId="5"/>
+  <cacheFields count="19">
+    <cacheField name="[Measures].[Contagem de Entregas]" caption="Contagem de Entregas" numFmtId="0" hierarchy="129" level="32767"/>
+    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Distrito]" caption="Distrito" numFmtId="0" hierarchy="69" level="1">
+      <sharedItems count="2">
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Distrito].&amp;[Lisboa]" c="Lisboa"/>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Distrito].&amp;[Porto]" c="Porto"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Concelho]" caption="Concelho" numFmtId="0" hierarchy="69" level="2" mappingCount="1">
+      <sharedItems count="2">
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Concelho].&amp;[Lisboa]&amp;[Lisboa]" c="Lisboa" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Concelho].&amp;[Porto]&amp;[Porto]" c="Porto" cp="1">
+          <x v="1"/>
+        </s>
+      </sharedItems>
+      <mpMap v="6"/>
+    </cacheField>
+    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia]" caption="Freguesia" numFmtId="0" hierarchy="69" level="3" mappingCount="1">
+      <sharedItems count="50">
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Ajuda]" c="Ajuda" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Alcântara]" c="Alcântara" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Alvalade]" c="Alvalade" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Anjos]" c="Anjos" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Beato]" c="Beato" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Benfica]" c="Benfica" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Campo Grande]" c="Campo Grande" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Campolide]" c="Campolide" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Carnide]" c="Carnide" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Coração de Jesus]" c="Coração de Jesus" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Encarnação]" c="Encarnação" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Lapa]" c="Lapa" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Lumiar]" c="Lumiar" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Madalena]" c="Madalena" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Mártires]" c="Mártires" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Marvila]" c="Marvila" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Nossa Senhora de Fátima]" c="Nossa Senhora de Fátima" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Pena]" c="Pena" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Penha de França]" c="Penha de França" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Prazeres]" c="Prazeres" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Sacramento]" c="Sacramento" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santa Catarina]" c="Santa Catarina" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santa Engrácia]" c="Santa Engrácia" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santa Isabel]" c="Santa Isabel" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santa Maria de Belém]" c="Santa Maria de Belém" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santa Maria dos Olivais]" c="Santa Maria dos Olivais" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santo Condestável]" c="Santo Condestável" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Santos-o-Velho]" c="Santos-o-Velho" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Cristóvão]" c="São Cristóvão" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Domingos de Benfica]" c="São Domingos de Benfica" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São João de Brito]" c="São João de Brito" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São João de Deus]" c="São João de Deus" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Jorge de Arroios]" c="São Jorge de Arroios" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São José]" c="São José" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Mamede]" c="São Mamede" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Nicolau]" c="São Nicolau" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Paulo]" c="São Paulo" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Sebastião da Pedreira]" c="São Sebastião da Pedreira" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[São Vicente de Fora]" c="São Vicente de Fora" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Lisboa]&amp;[Lisboa]&amp;[Sé]" c="Sé" cp="1">
+          <x/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Aldoar]" c="Aldoar" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Bonfim]" c="Bonfim" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Campanhã]" c="Campanhã" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Cedofeita]" c="Cedofeita" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Lordelo do Ouro]" c="Lordelo do Ouro" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Massarelos]" c="Massarelos" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Paranhos]" c="Paranhos" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Ramalde]" c="Ramalde" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Santo Ildefonso]" c="Santo Ildefonso" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].&amp;[Porto]&amp;[Porto]&amp;[Vitória]" c="Vitória" cp="1">
+          <x v="1"/>
+        </s>
+      </sharedItems>
+      <mpMap v="7"/>
+    </cacheField>
+    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Rua]" caption="Rua" numFmtId="0" hierarchy="69" level="4">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Número Da Porta]" caption="Número Da Porta" numFmtId="0" hierarchy="69" level="5">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Concelho].[Distrito]" caption="Distrito" propertyName="Distrito" numFmtId="0" hierarchy="69" level="2" memberPropertyField="1">
+      <sharedItems count="2">
+        <s v="Lisboa"/>
+        <s v="Porto"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Freguesia].[Concelho]" caption="Concelho" propertyName="Concelho" numFmtId="0" hierarchy="69" level="3" memberPropertyField="1">
+      <sharedItems count="2">
+        <s v="Lisboa"/>
+        <s v="Porto"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Rua].[Freguesia]" caption="Freguesia" propertyName="Freguesia" numFmtId="0" hierarchy="69" level="4" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Morada Facturacao].[Distrito - Número Da Porta].[Número Da Porta].[Rua]" caption="Rua" propertyName="Rua" numFmtId="0" hierarchy="69" level="5" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Tipo Servico].[Tipo].[Tipo]" caption="Tipo" numFmtId="0" hierarchy="72" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Ano]" caption="Ano" numFmtId="0" hierarchy="29" level="1">
+      <sharedItems count="4">
+        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2010]" c="2010"/>
+        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2011]" c="2011"/>
+        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2012]" c="2012"/>
+        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2013]" c="2013"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Trimestre]" caption="Trimestre" numFmtId="0" hierarchy="29" level="2" mappingCount="1">
+      <sharedItems count="2">
+        <s v="[Data Tentativa].[Ano - Dia].[Trimestre].&amp;[2013]&amp;[1]" c="1" cp="1">
+          <x/>
+        </s>
+        <s v="[Data Tentativa].[Ano - Dia].[Trimestre].&amp;[2013]&amp;[2]" c="2" cp="1">
+          <x/>
+        </s>
+      </sharedItems>
+      <mpMap v="15"/>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Mês Número]" caption="Mês Número" numFmtId="0" hierarchy="29" level="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Dia]" caption="Dia" numFmtId="0" hierarchy="29" level="4">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Trimestre].[Ano]" caption="Ano" propertyName="Ano" numFmtId="0" hierarchy="29" level="2" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2013" maxValue="2013" count="1">
+        <n v="2013"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Mês Número].[Trimestre]" caption="Trimestre" propertyName="Trimestre" numFmtId="0" hierarchy="29" level="3" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Dia].[Mês Número]" caption="Mês Número" propertyName="Mês Número" numFmtId="0" hierarchy="29" level="4" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="Dummy0" numFmtId="0" hierarchy="130" level="32767">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{63CAB8AC-B538-458d-9737-405883B0398D}">
+          <x14:cacheField ignore="1"/>
+        </ext>
+      </extLst>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="131">
+    <cacheHierarchy uniqueName="[Cliente].[Activo]" caption="Activo" attribute="1" defaultMemberUniqueName="[Cliente].[Activo].[All]" allUniqueName="[Cliente].[Activo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Codigo Postal]" caption="Codigo Postal" attribute="1" defaultMemberUniqueName="[Cliente].[Codigo Postal].[All]" allUniqueName="[Cliente].[Codigo Postal].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Educação]" caption="Educação" attribute="1" defaultMemberUniqueName="[Cliente].[Educação].[All]" allUniqueName="[Cliente].[Educação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Estado Civil]" caption="Estado Civil" attribute="1" defaultMemberUniqueName="[Cliente].[Estado Civil].[All]" allUniqueName="[Cliente].[Estado Civil].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Género]" caption="Género" attribute="1" defaultMemberUniqueName="[Cliente].[Género].[All]" allUniqueName="[Cliente].[Género].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Idade]" caption="Intervalo Idade" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Idade].[All]" allUniqueName="[Cliente].[Intervalo Idade].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Idade Nome]" caption="Intervalo Idade Nome" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Idade Nome].[All]" allUniqueName="[Cliente].[Intervalo Idade Nome].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento]" caption="Intervalo Rendimento" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento].[All]" allUniqueName="[Cliente].[Intervalo Rendimento].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento Classe]" caption="Intervalo Rendimento Classe" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento Classe].[All]" allUniqueName="[Cliente].[Intervalo Rendimento Classe].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento Codigo]" caption="Intervalo Rendimento Codigo" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento Codigo].[All]" allUniqueName="[Cliente].[Intervalo Rendimento Codigo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Nome De Contacto]" caption="Nome De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Nome De Contacto].[All]" allUniqueName="[Cliente].[Nome De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Número De Carros Possuidos]" caption="Número De Carros Possuidos" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Carros Possuidos].[All]" allUniqueName="[Cliente].[Número De Carros Possuidos].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Número De Filhos]" caption="Número De Filhos" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Filhos].[All]" allUniqueName="[Cliente].[Número De Filhos].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Número De Filhos Em Casa]" caption="Número De Filhos Em Casa" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Filhos Em Casa].[All]" allUniqueName="[Cliente].[Número De Filhos Em Casa].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Ocupação]" caption="Ocupação" attribute="1" defaultMemberUniqueName="[Cliente].[Ocupação].[All]" allUniqueName="[Cliente].[Ocupação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Por Designação]" caption="Por Designação" defaultMemberUniqueName="[Cliente].[Por Designação].[All]" allUniqueName="[Cliente].[Por Designação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Possui Casa]" caption="Possui Casa" attribute="1" defaultMemberUniqueName="[Cliente].[Possui Casa].[All]" allUniqueName="[Cliente].[Possui Casa].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Singular]" caption="Singular" attribute="1" defaultMemberUniqueName="[Cliente].[Singular].[All]" allUniqueName="[Cliente].[Singular].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Sobrenome De Contacto]" caption="Sobrenome De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Sobrenome De Contacto].[All]" allUniqueName="[Cliente].[Sobrenome De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Ano - Dia]" caption="Data Conclusao.Ano - Dia" time="1" defaultMemberUniqueName="[Data Conclusao].[Ano - Dia].[All]" allUniqueName="[Data Conclusao].[Ano - Dia].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Data]" caption="Data Conclusao.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Data].[All]" allUniqueName="[Data Conclusao].[Data].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Dia Da Semana Nome]" caption="Data Conclusao.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia Da Semana Nome].[All]" allUniqueName="[Data Conclusao].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Dia Da Semana Número]" caption="Data Conclusao.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia Da Semana Número].[All]" allUniqueName="[Data Conclusao].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Mês Nome]" caption="Data Conclusao.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Mês Nome].[All]" allUniqueName="[Data Conclusao].[Mês Nome].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Ano - Dia]" caption="Data Requisicao.Ano - Dia" time="1" defaultMemberUniqueName="[Data Requisicao].[Ano - Dia].[All]" allUniqueName="[Data Requisicao].[Ano - Dia].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Data]" caption="Data Requisicao.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Data].[All]" allUniqueName="[Data Requisicao].[Data].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Dia Da Semana Nome]" caption="Data Requisicao.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia Da Semana Nome].[All]" allUniqueName="[Data Requisicao].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Dia Da Semana Número]" caption="Data Requisicao.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia Da Semana Número].[All]" allUniqueName="[Data Requisicao].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Mês Nome]" caption="Data Requisicao.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Mês Nome].[All]" allUniqueName="[Data Requisicao].[Mês Nome].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Ano - Dia]" caption="Data Tentativa.Ano - Dia" time="1" defaultMemberUniqueName="[Data Tentativa].[Ano - Dia].[All]" allUniqueName="[Data Tentativa].[Ano - Dia].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="5" unbalanced="0">
+      <fieldsUsage count="5">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="11"/>
+        <fieldUsage x="12"/>
+        <fieldUsage x="13"/>
+        <fieldUsage x="14"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Data]" caption="Data Tentativa.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Data].[All]" allUniqueName="[Data Tentativa].[Data].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Dia Da Semana Nome]" caption="Data Tentativa.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia Da Semana Nome].[All]" allUniqueName="[Data Tentativa].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Dia Da Semana Número]" caption="Data Tentativa.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia Da Semana Número].[All]" allUniqueName="[Data Tentativa].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Mês Nome]" caption="Data Tentativa.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Mês Nome].[All]" allUniqueName="[Data Tentativa].[Mês Nome].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Activo]" caption="Activo" attribute="1" defaultMemberUniqueName="[Funcionário].[Activo].[All]" allUniqueName="[Funcionário].[Activo].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Localização - Loja]" caption="Localização - Loja" defaultMemberUniqueName="[Funcionário].[Localização - Loja].[All]" allUniqueName="[Funcionário].[Localização - Loja].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Nome]" caption="Nome" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome].[All]" allUniqueName="[Funcionário].[Nome].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Nome Do Chefe]" caption="Nome Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Do Chefe].[All]" allUniqueName="[Funcionário].[Nome Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Por Função Do Chefe]" caption="Por Função Do Chefe" defaultMemberUniqueName="[Funcionário].[Por Função Do Chefe].[All]" allUniqueName="[Funcionário].[Por Função Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Por Nome Completo Do Chefe]" caption="Por Nome Completo Do Chefe" defaultMemberUniqueName="[Funcionário].[Por Nome Completo Do Chefe].[All]" allUniqueName="[Funcionário].[Por Nome Completo Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Sobrenome]" caption="Sobrenome" attribute="1" defaultMemberUniqueName="[Funcionário].[Sobrenome].[All]" allUniqueName="[Funcionário].[Sobrenome].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Sobrenome Do Chefe]" caption="Sobrenome Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Sobrenome Do Chefe].[All]" allUniqueName="[Funcionário].[Sobrenome Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Conclusao].[Hora 12h]" caption="Hora Conclusao.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Conclusao].[Hora 12h].[All]" allUniqueName="[Hora Conclusao].[Hora 12h].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Conclusao].[Hora 24h]" caption="Hora Conclusao.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Conclusao].[Hora 24h].[All]" allUniqueName="[Hora Conclusao].[Hora 24h].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Entrega].[Hora 12h]" caption="Hora Entrega.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Entrega].[Hora 12h].[All]" allUniqueName="[Hora Entrega].[Hora 12h].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Entrega].[Hora 24h]" caption="Hora Entrega.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Entrega].[Hora 24h].[All]" allUniqueName="[Hora Entrega].[Hora 24h].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Requisicao].[Hora 12h]" caption="Hora Requisicao.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Requisicao].[Hora 12h].[All]" allUniqueName="[Hora Requisicao].[Hora 12h].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Requisicao].[Hora 24h]" caption="Hora Requisicao.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Requisicao].[Hora 24h].[All]" allUniqueName="[Hora Requisicao].[Hora 24h].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Tentativa].[Hora 12h]" caption="Hora Tentativa.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Tentativa].[Hora 12h].[All]" allUniqueName="[Hora Tentativa].[Hora 12h].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Tentativa].[Hora 24h]" caption="Hora Tentativa.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Tentativa].[Hora 24h].[All]" allUniqueName="[Hora Tentativa].[Hora 24h].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Intervalo]" caption="Intervalo Idade Cliente.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Intervalo].[All]" allUniqueName="[Intervalo Idade Cliente].[Intervalo].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Nome]" caption="Intervalo Idade Cliente.Nome" attribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Nome].[All]" allUniqueName="[Intervalo Idade Cliente].[Nome].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Intervalo]" caption="Intervalo Idade Na Requisição.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Intervalo].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Intervalo].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Nome]" caption="Intervalo Idade Na Requisição.Nome" attribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Nome].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Nome].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Classe]" caption="Intervalo Rendimento Cliente.Classe" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Classe].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Classe].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Codigo]" caption="Intervalo Rendimento Cliente.Codigo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Codigo].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Codigo].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Intervalo]" caption="Intervalo Rendimento Cliente.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Intervalo].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Intervalo].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Classe]" caption="Intervalo Rendimento Na Requisição.Classe" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Classe].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Classe].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Codigo]" caption="Intervalo Rendimento Na Requisição.Codigo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Codigo].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Codigo].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Intervalo]" caption="Intervalo Rendimento Na Requisição.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Intervalo].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Intervalo].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Código Postal]" caption="Morada Entrega.Código Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Código Postal].[All]" allUniqueName="[Morada Entrega].[Código Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Código Postal Completo]" caption="Morada Entrega.Código Postal Completo" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Código Postal Completo].[All]" allUniqueName="[Morada Entrega].[Código Postal Completo].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Designação Postal]" caption="Morada Entrega.Designação Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Designação Postal].[All]" allUniqueName="[Morada Entrega].[Designação Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Distrito - Número Da Porta]" caption="Morada Entrega.Distrito - Número Da Porta" defaultMemberUniqueName="[Morada Entrega].[Distrito - Número Da Porta].[All]" allUniqueName="[Morada Entrega].[Distrito - Número Da Porta].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Extensão Código Postal]" caption="Morada Entrega.Extensão Código Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Extensão Código Postal].[All]" allUniqueName="[Morada Entrega].[Extensão Código Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Localidade]" caption="Morada Entrega.Localidade" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Localidade].[All]" allUniqueName="[Morada Entrega].[Localidade].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Código Postal]" caption="Morada Facturacao.Código Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Código Postal].[All]" allUniqueName="[Morada Facturacao].[Código Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Código Postal Completo]" caption="Morada Facturacao.Código Postal Completo" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Código Postal Completo].[All]" allUniqueName="[Morada Facturacao].[Código Postal Completo].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Designação Postal]" caption="Morada Facturacao.Designação Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Designação Postal].[All]" allUniqueName="[Morada Facturacao].[Designação Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Distrito - Número Da Porta]" caption="Morada Facturacao.Distrito - Número Da Porta" defaultMemberUniqueName="[Morada Facturacao].[Distrito - Número Da Porta].[All]" allUniqueName="[Morada Facturacao].[Distrito - Número Da Porta].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="6" unbalanced="0">
+      <fieldsUsage count="6">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+        <fieldUsage x="2"/>
+        <fieldUsage x="3"/>
+        <fieldUsage x="4"/>
+        <fieldUsage x="5"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Extensão Código Postal]" caption="Morada Facturacao.Extensão Código Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Extensão Código Postal].[All]" allUniqueName="[Morada Facturacao].[Extensão Código Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Localidade]" caption="Morada Facturacao.Localidade" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Localidade].[All]" allUniqueName="[Morada Facturacao].[Localidade].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Tipo Servico].[Tipo]" caption="Tipo" attribute="1" defaultMemberUniqueName="[Tipo Servico].[Tipo].[All]" allUniqueName="[Tipo Servico].[Tipo].[All]" dimensionUniqueName="[Tipo Servico]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="10"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Cliente].[Designação]" caption="Designação" attribute="1" defaultMemberUniqueName="[Cliente].[Designação].[All]" allUniqueName="[Cliente].[Designação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente].[Keycol].[All]" allUniqueName="[Cliente].[Keycol].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Nome Completo De Contacto]" caption="Nome Completo De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Nome Completo De Contacto].[All]" allUniqueName="[Cliente].[Nome Completo De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Ano]" caption="Data Conclusao.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Ano].[All]" allUniqueName="[Data Conclusao].[Ano].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Dia]" caption="Data Conclusao.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia].[All]" allUniqueName="[Data Conclusao].[Dia].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Keycol]" caption="Data Conclusao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Conclusao].[Keycol].[All]" allUniqueName="[Data Conclusao].[Keycol].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Mês Número]" caption="Data Conclusao.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Mês Número].[All]" allUniqueName="[Data Conclusao].[Mês Número].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Trimestre]" caption="Data Conclusao.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Trimestre].[All]" allUniqueName="[Data Conclusao].[Trimestre].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Ano]" caption="Data Requisicao.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Ano].[All]" allUniqueName="[Data Requisicao].[Ano].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Dia]" caption="Data Requisicao.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia].[All]" allUniqueName="[Data Requisicao].[Dia].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Keycol]" caption="Data Requisicao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Requisicao].[Keycol].[All]" allUniqueName="[Data Requisicao].[Keycol].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Mês Número]" caption="Data Requisicao.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Mês Número].[All]" allUniqueName="[Data Requisicao].[Mês Número].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Trimestre]" caption="Data Requisicao.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Trimestre].[All]" allUniqueName="[Data Requisicao].[Trimestre].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Ano]" caption="Data Tentativa.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Ano].[All]" allUniqueName="[Data Tentativa].[Ano].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Dia]" caption="Data Tentativa.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia].[All]" allUniqueName="[Data Tentativa].[Dia].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Keycol]" caption="Data Tentativa.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Tentativa].[Keycol].[All]" allUniqueName="[Data Tentativa].[Keycol].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Mês Número]" caption="Data Tentativa.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Mês Número].[All]" allUniqueName="[Data Tentativa].[Mês Número].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Trimestre]" caption="Data Tentativa.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Trimestre].[All]" allUniqueName="[Data Tentativa].[Trimestre].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Função]" caption="Função" attribute="1" defaultMemberUniqueName="[Funcionário].[Função].[All]" allUniqueName="[Funcionário].[Função].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Função Do Chefe]" caption="Função Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Função Do Chefe].[All]" allUniqueName="[Funcionário].[Função Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Funcionário].[Keycol].[All]" allUniqueName="[Funcionário].[Keycol].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Localização]" caption="Localização" attribute="1" defaultMemberUniqueName="[Funcionário].[Localização].[All]" allUniqueName="[Funcionário].[Localização].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Loja]" caption="Loja" attribute="1" defaultMemberUniqueName="[Funcionário].[Loja].[All]" allUniqueName="[Funcionário].[Loja].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Nome Completo]" caption="Nome Completo" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Completo].[All]" allUniqueName="[Funcionário].[Nome Completo].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Nome Completo Do Chefe]" caption="Nome Completo Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Completo Do Chefe].[All]" allUniqueName="[Funcionário].[Nome Completo Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Hora Conclusao].[Keycol]" caption="Hora Conclusao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Conclusao].[Keycol].[All]" allUniqueName="[Hora Conclusao].[Keycol].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Hora Entrega].[Keycol]" caption="Hora Entrega.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Entrega].[Keycol].[All]" allUniqueName="[Hora Entrega].[Keycol].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Hora Requisicao].[Keycol]" caption="Hora Requisicao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Requisicao].[Keycol].[All]" allUniqueName="[Hora Requisicao].[Keycol].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Hora Tentativa].[Keycol]" caption="Hora Tentativa.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Tentativa].[Keycol].[All]" allUniqueName="[Hora Tentativa].[Keycol].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Keycol]" caption="Intervalo Idade Cliente.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Keycol].[All]" allUniqueName="[Intervalo Idade Cliente].[Keycol].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Keycol]" caption="Intervalo Idade Na Requisição.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Keycol].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Keycol].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Keycol]" caption="Intervalo Rendimento Cliente.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Keycol].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Keycol].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Keycol]" caption="Intervalo Rendimento Na Requisição.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Keycol].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Keycol].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Concelho]" caption="Morada Entrega.Concelho" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Concelho].[All]" allUniqueName="[Morada Entrega].[Concelho].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Distrito]" caption="Morada Entrega.Distrito" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Distrito].[All]" allUniqueName="[Morada Entrega].[Distrito].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Freguesia]" caption="Morada Entrega.Freguesia" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Freguesia].[All]" allUniqueName="[Morada Entrega].[Freguesia].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Keycol]" caption="Morada Entrega.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Morada Entrega].[Keycol].[All]" allUniqueName="[Morada Entrega].[Keycol].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Número Da Porta]" caption="Morada Entrega.Número Da Porta" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Número Da Porta].[All]" allUniqueName="[Morada Entrega].[Número Da Porta].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Rua]" caption="Morada Entrega.Rua" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Rua].[All]" allUniqueName="[Morada Entrega].[Rua].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Concelho]" caption="Morada Facturacao.Concelho" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Concelho].[All]" allUniqueName="[Morada Facturacao].[Concelho].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Distrito]" caption="Morada Facturacao.Distrito" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Distrito].[All]" allUniqueName="[Morada Facturacao].[Distrito].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Freguesia]" caption="Morada Facturacao.Freguesia" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Freguesia].[All]" allUniqueName="[Morada Facturacao].[Freguesia].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Keycol]" caption="Morada Facturacao.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Morada Facturacao].[Keycol].[All]" allUniqueName="[Morada Facturacao].[Keycol].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Número Da Porta]" caption="Morada Facturacao.Número Da Porta" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Número Da Porta].[All]" allUniqueName="[Morada Facturacao].[Número Da Porta].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Rua]" caption="Morada Facturacao.Rua" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Rua].[All]" allUniqueName="[Morada Facturacao].[Rua].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Tipo Servico].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Tipo Servico].[Keycol].[All]" allUniqueName="[Tipo Servico].[Keycol].[All]" dimensionUniqueName="[Tipo Servico]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Número De Entregas]" caption="Número De Entregas" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Valor]" caption="Valor" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Dentro Do SLA]" caption="Dentro Do SLA" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Concluido]" caption="Concluido" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Contagem de Servicos]" caption="Contagem de Servicos" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Número Entregas por Serviço]" caption="Número Entregas por Serviço" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Valor do Serviço]" caption="Valor do Serviço" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Serviço Dentro Do SLA]" caption="Serviço Dentro Do SLA" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Serviço Concluido]" caption="Serviço Concluido" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Sucesso]" caption="Sucesso" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Contagem de Entregas]" caption="Contagem de Entregas" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="Dummy0" caption="Activo" measure="1" count="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{8CF416AD-EC4C-4aba-99F5-12A058AE0983}">
+          <x14:cacheHierarchy ignore="1"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="17">
+    <dimension name="Cliente" uniqueName="[Cliente]" caption="Cliente"/>
+    <dimension name="Data Conclusao" uniqueName="[Data Conclusao]" caption="Data Conclusao"/>
+    <dimension name="Data Requisicao" uniqueName="[Data Requisicao]" caption="Data Requisicao"/>
+    <dimension name="Data Tentativa" uniqueName="[Data Tentativa]" caption="Data Tentativa"/>
+    <dimension name="Funcionário" uniqueName="[Funcionário]" caption="Funcionário"/>
+    <dimension name="Hora Conclusao" uniqueName="[Hora Conclusao]" caption="Hora Conclusao"/>
+    <dimension name="Hora Entrega" uniqueName="[Hora Entrega]" caption="Hora Entrega"/>
+    <dimension name="Hora Requisicao" uniqueName="[Hora Requisicao]" caption="Hora Requisicao"/>
+    <dimension name="Hora Tentativa" uniqueName="[Hora Tentativa]" caption="Hora Tentativa"/>
+    <dimension name="Intervalo Idade Cliente" uniqueName="[Intervalo Idade Cliente]" caption="Intervalo Idade Cliente"/>
+    <dimension name="Intervalo Idade Na Requisição" uniqueName="[Intervalo Idade Na Requisição]" caption="Intervalo Idade Na Requisição"/>
+    <dimension name="Intervalo Rendimento Cliente" uniqueName="[Intervalo Rendimento Cliente]" caption="Intervalo Rendimento Cliente"/>
+    <dimension name="Intervalo Rendimento Na Requisição" uniqueName="[Intervalo Rendimento Na Requisição]" caption="Intervalo Rendimento Na Requisição"/>
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Morada Entrega" uniqueName="[Morada Entrega]" caption="Morada Entrega"/>
+    <dimension name="Morada Facturacao" uniqueName="[Morada Facturacao]" caption="Morada Facturacao"/>
+    <dimension name="Tipo Servico" uniqueName="[Tipo Servico]" caption="Tipo Servico"/>
+  </dimensions>
+  <measureGroups count="2">
+    <measureGroup name="Entregas Dos Servicos" caption="Entregas Dos Servicos"/>
+    <measureGroup name="Servicos" caption="Servicos"/>
+  </measureGroups>
+  <maps count="25">
+    <map measureGroup="0" dimension="0"/>
+    <map measureGroup="0" dimension="1"/>
+    <map measureGroup="0" dimension="2"/>
+    <map measureGroup="0" dimension="3"/>
+    <map measureGroup="0" dimension="4"/>
+    <map measureGroup="0" dimension="5"/>
+    <map measureGroup="0" dimension="6"/>
+    <map measureGroup="0" dimension="7"/>
+    <map measureGroup="0" dimension="8"/>
+    <map measureGroup="0" dimension="9"/>
+    <map measureGroup="0" dimension="11"/>
+    <map measureGroup="0" dimension="14"/>
+    <map measureGroup="0" dimension="15"/>
+    <map measureGroup="0" dimension="16"/>
+    <map measureGroup="1" dimension="0"/>
+    <map measureGroup="1" dimension="1"/>
+    <map measureGroup="1" dimension="2"/>
+    <map measureGroup="1" dimension="5"/>
+    <map measureGroup="1" dimension="6"/>
+    <map measureGroup="1" dimension="7"/>
+    <map measureGroup="1" dimension="10"/>
+    <map measureGroup="1" dimension="12"/>
+    <map measureGroup="1" dimension="14"/>
+    <map measureGroup="1" dimension="15"/>
+    <map measureGroup="1" dimension="16"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Rui Miranda" refreshedDate="41444.925438888888" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+  <cacheSource type="external" connectionId="3"/>
+  <cacheFields count="16">
+    <cacheField name="[Measures].[Contagem de Entregas]" caption="Contagem de Entregas" numFmtId="0" hierarchy="129" level="32767"/>
+    <cacheField name="[Funcionário].[Localização - Loja].[Localização]" caption="Localização" numFmtId="0" hierarchy="35" level="1">
+      <sharedItems count="2">
+        <s v="[Funcionário].[Localização - Loja].[Localização].&amp;[Lisboa]" c="Lisboa"/>
+        <s v="[Funcionário].[Localização - Loja].[Localização].&amp;[Porto]" c="Porto"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Funcionário].[Localização - Loja].[Loja]" caption="Loja" numFmtId="0" hierarchy="35" level="2" mappingCount="1">
+      <sharedItems count="2">
+        <s v="[Funcionário].[Localização - Loja].[Loja].&amp;[Lisboa]&amp;[Sede]" c="Sede" cp="1">
+          <x/>
+        </s>
+        <s v="[Funcionário].[Localização - Loja].[Loja].&amp;[Porto]&amp;[Filial1]" c="Filial1" cp="1">
+          <x v="1"/>
+        </s>
+      </sharedItems>
+      <mpMap v="4"/>
+    </cacheField>
+    <cacheField name="[Funcionário].[Localização - Loja].[Nome Completo]" caption="Nome Completo" numFmtId="0" hierarchy="35" level="3" mappingCount="3">
+      <sharedItems count="3">
+        <s v="[Funcionário].[Localização - Loja].[Nome Completo].&amp;[Luciano Salgado]&amp;[Alarico Medina]" c="Alarico Medina" cp="3">
+          <x/>
+          <x/>
+          <x/>
+        </s>
+        <s v="[Funcionário].[Localização - Loja].[Nome Completo].&amp;[Sabrina Prada]&amp;[Vasco Moita]" c="Vasco Moita" cp="3">
+          <x/>
+          <x v="1"/>
+          <x v="1"/>
+        </s>
+        <s v="[Funcionário].[Localização - Loja].[Nome Completo].&amp;[Luciano Salgado]&amp;[Vanda Seabra]" u="1" c="Vanda Seabra"/>
+      </sharedItems>
+      <mpMap v="5"/>
+      <mpMap v="6"/>
+      <mpMap v="7"/>
+    </cacheField>
+    <cacheField name="[Funcionário].[Localização - Loja].[Loja].[Localização]" caption="Localização" propertyName="Localização" numFmtId="0" hierarchy="35" level="2" memberPropertyField="1">
+      <sharedItems count="2">
+        <s v="Lisboa"/>
+        <s v="Porto"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Funcionário].[Localização - Loja].[Nome Completo].[Função]" caption="Função" propertyName="Função" numFmtId="0" hierarchy="35" level="3" memberPropertyField="1">
+      <sharedItems count="1">
+        <s v="Paquete"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Funcionário].[Localização - Loja].[Nome Completo].[Loja]" caption="Loja" propertyName="Loja" numFmtId="0" hierarchy="35" level="3" memberPropertyField="1">
+      <sharedItems count="2">
+        <s v="Sede"/>
+        <s v="Filial1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Funcionário].[Localização - Loja].[Nome Completo].[Nome Completo Do Chefe]" caption="Nome Completo Do Chefe" propertyName="Nome Completo Do Chefe" numFmtId="0" hierarchy="35" level="3" memberPropertyField="1">
+      <sharedItems count="2">
+        <s v="Luciano Salgado"/>
+        <s v="Sabrina Prada"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Ano]" caption="Ano" numFmtId="0" hierarchy="29" level="1">
+      <sharedItems count="4">
+        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2010]" c="2010"/>
+        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2011]" c="2011"/>
+        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2012]" c="2012"/>
+        <s v="[Data Tentativa].[Ano - Dia].[Ano].&amp;[2013]" c="2013"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Trimestre]" caption="Trimestre" numFmtId="0" hierarchy="29" level="2" mappingCount="1">
+      <sharedItems count="2">
+        <s v="[Data Tentativa].[Ano - Dia].[Trimestre].&amp;[2013]&amp;[1]" c="1" cp="1">
+          <x/>
+        </s>
+        <s v="[Data Tentativa].[Ano - Dia].[Trimestre].&amp;[2013]&amp;[2]" c="2" cp="1">
+          <x/>
+        </s>
+      </sharedItems>
+      <mpMap v="12"/>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Mês Número]" caption="Mês Número" numFmtId="0" hierarchy="29" level="3" mappingCount="1">
+      <sharedItems count="3">
+        <s v="[Data Tentativa].[Ano - Dia].[Mês Número].&amp;[2013]&amp;[2]&amp;[4]" c="4" cp="1">
+          <x/>
+        </s>
+        <s v="[Data Tentativa].[Ano - Dia].[Mês Número].&amp;[2013]&amp;[2]&amp;[5]" c="5" cp="1">
+          <x/>
+        </s>
+        <s v="[Data Tentativa].[Ano - Dia].[Mês Número].&amp;[2013]&amp;[2]&amp;[6]" c="6" cp="1">
+          <x/>
+        </s>
+      </sharedItems>
+      <mpMap v="13"/>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Dia]" caption="Dia" numFmtId="0" hierarchy="29" level="4">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Trimestre].[Ano]" caption="Ano" propertyName="Ano" numFmtId="0" hierarchy="29" level="2" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2013" maxValue="2013" count="1">
+        <n v="2013"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Mês Número].[Trimestre]" caption="Trimestre" propertyName="Trimestre" numFmtId="0" hierarchy="29" level="3" memberPropertyField="1">
+      <sharedItems count="1">
+        <s v="2"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Data Tentativa].[Ano - Dia].[Dia].[Mês Número]" caption="Mês Número" propertyName="Mês Número" numFmtId="0" hierarchy="29" level="4" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Tipo Servico].[Tipo].[Tipo]" caption="Tipo" numFmtId="0" hierarchy="72" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="130">
+    <cacheHierarchy uniqueName="[Cliente].[Activo]" caption="Activo" attribute="1" defaultMemberUniqueName="[Cliente].[Activo].[All]" allUniqueName="[Cliente].[Activo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Codigo Postal]" caption="Codigo Postal" attribute="1" defaultMemberUniqueName="[Cliente].[Codigo Postal].[All]" allUniqueName="[Cliente].[Codigo Postal].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Educação]" caption="Educação" attribute="1" defaultMemberUniqueName="[Cliente].[Educação].[All]" allUniqueName="[Cliente].[Educação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Estado Civil]" caption="Estado Civil" attribute="1" defaultMemberUniqueName="[Cliente].[Estado Civil].[All]" allUniqueName="[Cliente].[Estado Civil].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Género]" caption="Género" attribute="1" defaultMemberUniqueName="[Cliente].[Género].[All]" allUniqueName="[Cliente].[Género].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Idade]" caption="Intervalo Idade" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Idade].[All]" allUniqueName="[Cliente].[Intervalo Idade].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Idade Nome]" caption="Intervalo Idade Nome" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Idade Nome].[All]" allUniqueName="[Cliente].[Intervalo Idade Nome].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento]" caption="Intervalo Rendimento" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento].[All]" allUniqueName="[Cliente].[Intervalo Rendimento].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento Classe]" caption="Intervalo Rendimento Classe" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento Classe].[All]" allUniqueName="[Cliente].[Intervalo Rendimento Classe].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Intervalo Rendimento Codigo]" caption="Intervalo Rendimento Codigo" attribute="1" defaultMemberUniqueName="[Cliente].[Intervalo Rendimento Codigo].[All]" allUniqueName="[Cliente].[Intervalo Rendimento Codigo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Nome De Contacto]" caption="Nome De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Nome De Contacto].[All]" allUniqueName="[Cliente].[Nome De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Número De Carros Possuidos]" caption="Número De Carros Possuidos" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Carros Possuidos].[All]" allUniqueName="[Cliente].[Número De Carros Possuidos].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Número De Filhos]" caption="Número De Filhos" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Filhos].[All]" allUniqueName="[Cliente].[Número De Filhos].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Número De Filhos Em Casa]" caption="Número De Filhos Em Casa" attribute="1" defaultMemberUniqueName="[Cliente].[Número De Filhos Em Casa].[All]" allUniqueName="[Cliente].[Número De Filhos Em Casa].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Ocupação]" caption="Ocupação" attribute="1" defaultMemberUniqueName="[Cliente].[Ocupação].[All]" allUniqueName="[Cliente].[Ocupação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Por Designação]" caption="Por Designação" defaultMemberUniqueName="[Cliente].[Por Designação].[All]" allUniqueName="[Cliente].[Por Designação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Possui Casa]" caption="Possui Casa" attribute="1" defaultMemberUniqueName="[Cliente].[Possui Casa].[All]" allUniqueName="[Cliente].[Possui Casa].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Singular]" caption="Singular" attribute="1" defaultMemberUniqueName="[Cliente].[Singular].[All]" allUniqueName="[Cliente].[Singular].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente].[Sobrenome De Contacto]" caption="Sobrenome De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Sobrenome De Contacto].[All]" allUniqueName="[Cliente].[Sobrenome De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Ano - Dia]" caption="Data Conclusao.Ano - Dia" time="1" defaultMemberUniqueName="[Data Conclusao].[Ano - Dia].[All]" allUniqueName="[Data Conclusao].[Ano - Dia].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Data]" caption="Data Conclusao.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Data].[All]" allUniqueName="[Data Conclusao].[Data].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Dia Da Semana Nome]" caption="Data Conclusao.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia Da Semana Nome].[All]" allUniqueName="[Data Conclusao].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Dia Da Semana Número]" caption="Data Conclusao.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia Da Semana Número].[All]" allUniqueName="[Data Conclusao].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Mês Nome]" caption="Data Conclusao.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Mês Nome].[All]" allUniqueName="[Data Conclusao].[Mês Nome].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Ano - Dia]" caption="Data Requisicao.Ano - Dia" time="1" defaultMemberUniqueName="[Data Requisicao].[Ano - Dia].[All]" allUniqueName="[Data Requisicao].[Ano - Dia].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Data]" caption="Data Requisicao.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Data].[All]" allUniqueName="[Data Requisicao].[Data].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Dia Da Semana Nome]" caption="Data Requisicao.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia Da Semana Nome].[All]" allUniqueName="[Data Requisicao].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Dia Da Semana Número]" caption="Data Requisicao.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia Da Semana Número].[All]" allUniqueName="[Data Requisicao].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Mês Nome]" caption="Data Requisicao.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Mês Nome].[All]" allUniqueName="[Data Requisicao].[Mês Nome].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Ano - Dia]" caption="Data Tentativa.Ano - Dia" time="1" defaultMemberUniqueName="[Data Tentativa].[Ano - Dia].[All]" allUniqueName="[Data Tentativa].[Ano - Dia].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="5" unbalanced="0">
+      <fieldsUsage count="5">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="8"/>
+        <fieldUsage x="9"/>
+        <fieldUsage x="10"/>
+        <fieldUsage x="11"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Data]" caption="Data Tentativa.Data" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Data].[All]" allUniqueName="[Data Tentativa].[Data].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Dia Da Semana Nome]" caption="Data Tentativa.Dia Da Semana Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia Da Semana Nome].[All]" allUniqueName="[Data Tentativa].[Dia Da Semana Nome].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Dia Da Semana Número]" caption="Data Tentativa.Dia Da Semana Número" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia Da Semana Número].[All]" allUniqueName="[Data Tentativa].[Dia Da Semana Número].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Mês Nome]" caption="Data Tentativa.Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Mês Nome].[All]" allUniqueName="[Data Tentativa].[Mês Nome].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Activo]" caption="Activo" attribute="1" defaultMemberUniqueName="[Funcionário].[Activo].[All]" allUniqueName="[Funcionário].[Activo].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Localização - Loja]" caption="Localização - Loja" defaultMemberUniqueName="[Funcionário].[Localização - Loja].[All]" allUniqueName="[Funcionário].[Localização - Loja].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="4" unbalanced="0">
+      <fieldsUsage count="4">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+        <fieldUsage x="2"/>
+        <fieldUsage x="3"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Funcionário].[Nome]" caption="Nome" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome].[All]" allUniqueName="[Funcionário].[Nome].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Nome Do Chefe]" caption="Nome Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Do Chefe].[All]" allUniqueName="[Funcionário].[Nome Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Por Função Do Chefe]" caption="Por Função Do Chefe" defaultMemberUniqueName="[Funcionário].[Por Função Do Chefe].[All]" allUniqueName="[Funcionário].[Por Função Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Por Nome Completo Do Chefe]" caption="Por Nome Completo Do Chefe" defaultMemberUniqueName="[Funcionário].[Por Nome Completo Do Chefe].[All]" allUniqueName="[Funcionário].[Por Nome Completo Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Sobrenome]" caption="Sobrenome" attribute="1" defaultMemberUniqueName="[Funcionário].[Sobrenome].[All]" allUniqueName="[Funcionário].[Sobrenome].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Sobrenome Do Chefe]" caption="Sobrenome Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Sobrenome Do Chefe].[All]" allUniqueName="[Funcionário].[Sobrenome Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Conclusao].[Hora 12h]" caption="Hora Conclusao.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Conclusao].[Hora 12h].[All]" allUniqueName="[Hora Conclusao].[Hora 12h].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Conclusao].[Hora 24h]" caption="Hora Conclusao.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Conclusao].[Hora 24h].[All]" allUniqueName="[Hora Conclusao].[Hora 24h].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Entrega].[Hora 12h]" caption="Hora Entrega.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Entrega].[Hora 12h].[All]" allUniqueName="[Hora Entrega].[Hora 12h].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Entrega].[Hora 24h]" caption="Hora Entrega.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Entrega].[Hora 24h].[All]" allUniqueName="[Hora Entrega].[Hora 24h].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Requisicao].[Hora 12h]" caption="Hora Requisicao.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Requisicao].[Hora 12h].[All]" allUniqueName="[Hora Requisicao].[Hora 12h].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Requisicao].[Hora 24h]" caption="Hora Requisicao.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Requisicao].[Hora 24h].[All]" allUniqueName="[Hora Requisicao].[Hora 24h].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Tentativa].[Hora 12h]" caption="Hora Tentativa.Hora 12h" attribute="1" time="1" defaultMemberUniqueName="[Hora Tentativa].[Hora 12h].[All]" allUniqueName="[Hora Tentativa].[Hora 12h].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Hora Tentativa].[Hora 24h]" caption="Hora Tentativa.Hora 24h" attribute="1" time="1" defaultMemberUniqueName="[Hora Tentativa].[Hora 24h].[All]" allUniqueName="[Hora Tentativa].[Hora 24h].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Intervalo]" caption="Intervalo Idade Cliente.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Intervalo].[All]" allUniqueName="[Intervalo Idade Cliente].[Intervalo].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Nome]" caption="Intervalo Idade Cliente.Nome" attribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Nome].[All]" allUniqueName="[Intervalo Idade Cliente].[Nome].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Intervalo]" caption="Intervalo Idade Na Requisição.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Intervalo].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Intervalo].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Nome]" caption="Intervalo Idade Na Requisição.Nome" attribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Nome].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Nome].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Classe]" caption="Intervalo Rendimento Cliente.Classe" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Classe].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Classe].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Codigo]" caption="Intervalo Rendimento Cliente.Codigo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Codigo].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Codigo].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Intervalo]" caption="Intervalo Rendimento Cliente.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Intervalo].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Intervalo].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Classe]" caption="Intervalo Rendimento Na Requisição.Classe" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Classe].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Classe].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Codigo]" caption="Intervalo Rendimento Na Requisição.Codigo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Codigo].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Codigo].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Intervalo]" caption="Intervalo Rendimento Na Requisição.Intervalo" attribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Intervalo].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Intervalo].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Código Postal]" caption="Morada Entrega.Código Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Código Postal].[All]" allUniqueName="[Morada Entrega].[Código Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Código Postal Completo]" caption="Morada Entrega.Código Postal Completo" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Código Postal Completo].[All]" allUniqueName="[Morada Entrega].[Código Postal Completo].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Designação Postal]" caption="Morada Entrega.Designação Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Designação Postal].[All]" allUniqueName="[Morada Entrega].[Designação Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Distrito - Número Da Porta]" caption="Morada Entrega.Distrito - Número Da Porta" defaultMemberUniqueName="[Morada Entrega].[Distrito - Número Da Porta].[All]" allUniqueName="[Morada Entrega].[Distrito - Número Da Porta].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Extensão Código Postal]" caption="Morada Entrega.Extensão Código Postal" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Extensão Código Postal].[All]" allUniqueName="[Morada Entrega].[Extensão Código Postal].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Localidade]" caption="Morada Entrega.Localidade" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Localidade].[All]" allUniqueName="[Morada Entrega].[Localidade].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Código Postal]" caption="Morada Facturacao.Código Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Código Postal].[All]" allUniqueName="[Morada Facturacao].[Código Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Código Postal Completo]" caption="Morada Facturacao.Código Postal Completo" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Código Postal Completo].[All]" allUniqueName="[Morada Facturacao].[Código Postal Completo].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Designação Postal]" caption="Morada Facturacao.Designação Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Designação Postal].[All]" allUniqueName="[Morada Facturacao].[Designação Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Distrito - Número Da Porta]" caption="Morada Facturacao.Distrito - Número Da Porta" defaultMemberUniqueName="[Morada Facturacao].[Distrito - Número Da Porta].[All]" allUniqueName="[Morada Facturacao].[Distrito - Número Da Porta].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Extensão Código Postal]" caption="Morada Facturacao.Extensão Código Postal" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Extensão Código Postal].[All]" allUniqueName="[Morada Facturacao].[Extensão Código Postal].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Localidade]" caption="Morada Facturacao.Localidade" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Localidade].[All]" allUniqueName="[Morada Facturacao].[Localidade].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Tipo Servico].[Tipo]" caption="Tipo" attribute="1" defaultMemberUniqueName="[Tipo Servico].[Tipo].[All]" allUniqueName="[Tipo Servico].[Tipo].[All]" dimensionUniqueName="[Tipo Servico]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="15"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Cliente].[Designação]" caption="Designação" attribute="1" defaultMemberUniqueName="[Cliente].[Designação].[All]" allUniqueName="[Cliente].[Designação].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente].[Keycol].[All]" allUniqueName="[Cliente].[Keycol].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Nome Completo De Contacto]" caption="Nome Completo De Contacto" attribute="1" defaultMemberUniqueName="[Cliente].[Nome Completo De Contacto].[All]" allUniqueName="[Cliente].[Nome Completo De Contacto].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Ano]" caption="Data Conclusao.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Ano].[All]" allUniqueName="[Data Conclusao].[Ano].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Dia]" caption="Data Conclusao.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Dia].[All]" allUniqueName="[Data Conclusao].[Dia].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Keycol]" caption="Data Conclusao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Conclusao].[Keycol].[All]" allUniqueName="[Data Conclusao].[Keycol].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Mês Número]" caption="Data Conclusao.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Mês Número].[All]" allUniqueName="[Data Conclusao].[Mês Número].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Conclusao].[Trimestre]" caption="Data Conclusao.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Conclusao].[Trimestre].[All]" allUniqueName="[Data Conclusao].[Trimestre].[All]" dimensionUniqueName="[Data Conclusao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Ano]" caption="Data Requisicao.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Ano].[All]" allUniqueName="[Data Requisicao].[Ano].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Dia]" caption="Data Requisicao.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Dia].[All]" allUniqueName="[Data Requisicao].[Dia].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Keycol]" caption="Data Requisicao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Requisicao].[Keycol].[All]" allUniqueName="[Data Requisicao].[Keycol].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Mês Número]" caption="Data Requisicao.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Mês Número].[All]" allUniqueName="[Data Requisicao].[Mês Número].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Requisicao].[Trimestre]" caption="Data Requisicao.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Requisicao].[Trimestre].[All]" allUniqueName="[Data Requisicao].[Trimestre].[All]" dimensionUniqueName="[Data Requisicao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Ano]" caption="Data Tentativa.Ano" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Ano].[All]" allUniqueName="[Data Tentativa].[Ano].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Dia]" caption="Data Tentativa.Dia" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Dia].[All]" allUniqueName="[Data Tentativa].[Dia].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Keycol]" caption="Data Tentativa.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data Tentativa].[Keycol].[All]" allUniqueName="[Data Tentativa].[Keycol].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Mês Número]" caption="Data Tentativa.Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Mês Número].[All]" allUniqueName="[Data Tentativa].[Mês Número].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Data Tentativa].[Trimestre]" caption="Data Tentativa.Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Data Tentativa].[Trimestre].[All]" allUniqueName="[Data Tentativa].[Trimestre].[All]" dimensionUniqueName="[Data Tentativa]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Função]" caption="Função" attribute="1" defaultMemberUniqueName="[Funcionário].[Função].[All]" allUniqueName="[Funcionário].[Função].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Função Do Chefe]" caption="Função Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Função Do Chefe].[All]" allUniqueName="[Funcionário].[Função Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Funcionário].[Keycol].[All]" allUniqueName="[Funcionário].[Keycol].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Localização]" caption="Localização" attribute="1" defaultMemberUniqueName="[Funcionário].[Localização].[All]" allUniqueName="[Funcionário].[Localização].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Loja]" caption="Loja" attribute="1" defaultMemberUniqueName="[Funcionário].[Loja].[All]" allUniqueName="[Funcionário].[Loja].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Nome Completo]" caption="Nome Completo" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Completo].[All]" allUniqueName="[Funcionário].[Nome Completo].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Funcionário].[Nome Completo Do Chefe]" caption="Nome Completo Do Chefe" attribute="1" defaultMemberUniqueName="[Funcionário].[Nome Completo Do Chefe].[All]" allUniqueName="[Funcionário].[Nome Completo Do Chefe].[All]" dimensionUniqueName="[Funcionário]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Hora Conclusao].[Keycol]" caption="Hora Conclusao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Conclusao].[Keycol].[All]" allUniqueName="[Hora Conclusao].[Keycol].[All]" dimensionUniqueName="[Hora Conclusao]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Hora Entrega].[Keycol]" caption="Hora Entrega.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Entrega].[Keycol].[All]" allUniqueName="[Hora Entrega].[Keycol].[All]" dimensionUniqueName="[Hora Entrega]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Hora Requisicao].[Keycol]" caption="Hora Requisicao.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Requisicao].[Keycol].[All]" allUniqueName="[Hora Requisicao].[Keycol].[All]" dimensionUniqueName="[Hora Requisicao]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Hora Tentativa].[Keycol]" caption="Hora Tentativa.Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Hora Tentativa].[Keycol].[All]" allUniqueName="[Hora Tentativa].[Keycol].[All]" dimensionUniqueName="[Hora Tentativa]" displayFolder="" count="0" memberValueDatatype="17" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Cliente].[Keycol]" caption="Intervalo Idade Cliente.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Idade Cliente].[Keycol].[All]" allUniqueName="[Intervalo Idade Cliente].[Keycol].[All]" dimensionUniqueName="[Intervalo Idade Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Intervalo Idade Na Requisição].[Keycol]" caption="Intervalo Idade Na Requisição.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Idade Na Requisição].[Keycol].[All]" allUniqueName="[Intervalo Idade Na Requisição].[Keycol].[All]" dimensionUniqueName="[Intervalo Idade Na Requisição]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Cliente].[Keycol]" caption="Intervalo Rendimento Cliente.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Rendimento Cliente].[Keycol].[All]" allUniqueName="[Intervalo Rendimento Cliente].[Keycol].[All]" dimensionUniqueName="[Intervalo Rendimento Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Intervalo Rendimento Na Requisição].[Keycol]" caption="Intervalo Rendimento Na Requisição.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intervalo Rendimento Na Requisição].[Keycol].[All]" allUniqueName="[Intervalo Rendimento Na Requisição].[Keycol].[All]" dimensionUniqueName="[Intervalo Rendimento Na Requisição]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Concelho]" caption="Morada Entrega.Concelho" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Concelho].[All]" allUniqueName="[Morada Entrega].[Concelho].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Distrito]" caption="Morada Entrega.Distrito" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Distrito].[All]" allUniqueName="[Morada Entrega].[Distrito].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Freguesia]" caption="Morada Entrega.Freguesia" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Freguesia].[All]" allUniqueName="[Morada Entrega].[Freguesia].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Keycol]" caption="Morada Entrega.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Morada Entrega].[Keycol].[All]" allUniqueName="[Morada Entrega].[Keycol].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Número Da Porta]" caption="Morada Entrega.Número Da Porta" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Número Da Porta].[All]" allUniqueName="[Morada Entrega].[Número Da Porta].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Entrega].[Rua]" caption="Morada Entrega.Rua" attribute="1" defaultMemberUniqueName="[Morada Entrega].[Rua].[All]" allUniqueName="[Morada Entrega].[Rua].[All]" dimensionUniqueName="[Morada Entrega]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Concelho]" caption="Morada Facturacao.Concelho" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Concelho].[All]" allUniqueName="[Morada Facturacao].[Concelho].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Distrito]" caption="Morada Facturacao.Distrito" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Distrito].[All]" allUniqueName="[Morada Facturacao].[Distrito].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Freguesia]" caption="Morada Facturacao.Freguesia" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Freguesia].[All]" allUniqueName="[Morada Facturacao].[Freguesia].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Keycol]" caption="Morada Facturacao.Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Morada Facturacao].[Keycol].[All]" allUniqueName="[Morada Facturacao].[Keycol].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Número Da Porta]" caption="Morada Facturacao.Número Da Porta" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Número Da Porta].[All]" allUniqueName="[Morada Facturacao].[Número Da Porta].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Morada Facturacao].[Rua]" caption="Morada Facturacao.Rua" attribute="1" defaultMemberUniqueName="[Morada Facturacao].[Rua].[All]" allUniqueName="[Morada Facturacao].[Rua].[All]" dimensionUniqueName="[Morada Facturacao]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Tipo Servico].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Tipo Servico].[Keycol].[All]" allUniqueName="[Tipo Servico].[Keycol].[All]" dimensionUniqueName="[Tipo Servico]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Número De Entregas]" caption="Número De Entregas" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Valor]" caption="Valor" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Dentro Do SLA]" caption="Dentro Do SLA" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Concluido]" caption="Concluido" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Contagem de Servicos]" caption="Contagem de Servicos" measure="1" displayFolder="" measureGroup="Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Número Entregas por Serviço]" caption="Número Entregas por Serviço" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Valor do Serviço]" caption="Valor do Serviço" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Serviço Dentro Do SLA]" caption="Serviço Dentro Do SLA" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Serviço Concluido]" caption="Serviço Concluido" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Sucesso]" caption="Sucesso" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Contagem de Entregas]" caption="Contagem de Entregas" measure="1" displayFolder="" measureGroup="Entregas Dos Servicos" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="17">
+    <dimension name="Cliente" uniqueName="[Cliente]" caption="Cliente"/>
+    <dimension name="Data Conclusao" uniqueName="[Data Conclusao]" caption="Data Conclusao"/>
+    <dimension name="Data Requisicao" uniqueName="[Data Requisicao]" caption="Data Requisicao"/>
+    <dimension name="Data Tentativa" uniqueName="[Data Tentativa]" caption="Data Tentativa"/>
+    <dimension name="Funcionário" uniqueName="[Funcionário]" caption="Funcionário"/>
+    <dimension name="Hora Conclusao" uniqueName="[Hora Conclusao]" caption="Hora Conclusao"/>
+    <dimension name="Hora Entrega" uniqueName="[Hora Entrega]" caption="Hora Entrega"/>
+    <dimension name="Hora Requisicao" uniqueName="[Hora Requisicao]" caption="Hora Requisicao"/>
+    <dimension name="Hora Tentativa" uniqueName="[Hora Tentativa]" caption="Hora Tentativa"/>
+    <dimension name="Intervalo Idade Cliente" uniqueName="[Intervalo Idade Cliente]" caption="Intervalo Idade Cliente"/>
+    <dimension name="Intervalo Idade Na Requisição" uniqueName="[Intervalo Idade Na Requisição]" caption="Intervalo Idade Na Requisição"/>
+    <dimension name="Intervalo Rendimento Cliente" uniqueName="[Intervalo Rendimento Cliente]" caption="Intervalo Rendimento Cliente"/>
+    <dimension name="Intervalo Rendimento Na Requisição" uniqueName="[Intervalo Rendimento Na Requisição]" caption="Intervalo Rendimento Na Requisição"/>
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Morada Entrega" uniqueName="[Morada Entrega]" caption="Morada Entrega"/>
+    <dimension name="Morada Facturacao" uniqueName="[Morada Facturacao]" caption="Morada Facturacao"/>
+    <dimension name="Tipo Servico" uniqueName="[Tipo Servico]" caption="Tipo Servico"/>
+  </dimensions>
+  <measureGroups count="2">
+    <measureGroup name="Entregas Dos Servicos" caption="Entregas Dos Servicos"/>
+    <measureGroup name="Servicos" caption="Servicos"/>
+  </measureGroups>
+  <maps count="25">
+    <map measureGroup="0" dimension="0"/>
+    <map measureGroup="0" dimension="1"/>
+    <map measureGroup="0" dimension="2"/>
+    <map measureGroup="0" dimension="3"/>
+    <map measureGroup="0" dimension="4"/>
+    <map measureGroup="0" dimension="5"/>
+    <map measureGroup="0" dimension="6"/>
+    <map measureGroup="0" dimension="7"/>
+    <map measureGroup="0" dimension="8"/>
+    <map measureGroup="0" dimension="9"/>
+    <map measureGroup="0" dimension="11"/>
+    <map measureGroup="0" dimension="14"/>
+    <map measureGroup="0" dimension="15"/>
+    <map measureGroup="0" dimension="16"/>
+    <map measureGroup="1" dimension="0"/>
+    <map measureGroup="1" dimension="1"/>
+    <map measureGroup="1" dimension="2"/>
+    <map measureGroup="1" dimension="5"/>
+    <map measureGroup="1" dimension="6"/>
+    <map measureGroup="1" dimension="7"/>
+    <map measureGroup="1" dimension="10"/>
+    <map measureGroup="1" dimension="12"/>
+    <map measureGroup="1" dimension="14"/>
+    <map measureGroup="1" dimension="15"/>
+    <map measureGroup="1" dimension="16"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Rui Miranda" refreshedDate="41444.925454745367" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+  <cacheSource type="external" connectionId="2"/>
+  <cacheFields count="9">
+    <cacheField name="[Measures].[Valor]" caption="Valor" numFmtId="0" hierarchy="10" level="32767"/>
+    <cacheField name="[Meses].[Ano - Mês Número].[Ano]" caption="Ano" numFmtId="0" level="1">
+      <sharedItems count="4">
+        <s v="[Meses].[Ano - Mês Número].[Ano].&amp;[2010]" c="2010"/>
+        <s v="[Meses].[Ano - Mês Número].[Ano].&amp;[2011]" c="2011"/>
+        <s v="[Meses].[Ano - Mês Número].[Ano].&amp;[2012]" c="2012"/>
+        <s v="[Meses].[Ano - Mês Número].[Ano].&amp;[2013]" c="2013"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Meses].[Ano - Mês Número].[Trimestre]" caption="Trimestre" numFmtId="0" level="2" mappingCount="1">
+      <sharedItems count="16">
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2010]&amp;[1]" c="1" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2010]&amp;[2]" c="2" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2010]&amp;[3]" c="3" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2010]&amp;[4]" c="4" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2011]&amp;[1]" c="1" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2011]&amp;[2]" c="2" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2011]&amp;[3]" c="3" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2011]&amp;[4]" c="4" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2012]&amp;[1]" c="1" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2012]&amp;[2]" c="2" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2012]&amp;[3]" c="3" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2012]&amp;[4]" c="4" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2013]&amp;[1]" c="1" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2013]&amp;[2]" c="2" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2013]&amp;[3]" c="3" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Trimestre].&amp;[2013]&amp;[4]" c="4" cp="1">
+          <x v="3"/>
+        </s>
+      </sharedItems>
+      <mpMap v="4"/>
+    </cacheField>
+    <cacheField name="[Meses].[Ano - Mês Número].[Mês Número]" caption="Mês Número" numFmtId="0" level="3" mappingCount="1">
+      <sharedItems count="48">
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[1]&amp;[1]" c="1" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[1]&amp;[2]" c="2" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[1]&amp;[3]" c="3" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[2]&amp;[4]" c="4" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[2]&amp;[5]" c="5" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[2]&amp;[6]" c="6" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[3]&amp;[7]" c="7" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[3]&amp;[8]" c="8" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[3]&amp;[9]" c="9" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[4]&amp;[10]" c="10" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[4]&amp;[11]" c="11" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2010]&amp;[4]&amp;[12]" c="12" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[1]&amp;[1]" c="1" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[1]&amp;[2]" c="2" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[1]&amp;[3]" c="3" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[2]&amp;[4]" c="4" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[2]&amp;[5]" c="5" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[2]&amp;[6]" c="6" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[3]&amp;[7]" c="7" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[3]&amp;[8]" c="8" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[3]&amp;[9]" c="9" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[4]&amp;[10]" c="10" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[4]&amp;[11]" c="11" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2011]&amp;[4]&amp;[12]" c="12" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[1]&amp;[1]" c="1" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[1]&amp;[2]" c="2" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[1]&amp;[3]" c="3" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[2]&amp;[4]" c="4" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[2]&amp;[5]" c="5" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[2]&amp;[6]" c="6" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[3]&amp;[7]" c="7" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[3]&amp;[8]" c="8" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[3]&amp;[9]" c="9" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[4]&amp;[10]" c="10" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[4]&amp;[11]" c="11" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2012]&amp;[4]&amp;[12]" c="12" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[1]&amp;[1]" c="1" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[1]&amp;[2]" c="2" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[1]&amp;[3]" c="3" cp="1">
+          <x/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[2]&amp;[4]" c="4" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[2]&amp;[5]" c="5" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[2]&amp;[6]" c="6" cp="1">
+          <x v="1"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[3]&amp;[7]" c="7" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[3]&amp;[8]" c="8" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[3]&amp;[9]" c="9" cp="1">
+          <x v="2"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[4]&amp;[10]" c="10" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[4]&amp;[11]" c="11" cp="1">
+          <x v="3"/>
+        </s>
+        <s v="[Meses].[Ano - Mês Número].[Mês Número].&amp;[2013]&amp;[4]&amp;[12]" c="12" cp="1">
+          <x v="3"/>
+        </s>
+      </sharedItems>
+      <mpMap v="5"/>
+    </cacheField>
+    <cacheField name="[Meses].[Ano - Mês Número].[Trimestre].[Ano]" caption="Ano" propertyName="Ano" numFmtId="0" level="2" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2010" maxValue="2013" count="4">
+        <n v="2010"/>
+        <n v="2011"/>
+        <n v="2012"/>
+        <n v="2013"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Meses].[Ano - Mês Número].[Mês Número].[Trimestre]" caption="Trimestre" propertyName="Trimestre" numFmtId="0" level="3" memberPropertyField="1">
+      <sharedItems count="4">
+        <s v="1"/>
+        <s v="2"/>
+        <s v="3"/>
+        <s v="4"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Rubrica].[Classe - Nome].[Classe]" caption="Classe" numFmtId="0" hierarchy="3" level="1">
+      <sharedItems count="2">
+        <s v="[Rubrica].[Classe - Nome].[Classe].&amp;[Custo]" c="Custo"/>
+        <s v="[Rubrica].[Classe - Nome].[Classe].&amp;[Proveito]" c="Proveito"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Rubrica].[Classe - Nome].[Nome]" caption="Nome" numFmtId="0" hierarchy="3" level="2" mappingCount="1">
+      <sharedItems count="4">
+        <s v="[Rubrica].[Classe - Nome].[Nome].&amp;[Custo]&amp;[Financeiro]" c="Financeiro" cp="1">
+          <x/>
+        </s>
+        <s v="[Rubrica].[Classe - Nome].[Nome].&amp;[Custo]&amp;[Material]" c="Material" cp="1">
+          <x/>
+        </s>
+        <s v="[Rubrica].[Classe - Nome].[Nome].&amp;[Custo]&amp;[Outros]" c="Outros" cp="1">
+          <x/>
+        </s>
+        <s v="[Rubrica].[Classe - Nome].[Nome].&amp;[Custo]&amp;[Salarios]" c="Salarios" cp="1">
+          <x/>
+        </s>
+      </sharedItems>
+      <mpMap v="8"/>
+    </cacheField>
+    <cacheField name="[Rubrica].[Classe - Nome].[Nome].[Classe]" caption="Classe" propertyName="Classe" numFmtId="0" hierarchy="3" level="2" memberPropertyField="1">
+      <sharedItems count="1">
+        <s v="Custo"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="12">
+    <cacheHierarchy uniqueName="[Meses].[Ano - Mês Número]" caption="Ano - Mês Número" time="1" defaultMemberUniqueName="[Meses].[Ano - Mês Número].[All]" allUniqueName="[Meses].[Ano - Mês Número].[All]" dimensionUniqueName="[Meses]" displayFolder="" count="4" unbalanced="0">
+      <fieldsUsage count="4">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+        <fieldUsage x="2"/>
+        <fieldUsage x="3"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Meses].[Mês Nome]" caption="Mês Nome" attribute="1" time="1" defaultMemberUniqueName="[Meses].[Mês Nome].[All]" allUniqueName="[Meses].[Mês Nome].[All]" dimensionUniqueName="[Meses]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Rubrica].[Classe]" caption="Classe" attribute="1" defaultMemberUniqueName="[Rubrica].[Classe].[All]" allUniqueName="[Rubrica].[Classe].[All]" dimensionUniqueName="[Rubrica]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Rubrica].[Classe - Nome]" caption="Classe - Nome" defaultMemberUniqueName="[Rubrica].[Classe - Nome].[All]" allUniqueName="[Rubrica].[Classe - Nome].[All]" dimensionUniqueName="[Rubrica]" displayFolder="" count="3" unbalanced="0">
+      <fieldsUsage count="3">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="6"/>
+        <fieldUsage x="7"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Rubrica].[Nome]" caption="Nome" attribute="1" defaultMemberUniqueName="[Rubrica].[Nome].[All]" allUniqueName="[Rubrica].[Nome].[All]" dimensionUniqueName="[Rubrica]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Meses].[Ano]" caption="Ano" attribute="1" time="1" defaultMemberUniqueName="[Meses].[Ano].[All]" allUniqueName="[Meses].[Ano].[All]" dimensionUniqueName="[Meses]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Meses].[Keycol]" caption="Keycol" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Meses].[Keycol].[All]" allUniqueName="[Meses].[Keycol].[All]" dimensionUniqueName="[Meses]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Meses].[Mês Número]" caption="Mês Número" attribute="1" time="1" defaultMemberUniqueName="[Meses].[Mês Número].[All]" allUniqueName="[Meses].[Mês Número].[All]" dimensionUniqueName="[Meses]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Meses].[Trimestre]" caption="Trimestre" attribute="1" time="1" defaultMemberUniqueName="[Meses].[Trimestre].[All]" allUniqueName="[Meses].[Trimestre].[All]" dimensionUniqueName="[Meses]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Rubrica].[Keycol]" caption="Keycol" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Rubrica].[Keycol].[All]" allUniqueName="[Rubrica].[Keycol].[All]" dimensionUniqueName="[Rubrica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Valor]" caption="Valor" measure="1" displayFolder="" measureGroup="Resultados" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Contagem de Resultados]" caption="Contagem de Resultados" measure="1" displayFolder="" measureGroup="Resultados" count="0"/>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="3">
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Meses" uniqueName="[Meses]" caption="Meses"/>
+    <dimension name="Rubrica" uniqueName="[Rubrica]" caption="Rubrica"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="Resultados" caption="Resultados"/>
+  </measureGroups>
+  <maps count="2">
+    <map measureGroup="0" dimension="1"/>
+    <map measureGroup="0" dimension="2"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Rui Miranda" refreshedDate="41444.126183564818" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Rui Miranda" refreshedDate="41444.926841203705" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="3"/>
   <cacheFields count="5">
     <cacheField name="[Tipo Servico].[Tipo].[Tipo]" caption="Tipo" numFmtId="0" hierarchy="72" level="1">
@@ -5195,7 +5195,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A4:E18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="19">
     <pivotField dataField="1" showAll="0"/>
@@ -5517,7 +5517,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:K21" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField dataField="1" showAll="0"/>
@@ -6389,7 +6389,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable12" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable12" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A3:K13" firstHeaderRow="1" firstDataRow="4" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField dataField="1" showAll="0"/>
@@ -6718,7 +6718,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:E5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
@@ -6769,8 +6769,8 @@
     </i>
   </colItems>
   <dataFields count="4">
+    <dataField fld="2" baseField="0" baseItem="0"/>
     <dataField fld="1" baseField="0" baseItem="0"/>
-    <dataField fld="2" baseField="0" baseItem="0"/>
     <dataField fld="3" baseField="0" baseItem="0"/>
     <dataField fld="4" baseField="0" baseItem="0"/>
   </dataFields>
@@ -6922,7 +6922,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" fieldListSortAscending="1">
   <location ref="A30:H101" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField dataField="1" showAll="0"/>
@@ -7733,7 +7733,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1">
-        <v>790.3999999999993</v>
+        <v>790.39999999999918</v>
       </c>
       <c r="C6" s="1">
         <v>402.48000000000013</v>
@@ -7770,13 +7770,13 @@
         <v>696.79999999999916</v>
       </c>
       <c r="C8" s="1">
-        <v>430.56000000000017</v>
+        <v>430.56000000000023</v>
       </c>
       <c r="D8" s="1">
         <v>1285.3499999999985</v>
       </c>
       <c r="E8" s="1">
-        <v>2412.7099999999978</v>
+        <v>2412.7099999999982</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -7787,7 +7787,7 @@
         <v>665.59999999999923</v>
       </c>
       <c r="C9" s="1">
-        <v>393.12000000000018</v>
+        <v>393.12000000000012</v>
       </c>
       <c r="D9" s="1">
         <v>1231.2299999999987</v>
@@ -7801,7 +7801,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="1">
-        <v>759.19999999999902</v>
+        <v>759.19999999999914</v>
       </c>
       <c r="C10" s="1">
         <v>383.7600000000001</v>
@@ -7824,10 +7824,10 @@
         <v>205.92</v>
       </c>
       <c r="D11" s="1">
-        <v>852.38999999999919</v>
+        <v>852.38999999999942</v>
       </c>
       <c r="E11" s="1">
-        <v>1536.7099999999989</v>
+        <v>1536.7099999999991</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -7838,10 +7838,10 @@
         <v>592.79999999999939</v>
       </c>
       <c r="C12" s="1">
-        <v>308.88000000000011</v>
+        <v>308.88</v>
       </c>
       <c r="D12" s="1">
-        <v>771.20999999999958</v>
+        <v>771.20999999999947</v>
       </c>
       <c r="E12" s="1">
         <v>1672.889999999999</v>
@@ -7872,7 +7872,7 @@
         <v>587.59999999999934</v>
       </c>
       <c r="C14" s="1">
-        <v>336.96000000000004</v>
+        <v>336.96000000000015</v>
       </c>
       <c r="D14" s="1">
         <v>1055.339999999999</v>
@@ -7886,7 +7886,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="1">
-        <v>759.19999999999902</v>
+        <v>759.19999999999925</v>
       </c>
       <c r="C15" s="1">
         <v>524.16000000000031</v>
@@ -7906,7 +7906,7 @@
         <v>623.99999999999932</v>
       </c>
       <c r="C16" s="1">
-        <v>355.68000000000018</v>
+        <v>355.68000000000012</v>
       </c>
       <c r="D16" s="1">
         <v>1082.399999999999</v>
@@ -7923,13 +7923,13 @@
         <v>682.09999999999923</v>
       </c>
       <c r="C17" s="1">
-        <v>365.42000000000013</v>
+        <v>365.42000000000007</v>
       </c>
       <c r="D17" s="1">
         <v>1286.1599999999985</v>
       </c>
       <c r="E17" s="1">
-        <v>2333.679999999998</v>
+        <v>2333.6799999999976</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -7937,16 +7937,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="1">
-        <v>7899.6999999999925</v>
+        <v>7899.6999999999916</v>
       </c>
       <c r="C18" s="1">
         <v>4324.7000000000016</v>
       </c>
       <c r="D18" s="1">
-        <v>13517.279999999986</v>
+        <v>13517.279999999984</v>
       </c>
       <c r="E18" s="1">
-        <v>25741.679999999975</v>
+        <v>25741.679999999978</v>
       </c>
     </row>
   </sheetData>
@@ -8145,16 +8145,16 @@
         <v>106</v>
       </c>
       <c r="H8" s="4">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I8" s="4">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="J8" s="4">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="K8" s="4">
-        <v>3760</v>
+        <v>3762</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -8180,16 +8180,16 @@
         <v>174</v>
       </c>
       <c r="H9" s="4">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="I9" s="4">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="J9" s="4">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="K9" s="4">
-        <v>5256</v>
+        <v>5261</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -8215,16 +8215,16 @@
         <v>207</v>
       </c>
       <c r="H10" s="4">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I10" s="4">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="J10" s="4">
-        <v>1127</v>
+        <v>1132</v>
       </c>
       <c r="K10" s="4">
-        <v>6705</v>
+        <v>6710</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -8250,16 +8250,16 @@
         <v>543</v>
       </c>
       <c r="H11" s="4">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="I11" s="4">
-        <v>1192</v>
+        <v>1201</v>
       </c>
       <c r="J11" s="4">
-        <v>2684</v>
+        <v>2693</v>
       </c>
       <c r="K11" s="4">
-        <v>15410</v>
+        <v>15419</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -8285,16 +8285,16 @@
         <v>595</v>
       </c>
       <c r="H12" s="4">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="I12" s="4">
-        <v>1357</v>
+        <v>1372</v>
       </c>
       <c r="J12" s="4">
-        <v>2899</v>
+        <v>2914</v>
       </c>
       <c r="K12" s="4">
-        <v>16239</v>
+        <v>16254</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -8320,16 +8320,16 @@
         <v>596</v>
       </c>
       <c r="H13" s="4">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="I13" s="4">
-        <v>1335</v>
+        <v>1348</v>
       </c>
       <c r="J13" s="4">
-        <v>2798</v>
+        <v>2811</v>
       </c>
       <c r="K13" s="4">
-        <v>15305</v>
+        <v>15318</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -8355,16 +8355,16 @@
         <v>551</v>
       </c>
       <c r="H14" s="4">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="I14" s="4">
-        <v>1220</v>
+        <v>1232</v>
       </c>
       <c r="J14" s="4">
-        <v>2536</v>
+        <v>2548</v>
       </c>
       <c r="K14" s="4">
-        <v>13760</v>
+        <v>13772</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -8390,16 +8390,16 @@
         <v>499</v>
       </c>
       <c r="H15" s="4">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="I15" s="4">
-        <v>1093</v>
+        <v>1104</v>
       </c>
       <c r="J15" s="4">
-        <v>2230</v>
+        <v>2241</v>
       </c>
       <c r="K15" s="4">
-        <v>12075</v>
+        <v>12086</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -8425,16 +8425,16 @@
         <v>439</v>
       </c>
       <c r="H16" s="4">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="I16" s="4">
-        <v>920</v>
+        <v>929</v>
       </c>
       <c r="J16" s="4">
-        <v>1868</v>
+        <v>1877</v>
       </c>
       <c r="K16" s="4">
-        <v>9840</v>
+        <v>9849</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -8460,16 +8460,16 @@
         <v>331</v>
       </c>
       <c r="H17" s="4">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="I17" s="4">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="J17" s="4">
-        <v>1284</v>
+        <v>1287</v>
       </c>
       <c r="K17" s="4">
-        <v>6047</v>
+        <v>6050</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -8495,16 +8495,16 @@
         <v>174</v>
       </c>
       <c r="H18" s="4">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I18" s="4">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="J18" s="4">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="K18" s="4">
-        <v>2590</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -8530,16 +8530,16 @@
         <v>70</v>
       </c>
       <c r="H19" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I19" s="4">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J19" s="4">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K19" s="4">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -8598,16 +8598,16 @@
         <v>4400</v>
       </c>
       <c r="H21" s="4">
-        <v>1343</v>
+        <v>1430</v>
       </c>
       <c r="I21" s="4">
-        <v>9700</v>
+        <v>9787</v>
       </c>
       <c r="J21" s="4">
-        <v>20370</v>
+        <v>20457</v>
       </c>
       <c r="K21" s="4">
-        <v>110917</v>
+        <v>111004</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -8640,15 +8640,15 @@
       </c>
       <c r="H22">
         <f t="shared" si="0"/>
-        <v>95.928571428571431</v>
+        <v>102.14285714285714</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>646.6</v>
+        <v>652.4</v>
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>1357.9333333333334</v>
+        <v>1363.7333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -8802,17 +8802,17 @@
         <v>1</v>
       </c>
       <c r="J7" s="4">
-        <v>1849</v>
+        <v>1870</v>
       </c>
       <c r="K7" s="5">
-        <v>0.84275296262534183</v>
+        <v>0.85232452142206017</v>
       </c>
       <c r="L7" s="4">
-        <v>4043</v>
+        <v>4064</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="4">
-        <v>23178</v>
+        <v>23199</v>
       </c>
       <c r="O7" s="5"/>
     </row>
@@ -8845,17 +8845,17 @@
         <v>1</v>
       </c>
       <c r="J8" s="4">
-        <v>1849</v>
+        <v>1870</v>
       </c>
       <c r="K8" s="5">
-        <v>0.84275296262534183</v>
+        <v>0.85232452142206017</v>
       </c>
       <c r="L8" s="4">
-        <v>4043</v>
+        <v>4064</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="4">
-        <v>23178</v>
+        <v>23199</v>
       </c>
       <c r="O8" s="5"/>
     </row>
@@ -8931,17 +8931,17 @@
         <v>1</v>
       </c>
       <c r="J10" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K10" s="5">
-        <v>0.83333333333333337</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="L10" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="4">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="O10" s="5"/>
     </row>
@@ -8974,17 +8974,17 @@
         <v>1</v>
       </c>
       <c r="J11" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K11" s="5">
-        <v>0.91428571428571426</v>
+        <v>0.94285714285714284</v>
       </c>
       <c r="L11" s="4">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="4">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="O11" s="5"/>
     </row>
@@ -9146,17 +9146,17 @@
         <v>1</v>
       </c>
       <c r="J15" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K15" s="5">
-        <v>0.51249999999999996</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="L15" s="4">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="4">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="O15" s="5"/>
     </row>
@@ -9189,17 +9189,17 @@
         <v>1</v>
       </c>
       <c r="J16" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K16" s="5">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="L16" s="4">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="4">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="O16" s="5"/>
     </row>
@@ -9275,17 +9275,17 @@
         <v>1</v>
       </c>
       <c r="J18" s="4">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="K18" s="5">
-        <v>0.91304347826086951</v>
+        <v>0.92028985507246375</v>
       </c>
       <c r="L18" s="4">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="M18" s="5"/>
       <c r="N18" s="4">
-        <v>2925</v>
+        <v>2927</v>
       </c>
       <c r="O18" s="5"/>
     </row>
@@ -9361,17 +9361,17 @@
         <v>1</v>
       </c>
       <c r="J20" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K20" s="5">
-        <v>0.86538461538461542</v>
+        <v>0.88461538461538458</v>
       </c>
       <c r="L20" s="4">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="4">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="O20" s="5"/>
     </row>
@@ -9447,17 +9447,17 @@
         <v>1</v>
       </c>
       <c r="J22" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K22" s="5">
-        <v>0.72727272727272729</v>
+        <v>0.75757575757575757</v>
       </c>
       <c r="L22" s="4">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="4">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="O22" s="5"/>
     </row>
@@ -9576,17 +9576,17 @@
         <v>1</v>
       </c>
       <c r="J25" s="4">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="K25" s="5">
-        <v>0.86559139784946237</v>
+        <v>0.88172043010752688</v>
       </c>
       <c r="L25" s="4">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="M25" s="5"/>
       <c r="N25" s="4">
-        <v>2193</v>
+        <v>2196</v>
       </c>
       <c r="O25" s="5"/>
     </row>
@@ -9619,17 +9619,17 @@
         <v>1</v>
       </c>
       <c r="J26" s="4">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K26" s="5">
-        <v>1.0535714285714286</v>
+        <v>1.0892857142857142</v>
       </c>
       <c r="L26" s="4">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="M26" s="5"/>
       <c r="N26" s="4">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="O26" s="5"/>
     </row>
@@ -9748,17 +9748,17 @@
         <v>1</v>
       </c>
       <c r="J29" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K29" s="5">
-        <v>0.44262295081967212</v>
+        <v>0.47540983606557374</v>
       </c>
       <c r="L29" s="4">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M29" s="5"/>
       <c r="N29" s="4">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="O29" s="5"/>
     </row>
@@ -10092,17 +10092,17 @@
         <v>1</v>
       </c>
       <c r="J37" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K37" s="5">
-        <v>0.8</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="L37" s="4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M37" s="5"/>
       <c r="N37" s="4">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="O37" s="5"/>
     </row>
@@ -10135,17 +10135,17 @@
         <v>1</v>
       </c>
       <c r="J38" s="4">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K38" s="5">
-        <v>0.93220338983050843</v>
+        <v>0.94915254237288138</v>
       </c>
       <c r="L38" s="4">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M38" s="5"/>
       <c r="N38" s="4">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="O38" s="5"/>
     </row>
@@ -10264,17 +10264,17 @@
         <v>1</v>
       </c>
       <c r="J41" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K41" s="5">
-        <v>1.1000000000000001</v>
+        <v>1.1125</v>
       </c>
       <c r="L41" s="4">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M41" s="5"/>
       <c r="N41" s="4">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="O41" s="5"/>
     </row>
@@ -10479,17 +10479,17 @@
         <v>1</v>
       </c>
       <c r="J46" s="4">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="K46" s="5">
-        <v>0.91216216216216217</v>
+        <v>0.93243243243243246</v>
       </c>
       <c r="L46" s="4">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="M46" s="5"/>
       <c r="N46" s="4">
-        <v>1745</v>
+        <v>1748</v>
       </c>
       <c r="O46" s="5"/>
     </row>
@@ -10608,17 +10608,17 @@
         <v>1</v>
       </c>
       <c r="J49" s="4">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="K49" s="5">
-        <v>1.1091954022988506</v>
+        <v>1.1135057471264367</v>
       </c>
       <c r="L49" s="4">
-        <v>1468</v>
+        <v>1471</v>
       </c>
       <c r="M49" s="5"/>
       <c r="N49" s="4">
-        <v>7279</v>
+        <v>7282</v>
       </c>
       <c r="O49" s="5"/>
     </row>
@@ -10651,17 +10651,17 @@
         <v>1</v>
       </c>
       <c r="J50" s="4">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="K50" s="5">
-        <v>1.1091954022988506</v>
+        <v>1.1135057471264367</v>
       </c>
       <c r="L50" s="4">
-        <v>1468</v>
+        <v>1471</v>
       </c>
       <c r="M50" s="5"/>
       <c r="N50" s="4">
-        <v>7279</v>
+        <v>7282</v>
       </c>
       <c r="O50" s="5"/>
     </row>
@@ -10737,17 +10737,17 @@
         <v>1</v>
       </c>
       <c r="J52" s="4">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K52" s="5">
-        <v>1.5533980582524272</v>
+        <v>1.5631067961165048</v>
       </c>
       <c r="L52" s="4">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M52" s="5"/>
       <c r="N52" s="4">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O52" s="5"/>
     </row>
@@ -10780,17 +10780,17 @@
         <v>1</v>
       </c>
       <c r="J53" s="4">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K53" s="5">
-        <v>0.93333333333333335</v>
+        <v>0.94444444444444442</v>
       </c>
       <c r="L53" s="4">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="M53" s="5"/>
       <c r="N53" s="4">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="O53" s="5"/>
     </row>
@@ -11081,17 +11081,17 @@
         <v>1</v>
       </c>
       <c r="J60" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K60" s="5">
-        <v>0.70175438596491224</v>
+        <v>0.7192982456140351</v>
       </c>
       <c r="L60" s="4">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M60" s="5"/>
       <c r="N60" s="4">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="O60" s="5"/>
     </row>
@@ -11124,17 +11124,17 @@
         <v>1</v>
       </c>
       <c r="J61" s="4">
-        <v>2621</v>
+        <v>2645</v>
       </c>
       <c r="K61" s="5">
-        <v>0.90692041522491351</v>
+        <v>0.91522491349480972</v>
       </c>
       <c r="L61" s="4">
-        <v>5511</v>
+        <v>5535</v>
       </c>
       <c r="M61" s="5"/>
       <c r="N61" s="4">
-        <v>30457</v>
+        <v>30481</v>
       </c>
       <c r="O61" s="5"/>
     </row>
@@ -11247,16 +11247,16 @@
         <v>130</v>
       </c>
       <c r="H7" s="4">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="I7" s="4">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="J7" s="4">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="K7" s="4">
-        <v>3512</v>
+        <v>3516</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -11282,16 +11282,16 @@
         <v>130</v>
       </c>
       <c r="H8" s="4">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="I8" s="4">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="J8" s="4">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="K8" s="4">
-        <v>3512</v>
+        <v>3516</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -11317,16 +11317,16 @@
         <v>130</v>
       </c>
       <c r="H9" s="4">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="I9" s="4">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="J9" s="4">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="K9" s="4">
-        <v>3512</v>
+        <v>3516</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -11451,16 +11451,16 @@
         <v>191</v>
       </c>
       <c r="H13" s="4">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="I13" s="4">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="J13" s="4">
-        <v>1026</v>
+        <v>1030</v>
       </c>
       <c r="K13" s="4">
-        <v>6041</v>
+        <v>6045</v>
       </c>
     </row>
   </sheetData>
@@ -11473,7 +11473,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11482,7 +11482,7 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -11490,10 +11490,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" t="s">
         <v>127</v>
-      </c>
-      <c r="C1" t="s">
-        <v>128</v>
       </c>
       <c r="D1" t="s">
         <v>23</v>
@@ -11507,16 +11507,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="4">
-        <v>65484</v>
+        <v>51637</v>
       </c>
       <c r="C2" s="4">
-        <v>51567</v>
+        <v>65534</v>
       </c>
       <c r="D2" s="4">
-        <v>67079</v>
+        <v>67130</v>
       </c>
       <c r="E2" s="4">
-        <v>46866</v>
+        <v>46902</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -11524,16 +11524,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>12853</v>
+        <v>14420</v>
       </c>
       <c r="C3" s="4">
-        <v>14408</v>
+        <v>12865</v>
       </c>
       <c r="D3" s="4">
-        <v>13287</v>
+        <v>13299</v>
       </c>
       <c r="E3" s="4">
-        <v>13287</v>
+        <v>13299</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -11541,16 +11541,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>30551</v>
+        <v>33220</v>
       </c>
       <c r="C4" s="4">
-        <v>33161</v>
+        <v>30575</v>
       </c>
       <c r="D4" s="4">
-        <v>30551</v>
+        <v>30575</v>
       </c>
       <c r="E4" s="4">
-        <v>30551</v>
+        <v>30575</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -11558,16 +11558,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>108888</v>
+        <v>99277</v>
       </c>
       <c r="C5" s="4">
-        <v>99136</v>
+        <v>108974</v>
       </c>
       <c r="D5" s="4">
-        <v>110917</v>
+        <v>111004</v>
       </c>
       <c r="E5" s="4">
-        <v>90704</v>
+        <v>90776</v>
       </c>
     </row>
   </sheetData>
@@ -12902,10 +12902,10 @@
         <v>-199372.67000000004</v>
       </c>
       <c r="G84" s="1">
-        <v>146122</v>
+        <v>146758.59999999998</v>
       </c>
       <c r="H84" s="1">
-        <v>-53250.669999999984</v>
+        <v>-52614.069999999992</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -13032,10 +13032,10 @@
         <v>-50143.049999999996</v>
       </c>
       <c r="G89" s="1">
-        <v>69592.45</v>
+        <v>70229.05</v>
       </c>
       <c r="H89" s="1">
-        <v>19449.400000000001</v>
+        <v>20086.000000000007</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -13098,10 +13098,10 @@
         <v>-15881.1</v>
       </c>
       <c r="G92" s="1">
-        <v>9570.9500000000007</v>
+        <v>10207.549999999999</v>
       </c>
       <c r="H92" s="1">
-        <v>-6310.15</v>
+        <v>-5673.5500000000011</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -13268,10 +13268,10 @@
         <v>-839235.14999999898</v>
       </c>
       <c r="G101" s="1">
-        <v>775470.09000000008</v>
+        <v>776106.69000000018</v>
       </c>
       <c r="H101" s="1">
-        <v>-63765.06000000007</v>
+        <v>-63128.460000000079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>